<commit_message>
1- add sow, hay & harv con to croppyomo. 2- add misc cost to crop.py 3- hookup croplabourpyomo
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS 2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF07EA1-2B55-4596-8259-9A33245B1214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80335700-F625-4BB6-9344-E3760A56B209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -43,14 +43,14 @@
     <definedName name="fuel_adj_tractor" localSheetId="4">'Mach 1'!$B$37</definedName>
     <definedName name="grain_income_date" localSheetId="0">Price!$B$32</definedName>
     <definedName name="grain_income_length" localSheetId="0">Price!$B$34</definedName>
-    <definedName name="grain_price" localSheetId="0">Price!$A$36:$G$47</definedName>
-    <definedName name="harv_eff" localSheetId="4">'Mach 1'!$B$62</definedName>
-    <definedName name="harv_fuel_consumption" localSheetId="4">'Mach 1'!$B$58</definedName>
-    <definedName name="harvest_maint" localSheetId="4">'Mach 1'!$A$76:$B$86</definedName>
-    <definedName name="harvest_speed" localSheetId="4">'Mach 1'!$A$64:$B$74</definedName>
+    <definedName name="grain_price" localSheetId="0">Price!$A$36:$H$47</definedName>
+    <definedName name="harv_eff" localSheetId="4">'Mach 1'!$B$72</definedName>
+    <definedName name="harv_fuel_consumption" localSheetId="4">'Mach 1'!$B$68</definedName>
+    <definedName name="harvest_maint" localSheetId="4">'Mach 1'!$A$86:$B$96</definedName>
+    <definedName name="harvest_speed" localSheetId="4">'Mach 1'!$A$74:$B$84</definedName>
     <definedName name="harvest_yield" localSheetId="3">'Mach General'!$A$6:$B$16</definedName>
-    <definedName name="harvester_width" localSheetId="4">'Mach 1'!$B$56</definedName>
-    <definedName name="oil_grease_factor_harv" localSheetId="4">'Mach 1'!$B$60</definedName>
+    <definedName name="harvester_width" localSheetId="4">'Mach 1'!$B$66</definedName>
+    <definedName name="oil_grease_factor_harv" localSheetId="4">'Mach 1'!$B$70</definedName>
     <definedName name="oil_grease_factor_tractor" localSheetId="4">'Mach 1'!$B$24</definedName>
     <definedName name="repair_maint_factor_tractor" localSheetId="4">'Mach 1'!$B$26</definedName>
     <definedName name="ria" localSheetId="2">'Feed Budget'!$B$3</definedName>
@@ -61,24 +61,24 @@
     <definedName name="rik" localSheetId="2">'Feed Budget'!$B$7</definedName>
     <definedName name="seeder_base_crop" localSheetId="4">'Mach 1'!#REF!</definedName>
     <definedName name="seeder_speed_base" localSheetId="4">'Mach 1'!$B$33</definedName>
-    <definedName name="seeder_speed_crop_adj" localSheetId="4">'Mach 1'!$A$41:$B$53</definedName>
+    <definedName name="seeder_speed_crop_adj" localSheetId="4">'Mach 1'!$A$41:$B$63</definedName>
     <definedName name="seeder_width" localSheetId="4">'Mach 1'!$B$29</definedName>
     <definedName name="seeding_eff" localSheetId="4">'Mach 1'!$B$31</definedName>
-    <definedName name="sprayer_eff" localSheetId="4">'Mach 1'!$B$93</definedName>
-    <definedName name="sprayer_fuel_consumption" localSheetId="4">'Mach 1'!$B$95</definedName>
-    <definedName name="sprayer_maint" localSheetId="4">'Mach 1'!$B$97</definedName>
-    <definedName name="sprayer_speed" localSheetId="4">'Mach 1'!$B$91</definedName>
-    <definedName name="sprayer_width" localSheetId="4">'Mach 1'!$B$89</definedName>
-    <definedName name="spreader_cap" localSheetId="4">'Mach 1'!$B$111</definedName>
-    <definedName name="spreader_eff" localSheetId="4">'Mach 1'!$B$117</definedName>
-    <definedName name="spreader_fuel" localSheetId="4">'Mach 1'!$B$100</definedName>
-    <definedName name="spreader_maint" localSheetId="4">'Mach 1'!$B$119</definedName>
-    <definedName name="spreader_speed" localSheetId="4">'Mach 1'!$B$115</definedName>
-    <definedName name="spreader_width" localSheetId="4">'Mach 1'!$A$102:$B$109</definedName>
-    <definedName name="stubble_fuel_consumption" localSheetId="4">'Mach 1'!$B$122</definedName>
-    <definedName name="stubble_maint" localSheetId="4">'Mach 1'!$B$124</definedName>
+    <definedName name="sprayer_eff" localSheetId="4">'Mach 1'!$B$103</definedName>
+    <definedName name="sprayer_fuel_consumption" localSheetId="4">'Mach 1'!$B$105</definedName>
+    <definedName name="sprayer_maint" localSheetId="4">'Mach 1'!$B$107</definedName>
+    <definedName name="sprayer_speed" localSheetId="4">'Mach 1'!$B$101</definedName>
+    <definedName name="sprayer_width" localSheetId="4">'Mach 1'!$B$99</definedName>
+    <definedName name="spreader_cap" localSheetId="4">'Mach 1'!$B$121</definedName>
+    <definedName name="spreader_eff" localSheetId="4">'Mach 1'!$B$127</definedName>
+    <definedName name="spreader_fuel" localSheetId="4">'Mach 1'!$B$110</definedName>
+    <definedName name="spreader_maint" localSheetId="4">'Mach 1'!$B$129</definedName>
+    <definedName name="spreader_speed" localSheetId="4">'Mach 1'!$B$125</definedName>
+    <definedName name="spreader_width" localSheetId="4">'Mach 1'!$A$112:$B$119</definedName>
+    <definedName name="stubble_fuel_consumption" localSheetId="4">'Mach 1'!$B$132</definedName>
+    <definedName name="stubble_maint" localSheetId="4">'Mach 1'!$B$134</definedName>
     <definedName name="tillage_maint" localSheetId="4">'Mach 1'!$B$39</definedName>
-    <definedName name="time_fill_spreader" localSheetId="4">'Mach 1'!$B$113</definedName>
+    <definedName name="time_fill_spreader" localSheetId="4">'Mach 1'!$B$123</definedName>
     <definedName name="variable_dep" localSheetId="1">Finance!#REF!</definedName>
     <definedName name="variable_dep" localSheetId="4">'Mach 1'!$B$5</definedName>
   </definedNames>
@@ -273,6 +273,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="H36" authorId="0" shapeId="0" xr:uid="{4FB247CF-E152-434A-876A-FF5F0ADAA4D0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+%
+includes 5% stamp duty</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A50" authorId="0" shapeId="0" xr:uid="{A067DE07-A282-4047-AC13-801EB51C2DD0}">
       <text>
         <r>
@@ -985,7 +1010,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A56" authorId="0" shapeId="0" xr:uid="{EB3EC863-815A-4F07-ADF1-BACEDBEA528E}">
+    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{EB3EC863-815A-4F07-ADF1-BACEDBEA528E}">
       <text>
         <r>
           <rPr>
@@ -1009,7 +1034,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A58" authorId="0" shapeId="0" xr:uid="{3377AFBB-BAF8-4184-9D43-0D43F3CF0BCD}">
+    <comment ref="A68" authorId="0" shapeId="0" xr:uid="{3377AFBB-BAF8-4184-9D43-0D43F3CF0BCD}">
       <text>
         <r>
           <rPr>
@@ -1033,7 +1058,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B58" authorId="0" shapeId="0" xr:uid="{8F650DD9-B6D6-4B19-A197-CD333C815375}">
+    <comment ref="B68" authorId="0" shapeId="0" xr:uid="{8F650DD9-B6D6-4B19-A197-CD333C815375}">
       <text>
         <r>
           <rPr>
@@ -1058,7 +1083,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A60" authorId="0" shapeId="0" xr:uid="{1F923DBF-9E7F-4464-8708-2B0AF1340A76}">
+    <comment ref="A70" authorId="0" shapeId="0" xr:uid="{1F923DBF-9E7F-4464-8708-2B0AF1340A76}">
       <text>
         <r>
           <rPr>
@@ -1082,7 +1107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A62" authorId="0" shapeId="0" xr:uid="{925041D9-BB4A-4730-BA16-A60ED3E49090}">
+    <comment ref="A72" authorId="0" shapeId="0" xr:uid="{925041D9-BB4A-4730-BA16-A60ED3E49090}">
       <text>
         <r>
           <rPr>
@@ -1106,7 +1131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A64" authorId="0" shapeId="0" xr:uid="{83C78BD9-1F45-41C1-83A8-FF872B400F8F}">
+    <comment ref="A74" authorId="0" shapeId="0" xr:uid="{83C78BD9-1F45-41C1-83A8-FF872B400F8F}">
       <text>
         <r>
           <rPr>
@@ -1131,7 +1156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A76" authorId="0" shapeId="0" xr:uid="{03C07A35-AAEB-46EF-9545-55B9E522D28F}">
+    <comment ref="A86" authorId="0" shapeId="0" xr:uid="{03C07A35-AAEB-46EF-9545-55B9E522D28F}">
       <text>
         <r>
           <rPr>
@@ -1156,7 +1181,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A89" authorId="0" shapeId="0" xr:uid="{821E0CE2-6A9B-42C2-9F86-0C81A466AB82}">
+    <comment ref="A99" authorId="0" shapeId="0" xr:uid="{821E0CE2-6A9B-42C2-9F86-0C81A466AB82}">
       <text>
         <r>
           <rPr>
@@ -1180,7 +1205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A91" authorId="0" shapeId="0" xr:uid="{D25B8429-9410-44C7-8574-A6DC0E08A456}">
+    <comment ref="A101" authorId="0" shapeId="0" xr:uid="{D25B8429-9410-44C7-8574-A6DC0E08A456}">
       <text>
         <r>
           <rPr>
@@ -1204,7 +1229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A93" authorId="0" shapeId="0" xr:uid="{BB9ACD3C-8B60-44E6-911C-6ADC9B17BEE9}">
+    <comment ref="A103" authorId="0" shapeId="0" xr:uid="{BB9ACD3C-8B60-44E6-911C-6ADC9B17BEE9}">
       <text>
         <r>
           <rPr>
@@ -1228,7 +1253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A95" authorId="0" shapeId="0" xr:uid="{8AE1C4AE-C9A6-42B8-87F4-4B73EC5E1B5E}">
+    <comment ref="A105" authorId="0" shapeId="0" xr:uid="{8AE1C4AE-C9A6-42B8-87F4-4B73EC5E1B5E}">
       <text>
         <r>
           <rPr>
@@ -1252,7 +1277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A97" authorId="0" shapeId="0" xr:uid="{64BD9D49-D5FD-46A7-90EB-ABA6BC4DD5BF}">
+    <comment ref="A107" authorId="0" shapeId="0" xr:uid="{64BD9D49-D5FD-46A7-90EB-ABA6BC4DD5BF}">
       <text>
         <r>
           <rPr>
@@ -1276,7 +1301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A100" authorId="0" shapeId="0" xr:uid="{B3CC4513-8BFF-4910-ABF7-F746405E57E7}">
+    <comment ref="A110" authorId="0" shapeId="0" xr:uid="{B3CC4513-8BFF-4910-ABF7-F746405E57E7}">
       <text>
         <r>
           <rPr>
@@ -1300,7 +1325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A102" authorId="0" shapeId="0" xr:uid="{4922BC00-7562-4251-AF4D-B71E622B07C0}">
+    <comment ref="A112" authorId="0" shapeId="0" xr:uid="{4922BC00-7562-4251-AF4D-B71E622B07C0}">
       <text>
         <r>
           <rPr>
@@ -1325,7 +1350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A111" authorId="0" shapeId="0" xr:uid="{22E62F09-30E0-4CD0-81DE-F02394555AD3}">
+    <comment ref="A121" authorId="0" shapeId="0" xr:uid="{22E62F09-30E0-4CD0-81DE-F02394555AD3}">
       <text>
         <r>
           <rPr>
@@ -1349,7 +1374,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A113" authorId="0" shapeId="0" xr:uid="{AF9CD173-26D1-4803-84AA-A1C88C31B999}">
+    <comment ref="A123" authorId="0" shapeId="0" xr:uid="{AF9CD173-26D1-4803-84AA-A1C88C31B999}">
       <text>
         <r>
           <rPr>
@@ -1373,7 +1398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A115" authorId="0" shapeId="0" xr:uid="{B466F8A9-62FF-4035-B41F-6123131A64B2}">
+    <comment ref="A125" authorId="0" shapeId="0" xr:uid="{B466F8A9-62FF-4035-B41F-6123131A64B2}">
       <text>
         <r>
           <rPr>
@@ -1397,7 +1422,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A117" authorId="0" shapeId="0" xr:uid="{D36EEB6F-4421-421C-BD2B-38C8EED80323}">
+    <comment ref="A127" authorId="0" shapeId="0" xr:uid="{D36EEB6F-4421-421C-BD2B-38C8EED80323}">
       <text>
         <r>
           <rPr>
@@ -1421,7 +1446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A119" authorId="0" shapeId="0" xr:uid="{476F3EA8-18FE-4BF1-857E-DB0233D5DFAB}">
+    <comment ref="A129" authorId="0" shapeId="0" xr:uid="{476F3EA8-18FE-4BF1-857E-DB0233D5DFAB}">
       <text>
         <r>
           <rPr>
@@ -1445,7 +1470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A122" authorId="0" shapeId="0" xr:uid="{9163A97B-97F8-4781-A636-98B9A4B8C98E}">
+    <comment ref="A132" authorId="0" shapeId="0" xr:uid="{9163A97B-97F8-4781-A636-98B9A4B8C98E}">
       <text>
         <r>
           <rPr>
@@ -1469,7 +1494,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A124" authorId="0" shapeId="0" xr:uid="{30ECEA2E-A5CE-459D-8EC2-C4E59BCFCA95}">
+    <comment ref="A134" authorId="0" shapeId="0" xr:uid="{30ECEA2E-A5CE-459D-8EC2-C4E59BCFCA95}">
       <text>
         <r>
           <rPr>
@@ -1498,7 +1523,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="132">
   <si>
     <t>Machinery</t>
   </si>
@@ -1861,6 +1886,39 @@
   </si>
   <si>
     <t>of</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>sr</t>
+  </si>
+  <si>
+    <t>ur</t>
+  </si>
+  <si>
+    <t>xr</t>
+  </si>
+  <si>
+    <t>jr</t>
+  </si>
+  <si>
+    <t>tr</t>
+  </si>
+  <si>
+    <t>uc</t>
+  </si>
+  <si>
+    <t>xc</t>
+  </si>
+  <si>
+    <t>jc</t>
+  </si>
+  <si>
+    <t>tc</t>
+  </si>
+  <si>
+    <t>insurance</t>
   </si>
 </sst>
 </file>
@@ -2421,10 +2479,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF2F00E-8A84-429F-9A28-0BBAA9C21CDC}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:B59"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2630,8 +2688,8 @@
         <v>43814</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>105</v>
       </c>
@@ -2639,10 +2697,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>92</v>
       </c>
@@ -2664,8 +2722,11 @@
       <c r="G36" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H36" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>5</v>
       </c>
@@ -2688,8 +2749,12 @@
       <c r="G37" s="4">
         <v>12.05</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H37" s="4">
+        <f>0.86*1.05</f>
+        <v>0.90300000000000002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>4</v>
       </c>
@@ -2712,8 +2777,12 @@
       <c r="G38" s="4">
         <v>13.45</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H38" s="4">
+        <f>0.86*1.05</f>
+        <v>0.90300000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>6</v>
       </c>
@@ -2734,8 +2803,12 @@
       <c r="G39" s="4">
         <v>12.85</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H39" s="4">
+        <f>0.86*1.05</f>
+        <v>0.90300000000000002</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>95</v>
       </c>
@@ -2756,8 +2829,12 @@
       <c r="G40" s="4">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H40" s="4">
+        <f>0.86*1.05</f>
+        <v>0.90300000000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>8</v>
       </c>
@@ -2778,8 +2855,12 @@
       <c r="G41" s="4">
         <v>21.95</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H41" s="4">
+        <f>1.04*1.05</f>
+        <v>1.0920000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>9</v>
       </c>
@@ -2800,8 +2881,12 @@
       <c r="G42" s="4">
         <v>21.95</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H42" s="4">
+        <f>1.04*1.05</f>
+        <v>1.0920000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>7</v>
       </c>
@@ -2822,8 +2907,12 @@
       <c r="G43" s="4">
         <v>12.05</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H43" s="4">
+        <f>1.04*1.05</f>
+        <v>1.0920000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>10</v>
       </c>
@@ -2844,8 +2933,12 @@
       <c r="G44" s="4">
         <v>15.85</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H44" s="4">
+        <f>1.04*1.05</f>
+        <v>1.0920000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>96</v>
       </c>
@@ -2864,8 +2957,12 @@
       <c r="G45" s="4">
         <v>15.85</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H45" s="4">
+        <f>1.04*1.05</f>
+        <v>1.0920000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>97</v>
       </c>
@@ -2884,8 +2981,12 @@
       <c r="G46" s="4">
         <v>15.85</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H46" s="4">
+        <f t="shared" ref="H46:H47" si="1">1.04*1.05</f>
+        <v>1.0920000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>98</v>
       </c>
@@ -2903,6 +3004,10 @@
       </c>
       <c r="G47" s="4">
         <v>15.85</v>
+      </c>
+      <c r="H47" s="4">
+        <f t="shared" si="1"/>
+        <v>1.0920000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2998,7 +3103,7 @@
   <dimension ref="A2:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3132,8 +3237,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:B33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3368,10 +3473,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A689975D-2450-4766-909D-59787FB65B03}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A2:C124"/>
+  <dimension ref="A2:C134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3613,7 +3718,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>5</v>
+        <v>121</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
@@ -3621,7 +3726,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
@@ -3629,7 +3734,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
@@ -3637,7 +3742,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
@@ -3645,7 +3750,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
@@ -3653,7 +3758,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>8</v>
+        <v>126</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
@@ -3661,7 +3766,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>9</v>
+        <v>127</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
@@ -3669,7 +3774,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="B49" s="4">
         <v>1</v>
@@ -3677,7 +3782,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
@@ -3685,7 +3790,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="B51" s="4">
         <v>1</v>
@@ -3693,7 +3798,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>97</v>
+        <v>5</v>
       </c>
       <c r="B52" s="4">
         <v>1</v>
@@ -3701,410 +3806,490 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>98</v>
+        <v>4</v>
       </c>
       <c r="B53" s="4">
         <v>1</v>
       </c>
     </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" s="4">
+        <v>1</v>
+      </c>
+    </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
-        <v>49</v>
+      <c r="A55" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>50</v>
+        <v>120</v>
       </c>
       <c r="B56" s="4">
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="4">
+        <v>1</v>
+      </c>
+    </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="B58" s="4">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="4">
+        <v>1</v>
+      </c>
+    </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="B60" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="4">
+        <v>1</v>
+      </c>
+    </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="B62" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B64" s="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B63" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B65" s="4">
-        <v>8</v>
+      <c r="A65" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="B66" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" s="4">
-        <v>8</v>
-      </c>
-    </row>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B68" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B69" s="4">
-        <v>6</v>
-      </c>
-    </row>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B70" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B71" s="4">
-        <v>5.5</v>
-      </c>
-    </row>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B72" s="4">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B73" s="4">
-        <v>5.5</v>
-      </c>
-    </row>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B74" s="4">
-        <v>5.5</v>
+        <v>53</v>
+      </c>
+      <c r="B74" s="4"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" s="4">
+        <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B76" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="B76" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B77" s="4">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B78" s="4">
-        <v>33</v>
+        <v>6</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B79" s="4">
         <v>6</v>
-      </c>
-      <c r="B79" s="4">
-        <v>33</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B80" s="4">
-        <v>38</v>
+        <v>6</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B81" s="4">
-        <v>38</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="B82" s="4">
-        <v>33</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>10</v>
+        <v>97</v>
       </c>
       <c r="B83" s="4">
-        <v>38</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B84" s="4">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B85" s="4">
-        <v>38</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B86" s="4">
-        <v>38</v>
+        <v>54</v>
+      </c>
+      <c r="B86" s="4"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" s="4">
+        <v>33</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="3" t="s">
-        <v>55</v>
+      <c r="A88" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B88" s="4">
+        <v>33</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="B89" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="4">
+        <v>38</v>
+      </c>
+    </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B91" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B92" s="4">
+        <v>33</v>
+      </c>
+    </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="B93" s="4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B94" s="4">
+        <v>38</v>
+      </c>
+    </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="B95" s="4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B97" s="4">
-        <v>1.3</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B96" s="4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B100" s="4">
-        <v>11.3</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B102" s="4"/>
-    </row>
+      <c r="A99" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B99" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B101" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B103" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B104" s="4"/>
-    </row>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B105" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B106" s="4">
-        <v>15</v>
-      </c>
-    </row>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B107" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B108" s="4">
-        <v>20</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B109" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B111" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="A109" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B110" s="4">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B112" s="4"/>
+    </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B113" s="4">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B114" s="4"/>
+    </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B115" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B116" s="4">
+        <v>15</v>
+      </c>
+    </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B117" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B118" s="4">
+        <v>20</v>
+      </c>
+    </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B119" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B121" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B123" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B125" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B127" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B119" s="4">
+      <c r="B129" s="4">
         <v>14.3</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="3" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="4" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B122" s="4">
+      <c r="B132" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="4" t="s">
+    <row r="133" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B124" s="4">
+      <c r="B134" s="4">
         <v>1.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
convert labour inputs to excel
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80335700-F625-4BB6-9344-E3760A56B209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD04505-4C46-47FB-ABE1-88C64ED19EFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,9 @@
   <definedNames>
     <definedName name="approx_hay_yield" localSheetId="3">'Mach General'!$B$3</definedName>
     <definedName name="cart_hay" localSheetId="0">Price!$B$26</definedName>
+    <definedName name="casual_cost">Price!$B$72</definedName>
+    <definedName name="casual_super">Price!$B$74</definedName>
+    <definedName name="casual_workers_comp">Price!$B$76</definedName>
     <definedName name="clearing_value" localSheetId="4">'Mach 1'!$A$8:$B$21</definedName>
     <definedName name="contract_bail" localSheetId="0">Price!$B$24</definedName>
     <definedName name="contract_harv_cost" localSheetId="0">Price!$A$7:$B$17</definedName>
@@ -50,8 +53,13 @@
     <definedName name="harvest_speed" localSheetId="4">'Mach 1'!$A$74:$B$84</definedName>
     <definedName name="harvest_yield" localSheetId="3">'Mach General'!$A$6:$B$16</definedName>
     <definedName name="harvester_width" localSheetId="4">'Mach 1'!$B$66</definedName>
+    <definedName name="manager_cost">Price!$B$62</definedName>
     <definedName name="oil_grease_factor_harv" localSheetId="4">'Mach 1'!$B$70</definedName>
     <definedName name="oil_grease_factor_tractor" localSheetId="4">'Mach 1'!$B$24</definedName>
+    <definedName name="permanent_cost">Price!$B$64</definedName>
+    <definedName name="permanent_ls_leave">Price!$B$70</definedName>
+    <definedName name="permanent_super">Price!$B$66</definedName>
+    <definedName name="permanent_workers_comp">Price!$B$68</definedName>
     <definedName name="repair_maint_factor_tractor" localSheetId="4">'Mach 1'!$B$26</definedName>
     <definedName name="ria" localSheetId="2">'Feed Budget'!$B$3</definedName>
     <definedName name="rib" localSheetId="2">'Feed Budget'!$B$5</definedName>
@@ -346,6 +354,79 @@
         </r>
       </text>
     </comment>
+    <comment ref="A62" authorId="0" shapeId="0" xr:uid="{387FDAF3-8781-41B0-A9D1-44EF18159679}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+$/yr</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A64" authorId="0" shapeId="0" xr:uid="{2FAFB650-F4A0-43AA-A1A4-FD1CE25983D6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+$/yr
+before super</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A70" authorId="0" shapeId="0" xr:uid="{04D6553C-E8DC-4A56-AAAA-8F71B24DF403}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+LS leave</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1523,7 +1604,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="141">
   <si>
     <t>Machinery</t>
   </si>
@@ -1919,13 +2000,40 @@
   </si>
   <si>
     <t>insurance</t>
+  </si>
+  <si>
+    <t>Labour</t>
+  </si>
+  <si>
+    <t>manager_cost</t>
+  </si>
+  <si>
+    <t>permanent_cost</t>
+  </si>
+  <si>
+    <t>permanent_super</t>
+  </si>
+  <si>
+    <t>permanent_workers_comp</t>
+  </si>
+  <si>
+    <t>permanent_ls_leave</t>
+  </si>
+  <si>
+    <t>casual_cost</t>
+  </si>
+  <si>
+    <t>casual_super</t>
+  </si>
+  <si>
+    <t>casual_workers_comp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1959,6 +2067,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2479,10 +2600,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF2F00E-8A84-429F-9A28-0BBAA9C21CDC}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3088,6 +3209,75 @@
       </c>
       <c r="B59" s="4">
         <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B62" s="4">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B64" s="4">
+        <v>80000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B66" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" s="4">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B70" s="4">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B72" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B74" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B76" s="4">
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
altered cont lucerne and tedera handling. Part way through Pas Pyomo
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD04505-4C46-47FB-ABE1-88C64ED19EFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0F4910-5771-448A-8EDF-6E67710844B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,9 @@
   <definedNames>
     <definedName name="approx_hay_yield" localSheetId="3">'Mach General'!$B$3</definedName>
     <definedName name="cart_hay" localSheetId="0">Price!$B$26</definedName>
-    <definedName name="casual_cost">Price!$B$72</definedName>
-    <definedName name="casual_super">Price!$B$74</definedName>
-    <definedName name="casual_workers_comp">Price!$B$76</definedName>
+    <definedName name="casual_cost">Price!$B$74</definedName>
+    <definedName name="casual_super">Price!$B$76</definedName>
+    <definedName name="casual_workers_comp">Price!$B$78</definedName>
     <definedName name="clearing_value" localSheetId="4">'Mach 1'!$A$8:$B$21</definedName>
     <definedName name="contract_bail" localSheetId="0">Price!$B$24</definedName>
     <definedName name="contract_harv_cost" localSheetId="0">Price!$A$7:$B$17</definedName>
@@ -34,32 +34,33 @@
     <definedName name="contract_mow_hay" localSheetId="0">Price!$B$22</definedName>
     <definedName name="contract_seed_cost" localSheetId="0">Price!$B$19</definedName>
     <definedName name="credit_interest" localSheetId="1">Finance!$B$3</definedName>
+    <definedName name="crp_insurance_date">Price!$B$36</definedName>
     <definedName name="debit_interest" localSheetId="1">Finance!$B$5</definedName>
     <definedName name="dep_area" localSheetId="4">'Mach 1'!$B$3</definedName>
     <definedName name="diesel" localSheetId="0">Price!$B$3</definedName>
     <definedName name="diesel_rebate" localSheetId="0">Price!$B$5</definedName>
     <definedName name="draft_seeding" localSheetId="4">'Mach 1'!$B$35</definedName>
-    <definedName name="fert_cartage_cost" localSheetId="0">Price!$B$50</definedName>
-    <definedName name="fert_cost" localSheetId="0">Price!$A$52:$B$59</definedName>
+    <definedName name="fert_cartage_cost" localSheetId="0">Price!$B$52</definedName>
+    <definedName name="fert_cost" localSheetId="0">Price!$A$54:$B$61</definedName>
     <definedName name="fixed_dep" localSheetId="1">Finance!$B$8</definedName>
     <definedName name="flagfall" localSheetId="0">Price!$B$30</definedName>
     <definedName name="fuel_adj_tractor" localSheetId="4">'Mach 1'!$B$37</definedName>
     <definedName name="grain_income_date" localSheetId="0">Price!$B$32</definedName>
     <definedName name="grain_income_length" localSheetId="0">Price!$B$34</definedName>
-    <definedName name="grain_price" localSheetId="0">Price!$A$36:$H$47</definedName>
-    <definedName name="harv_eff" localSheetId="4">'Mach 1'!$B$72</definedName>
-    <definedName name="harv_fuel_consumption" localSheetId="4">'Mach 1'!$B$68</definedName>
-    <definedName name="harvest_maint" localSheetId="4">'Mach 1'!$A$86:$B$96</definedName>
-    <definedName name="harvest_speed" localSheetId="4">'Mach 1'!$A$74:$B$84</definedName>
+    <definedName name="grain_price" localSheetId="0">Price!$A$38:$H$49</definedName>
+    <definedName name="harv_eff" localSheetId="4">'Mach 1'!$B$65</definedName>
+    <definedName name="harv_fuel_consumption" localSheetId="4">'Mach 1'!$B$61</definedName>
+    <definedName name="harvest_maint" localSheetId="4">'Mach 1'!$A$79:$B$89</definedName>
+    <definedName name="harvest_speed" localSheetId="4">'Mach 1'!$A$67:$B$77</definedName>
     <definedName name="harvest_yield" localSheetId="3">'Mach General'!$A$6:$B$16</definedName>
-    <definedName name="harvester_width" localSheetId="4">'Mach 1'!$B$66</definedName>
-    <definedName name="manager_cost">Price!$B$62</definedName>
-    <definedName name="oil_grease_factor_harv" localSheetId="4">'Mach 1'!$B$70</definedName>
+    <definedName name="harvester_width" localSheetId="4">'Mach 1'!$B$59</definedName>
+    <definedName name="manager_cost">Price!$B$64</definedName>
+    <definedName name="oil_grease_factor_harv" localSheetId="4">'Mach 1'!$B$63</definedName>
     <definedName name="oil_grease_factor_tractor" localSheetId="4">'Mach 1'!$B$24</definedName>
-    <definedName name="permanent_cost">Price!$B$64</definedName>
-    <definedName name="permanent_ls_leave">Price!$B$70</definedName>
-    <definedName name="permanent_super">Price!$B$66</definedName>
-    <definedName name="permanent_workers_comp">Price!$B$68</definedName>
+    <definedName name="permanent_cost">Price!$B$66</definedName>
+    <definedName name="permanent_ls_leave">Price!$B$72</definedName>
+    <definedName name="permanent_super">Price!$B$68</definedName>
+    <definedName name="permanent_workers_comp">Price!$B$70</definedName>
     <definedName name="repair_maint_factor_tractor" localSheetId="4">'Mach 1'!$B$26</definedName>
     <definedName name="ria" localSheetId="2">'Feed Budget'!$B$3</definedName>
     <definedName name="rib" localSheetId="2">'Feed Budget'!$B$5</definedName>
@@ -69,24 +70,24 @@
     <definedName name="rik" localSheetId="2">'Feed Budget'!$B$7</definedName>
     <definedName name="seeder_base_crop" localSheetId="4">'Mach 1'!#REF!</definedName>
     <definedName name="seeder_speed_base" localSheetId="4">'Mach 1'!$B$33</definedName>
-    <definedName name="seeder_speed_crop_adj" localSheetId="4">'Mach 1'!$A$41:$B$63</definedName>
+    <definedName name="seeder_speed_crop_adj" localSheetId="4">'Mach 1'!$A$41:$B$56</definedName>
     <definedName name="seeder_width" localSheetId="4">'Mach 1'!$B$29</definedName>
     <definedName name="seeding_eff" localSheetId="4">'Mach 1'!$B$31</definedName>
-    <definedName name="sprayer_eff" localSheetId="4">'Mach 1'!$B$103</definedName>
-    <definedName name="sprayer_fuel_consumption" localSheetId="4">'Mach 1'!$B$105</definedName>
-    <definedName name="sprayer_maint" localSheetId="4">'Mach 1'!$B$107</definedName>
-    <definedName name="sprayer_speed" localSheetId="4">'Mach 1'!$B$101</definedName>
-    <definedName name="sprayer_width" localSheetId="4">'Mach 1'!$B$99</definedName>
-    <definedName name="spreader_cap" localSheetId="4">'Mach 1'!$B$121</definedName>
-    <definedName name="spreader_eff" localSheetId="4">'Mach 1'!$B$127</definedName>
-    <definedName name="spreader_fuel" localSheetId="4">'Mach 1'!$B$110</definedName>
-    <definedName name="spreader_maint" localSheetId="4">'Mach 1'!$B$129</definedName>
-    <definedName name="spreader_speed" localSheetId="4">'Mach 1'!$B$125</definedName>
-    <definedName name="spreader_width" localSheetId="4">'Mach 1'!$A$112:$B$119</definedName>
-    <definedName name="stubble_fuel_consumption" localSheetId="4">'Mach 1'!$B$132</definedName>
-    <definedName name="stubble_maint" localSheetId="4">'Mach 1'!$B$134</definedName>
+    <definedName name="sprayer_eff" localSheetId="4">'Mach 1'!$B$96</definedName>
+    <definedName name="sprayer_fuel_consumption" localSheetId="4">'Mach 1'!$B$98</definedName>
+    <definedName name="sprayer_maint" localSheetId="4">'Mach 1'!$B$100</definedName>
+    <definedName name="sprayer_speed" localSheetId="4">'Mach 1'!$B$94</definedName>
+    <definedName name="sprayer_width" localSheetId="4">'Mach 1'!$B$92</definedName>
+    <definedName name="spreader_cap" localSheetId="4">'Mach 1'!$B$114</definedName>
+    <definedName name="spreader_eff" localSheetId="4">'Mach 1'!$B$120</definedName>
+    <definedName name="spreader_fuel" localSheetId="4">'Mach 1'!$B$103</definedName>
+    <definedName name="spreader_maint" localSheetId="4">'Mach 1'!$B$122</definedName>
+    <definedName name="spreader_speed" localSheetId="4">'Mach 1'!$B$118</definedName>
+    <definedName name="spreader_width" localSheetId="4">'Mach 1'!$A$105:$B$112</definedName>
+    <definedName name="stubble_fuel_consumption" localSheetId="4">'Mach 1'!$B$125</definedName>
+    <definedName name="stubble_maint" localSheetId="4">'Mach 1'!$B$127</definedName>
     <definedName name="tillage_maint" localSheetId="4">'Mach 1'!$B$39</definedName>
-    <definedName name="time_fill_spreader" localSheetId="4">'Mach 1'!$B$123</definedName>
+    <definedName name="time_fill_spreader" localSheetId="4">'Mach 1'!$B$116</definedName>
     <definedName name="variable_dep" localSheetId="1">Finance!#REF!</definedName>
     <definedName name="variable_dep" localSheetId="4">'Mach 1'!$B$5</definedName>
   </definedNames>
@@ -233,7 +234,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{AADA8BF6-3C74-42A3-89A9-C83C52099507}">
+    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{866957A5-947F-4D3A-AA52-98FF53EFB716}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+date when crop insurance is paid</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{AADA8BF6-3C74-42A3-89A9-C83C52099507}">
       <text>
         <r>
           <rPr>
@@ -257,7 +282,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G36" authorId="0" shapeId="0" xr:uid="{AA76DADF-BBD9-4AA9-8375-76B8BFDBE1E6}">
+    <comment ref="G38" authorId="0" shapeId="0" xr:uid="{AA76DADF-BBD9-4AA9-8375-76B8BFDBE1E6}">
       <text>
         <r>
           <rPr>
@@ -281,7 +306,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H36" authorId="0" shapeId="0" xr:uid="{4FB247CF-E152-434A-876A-FF5F0ADAA4D0}">
+    <comment ref="H38" authorId="0" shapeId="0" xr:uid="{4FB247CF-E152-434A-876A-FF5F0ADAA4D0}">
       <text>
         <r>
           <rPr>
@@ -306,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A50" authorId="0" shapeId="0" xr:uid="{A067DE07-A282-4047-AC13-801EB51C2DD0}">
+    <comment ref="A52" authorId="0" shapeId="0" xr:uid="{A067DE07-A282-4047-AC13-801EB51C2DD0}">
       <text>
         <r>
           <rPr>
@@ -330,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B52" authorId="0" shapeId="0" xr:uid="{AC27F3B8-73DE-4D0D-B21B-28C220A98ADC}">
+    <comment ref="B54" authorId="0" shapeId="0" xr:uid="{AC27F3B8-73DE-4D0D-B21B-28C220A98ADC}">
       <text>
         <r>
           <rPr>
@@ -354,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A62" authorId="0" shapeId="0" xr:uid="{387FDAF3-8781-41B0-A9D1-44EF18159679}">
+    <comment ref="A64" authorId="0" shapeId="0" xr:uid="{387FDAF3-8781-41B0-A9D1-44EF18159679}">
       <text>
         <r>
           <rPr>
@@ -378,7 +403,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A64" authorId="0" shapeId="0" xr:uid="{2FAFB650-F4A0-43AA-A1A4-FD1CE25983D6}">
+    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{2FAFB650-F4A0-43AA-A1A4-FD1CE25983D6}">
       <text>
         <r>
           <rPr>
@@ -403,7 +428,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A70" authorId="0" shapeId="0" xr:uid="{04D6553C-E8DC-4A56-AAAA-8F71B24DF403}">
+    <comment ref="A72" authorId="0" shapeId="0" xr:uid="{04D6553C-E8DC-4A56-AAAA-8F71B24DF403}">
       <text>
         <r>
           <rPr>
@@ -1091,7 +1116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{EB3EC863-815A-4F07-ADF1-BACEDBEA528E}">
+    <comment ref="A59" authorId="0" shapeId="0" xr:uid="{EB3EC863-815A-4F07-ADF1-BACEDBEA528E}">
       <text>
         <r>
           <rPr>
@@ -1115,7 +1140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A68" authorId="0" shapeId="0" xr:uid="{3377AFBB-BAF8-4184-9D43-0D43F3CF0BCD}">
+    <comment ref="A61" authorId="0" shapeId="0" xr:uid="{3377AFBB-BAF8-4184-9D43-0D43F3CF0BCD}">
       <text>
         <r>
           <rPr>
@@ -1139,7 +1164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B68" authorId="0" shapeId="0" xr:uid="{8F650DD9-B6D6-4B19-A197-CD333C815375}">
+    <comment ref="B61" authorId="0" shapeId="0" xr:uid="{8F650DD9-B6D6-4B19-A197-CD333C815375}">
       <text>
         <r>
           <rPr>
@@ -1164,7 +1189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A70" authorId="0" shapeId="0" xr:uid="{1F923DBF-9E7F-4464-8708-2B0AF1340A76}">
+    <comment ref="A63" authorId="0" shapeId="0" xr:uid="{1F923DBF-9E7F-4464-8708-2B0AF1340A76}">
       <text>
         <r>
           <rPr>
@@ -1188,7 +1213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A72" authorId="0" shapeId="0" xr:uid="{925041D9-BB4A-4730-BA16-A60ED3E49090}">
+    <comment ref="A65" authorId="0" shapeId="0" xr:uid="{925041D9-BB4A-4730-BA16-A60ED3E49090}">
       <text>
         <r>
           <rPr>
@@ -1212,7 +1237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A74" authorId="0" shapeId="0" xr:uid="{83C78BD9-1F45-41C1-83A8-FF872B400F8F}">
+    <comment ref="A67" authorId="0" shapeId="0" xr:uid="{83C78BD9-1F45-41C1-83A8-FF872B400F8F}">
       <text>
         <r>
           <rPr>
@@ -1237,7 +1262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A86" authorId="0" shapeId="0" xr:uid="{03C07A35-AAEB-46EF-9545-55B9E522D28F}">
+    <comment ref="A79" authorId="0" shapeId="0" xr:uid="{03C07A35-AAEB-46EF-9545-55B9E522D28F}">
       <text>
         <r>
           <rPr>
@@ -1262,7 +1287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A99" authorId="0" shapeId="0" xr:uid="{821E0CE2-6A9B-42C2-9F86-0C81A466AB82}">
+    <comment ref="A92" authorId="0" shapeId="0" xr:uid="{821E0CE2-6A9B-42C2-9F86-0C81A466AB82}">
       <text>
         <r>
           <rPr>
@@ -1286,7 +1311,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A101" authorId="0" shapeId="0" xr:uid="{D25B8429-9410-44C7-8574-A6DC0E08A456}">
+    <comment ref="A94" authorId="0" shapeId="0" xr:uid="{D25B8429-9410-44C7-8574-A6DC0E08A456}">
       <text>
         <r>
           <rPr>
@@ -1310,7 +1335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A103" authorId="0" shapeId="0" xr:uid="{BB9ACD3C-8B60-44E6-911C-6ADC9B17BEE9}">
+    <comment ref="A96" authorId="0" shapeId="0" xr:uid="{BB9ACD3C-8B60-44E6-911C-6ADC9B17BEE9}">
       <text>
         <r>
           <rPr>
@@ -1334,7 +1359,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A105" authorId="0" shapeId="0" xr:uid="{8AE1C4AE-C9A6-42B8-87F4-4B73EC5E1B5E}">
+    <comment ref="A98" authorId="0" shapeId="0" xr:uid="{8AE1C4AE-C9A6-42B8-87F4-4B73EC5E1B5E}">
       <text>
         <r>
           <rPr>
@@ -1358,7 +1383,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A107" authorId="0" shapeId="0" xr:uid="{64BD9D49-D5FD-46A7-90EB-ABA6BC4DD5BF}">
+    <comment ref="A100" authorId="0" shapeId="0" xr:uid="{64BD9D49-D5FD-46A7-90EB-ABA6BC4DD5BF}">
       <text>
         <r>
           <rPr>
@@ -1382,7 +1407,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A110" authorId="0" shapeId="0" xr:uid="{B3CC4513-8BFF-4910-ABF7-F746405E57E7}">
+    <comment ref="A103" authorId="0" shapeId="0" xr:uid="{B3CC4513-8BFF-4910-ABF7-F746405E57E7}">
       <text>
         <r>
           <rPr>
@@ -1406,7 +1431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A112" authorId="0" shapeId="0" xr:uid="{4922BC00-7562-4251-AF4D-B71E622B07C0}">
+    <comment ref="A105" authorId="0" shapeId="0" xr:uid="{4922BC00-7562-4251-AF4D-B71E622B07C0}">
       <text>
         <r>
           <rPr>
@@ -1431,7 +1456,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A121" authorId="0" shapeId="0" xr:uid="{22E62F09-30E0-4CD0-81DE-F02394555AD3}">
+    <comment ref="A114" authorId="0" shapeId="0" xr:uid="{22E62F09-30E0-4CD0-81DE-F02394555AD3}">
       <text>
         <r>
           <rPr>
@@ -1455,7 +1480,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A123" authorId="0" shapeId="0" xr:uid="{AF9CD173-26D1-4803-84AA-A1C88C31B999}">
+    <comment ref="A116" authorId="0" shapeId="0" xr:uid="{AF9CD173-26D1-4803-84AA-A1C88C31B999}">
       <text>
         <r>
           <rPr>
@@ -1479,7 +1504,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A125" authorId="0" shapeId="0" xr:uid="{B466F8A9-62FF-4035-B41F-6123131A64B2}">
+    <comment ref="A118" authorId="0" shapeId="0" xr:uid="{B466F8A9-62FF-4035-B41F-6123131A64B2}">
       <text>
         <r>
           <rPr>
@@ -1503,7 +1528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A127" authorId="0" shapeId="0" xr:uid="{D36EEB6F-4421-421C-BD2B-38C8EED80323}">
+    <comment ref="A120" authorId="0" shapeId="0" xr:uid="{D36EEB6F-4421-421C-BD2B-38C8EED80323}">
       <text>
         <r>
           <rPr>
@@ -1527,7 +1552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A129" authorId="0" shapeId="0" xr:uid="{476F3EA8-18FE-4BF1-857E-DB0233D5DFAB}">
+    <comment ref="A122" authorId="0" shapeId="0" xr:uid="{476F3EA8-18FE-4BF1-857E-DB0233D5DFAB}">
       <text>
         <r>
           <rPr>
@@ -1551,7 +1576,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A132" authorId="0" shapeId="0" xr:uid="{9163A97B-97F8-4781-A636-98B9A4B8C98E}">
+    <comment ref="A125" authorId="0" shapeId="0" xr:uid="{9163A97B-97F8-4781-A636-98B9A4B8C98E}">
       <text>
         <r>
           <rPr>
@@ -1575,7 +1600,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A134" authorId="0" shapeId="0" xr:uid="{30ECEA2E-A5CE-459D-8EC2-C4E59BCFCA95}">
+    <comment ref="A127" authorId="0" shapeId="0" xr:uid="{30ECEA2E-A5CE-459D-8EC2-C4E59BCFCA95}">
       <text>
         <r>
           <rPr>
@@ -1604,7 +1629,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="135">
   <si>
     <t>Machinery</t>
   </si>
@@ -1969,36 +1994,6 @@
     <t>of</t>
   </si>
   <si>
-    <t>ar</t>
-  </si>
-  <si>
-    <t>sr</t>
-  </si>
-  <si>
-    <t>ur</t>
-  </si>
-  <si>
-    <t>xr</t>
-  </si>
-  <si>
-    <t>jr</t>
-  </si>
-  <si>
-    <t>tr</t>
-  </si>
-  <si>
-    <t>uc</t>
-  </si>
-  <si>
-    <t>xc</t>
-  </si>
-  <si>
-    <t>jc</t>
-  </si>
-  <si>
-    <t>tc</t>
-  </si>
-  <si>
     <t>insurance</t>
   </si>
   <si>
@@ -2027,6 +2022,18 @@
   </si>
   <si>
     <t>casual_workers_comp</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>tedera</t>
+  </si>
+  <si>
+    <t>lucerne</t>
+  </si>
+  <si>
+    <t>insurance date</t>
   </si>
 </sst>
 </file>
@@ -2600,10 +2607,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF2F00E-8A84-429F-9A28-0BBAA9C21CDC}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H76"/>
+  <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2818,111 +2825,66 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
-    </row>
+    <row r="35" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>131</v>
+        <v>134</v>
+      </c>
+      <c r="B36" s="6">
+        <v>43692</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="4">
-        <v>295</v>
-      </c>
-      <c r="C37" s="4">
-        <v>280</v>
-      </c>
-      <c r="D37" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="E37" s="4">
-        <f t="shared" ref="E37:E46" si="0">1-D37</f>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="F37" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="G37" s="4">
-        <v>12.05</v>
-      </c>
-      <c r="H37" s="4">
-        <f>0.86*1.05</f>
-        <v>0.90300000000000002</v>
-      </c>
+      <c r="A37" s="3"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="4">
-        <v>295</v>
-      </c>
-      <c r="C38" s="4">
-        <v>265</v>
-      </c>
-      <c r="D38" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E38" s="4">
-        <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="F38" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="G38" s="4">
-        <v>13.45</v>
-      </c>
-      <c r="H38" s="4">
-        <f>0.86*1.05</f>
-        <v>0.90300000000000002</v>
+        <v>92</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39" s="4">
-        <v>235</v>
-      </c>
-      <c r="C39" s="4"/>
+        <v>295</v>
+      </c>
+      <c r="C39" s="4">
+        <v>280</v>
+      </c>
       <c r="D39" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="E39:E48" si="0">1-D39</f>
+        <v>0.19999999999999996</v>
       </c>
       <c r="F39" s="4">
         <v>0.15</v>
       </c>
       <c r="G39" s="4">
-        <v>12.85</v>
+        <v>12.05</v>
       </c>
       <c r="H39" s="4">
         <f>0.86*1.05</f>
@@ -2931,24 +2893,26 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>95</v>
+        <v>4</v>
       </c>
       <c r="B40" s="4">
-        <v>150</v>
-      </c>
-      <c r="C40" s="4"/>
+        <v>295</v>
+      </c>
+      <c r="C40" s="4">
+        <v>265</v>
+      </c>
       <c r="D40" s="4">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E40" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="F40" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="G40" s="4">
-        <v>1.5</v>
+        <v>13.45</v>
       </c>
       <c r="H40" s="4">
         <f>0.86*1.05</f>
@@ -2957,10 +2921,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B41" s="4">
-        <v>550</v>
+        <v>235</v>
       </c>
       <c r="C41" s="4"/>
       <c r="D41" s="4">
@@ -2971,22 +2935,22 @@
         <v>0</v>
       </c>
       <c r="F41" s="4">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="G41" s="4">
-        <v>21.95</v>
+        <v>12.85</v>
       </c>
       <c r="H41" s="4">
-        <f>1.04*1.05</f>
-        <v>1.0920000000000001</v>
+        <f>0.86*1.05</f>
+        <v>0.90300000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="B42" s="4">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4">
@@ -2997,22 +2961,22 @@
         <v>0</v>
       </c>
       <c r="F42" s="4">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="G42" s="4">
-        <v>21.95</v>
+        <v>1.5</v>
       </c>
       <c r="H42" s="4">
-        <f>1.04*1.05</f>
-        <v>1.0920000000000001</v>
+        <f>0.86*1.05</f>
+        <v>0.90300000000000002</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B43" s="4">
-        <v>305</v>
+        <v>550</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4">
@@ -3023,10 +2987,10 @@
         <v>0</v>
       </c>
       <c r="F43" s="4">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="G43" s="4">
-        <v>12.05</v>
+        <v>21.95</v>
       </c>
       <c r="H43" s="4">
         <f>1.04*1.05</f>
@@ -3035,10 +2999,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" s="4">
-        <v>350</v>
+        <v>550</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4">
@@ -3049,10 +3013,10 @@
         <v>0</v>
       </c>
       <c r="F44" s="4">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="G44" s="4">
-        <v>15.85</v>
+        <v>21.95</v>
       </c>
       <c r="H44" s="4">
         <f>1.04*1.05</f>
@@ -3061,9 +3025,11 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B45" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="B45" s="4">
+        <v>305</v>
+      </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4">
         <v>1</v>
@@ -3076,7 +3042,7 @@
         <v>0.15</v>
       </c>
       <c r="G45" s="4">
-        <v>15.85</v>
+        <v>12.05</v>
       </c>
       <c r="H45" s="4">
         <f>1.04*1.05</f>
@@ -3085,9 +3051,11 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B46" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B46" s="4">
+        <v>350</v>
+      </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4">
         <v>1</v>
@@ -3103,13 +3071,13 @@
         <v>15.85</v>
       </c>
       <c r="H46" s="4">
-        <f t="shared" ref="H46:H47" si="1">1.04*1.05</f>
+        <f>1.04*1.05</f>
         <v>1.0920000000000001</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -3117,7 +3085,7 @@
         <v>1</v>
       </c>
       <c r="E47" s="4">
-        <f>1-D47</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F47" s="4">
@@ -3127,106 +3095,146 @@
         <v>15.85</v>
       </c>
       <c r="H47" s="4">
+        <f>1.04*1.05</f>
+        <v>1.0920000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4">
+        <v>1</v>
+      </c>
+      <c r="E48" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F48" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G48" s="4">
+        <v>15.85</v>
+      </c>
+      <c r="H48" s="4">
+        <f t="shared" ref="H48:H49" si="1">1.04*1.05</f>
+        <v>1.0920000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4">
+        <v>1</v>
+      </c>
+      <c r="E49" s="4">
+        <f>1-D49</f>
+        <v>0</v>
+      </c>
+      <c r="F49" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G49" s="4">
+        <v>15.85</v>
+      </c>
+      <c r="H49" s="4">
         <f t="shared" si="1"/>
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B50" s="4">
+      <c r="B52" s="4">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
+    <row r="53" spans="1:8" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B54" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B53" s="4">
+      <c r="B55" s="4">
         <v>624</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B56" s="4">
         <v>455</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B55" s="4">
+      <c r="B57" s="4">
         <v>401</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B58" s="4">
         <v>440</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="4">
+      <c r="B59" s="4">
         <v>339</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B58" s="4">
+      <c r="B60" s="4">
         <v>541</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B61" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B62" s="4">
-        <v>80000</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B64" s="4">
         <v>80000</v>
@@ -3234,49 +3242,57 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B66" s="4">
-        <v>0.09</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B68" s="4">
-        <v>3.5000000000000003E-2</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="B70" s="4">
-        <v>2.3E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="B72" s="4">
-        <v>28</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="B74" s="4">
-        <v>0.09</v>
+        <v>28</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="B76" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B78" s="4">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
@@ -3663,10 +3679,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A689975D-2450-4766-909D-59787FB65B03}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A2:C134"/>
+  <dimension ref="A2:C127"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3908,7 +3924,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
@@ -3916,7 +3932,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
@@ -3924,7 +3940,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
@@ -3932,7 +3948,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>124</v>
+        <v>5</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
@@ -3940,7 +3956,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>125</v>
+        <v>4</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
@@ -3948,7 +3964,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>126</v>
+        <v>6</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
@@ -3956,7 +3972,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
@@ -3964,7 +3980,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B49" s="4">
         <v>1</v>
@@ -3972,7 +3988,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>129</v>
+        <v>8</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
@@ -3980,7 +3996,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="B51" s="4">
         <v>1</v>
@@ -3988,7 +4004,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B52" s="4">
         <v>1</v>
@@ -3996,7 +4012,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B53" s="4">
         <v>1</v>
@@ -4004,7 +4020,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
@@ -4012,7 +4028,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B55" s="4">
         <v>1</v>
@@ -4020,466 +4036,410 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="B56" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" s="4">
-        <v>1</v>
-      </c>
-    </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B58" s="4">
-        <v>1</v>
+      <c r="A58" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B59" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B60" s="4">
-        <v>1</v>
-      </c>
-    </row>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="B61" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B62" s="4">
-        <v>1</v>
-      </c>
-    </row>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="B63" s="4">
-        <v>1</v>
-      </c>
-    </row>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B66" s="4">
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="A65" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B65" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B67" s="4"/>
+    </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="B68" s="4">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69" s="4">
+        <v>8</v>
+      </c>
+    </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="B70" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71" s="4">
+        <v>6</v>
+      </c>
+    </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="B72" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B73" s="4">
+        <v>6</v>
+      </c>
+    </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B74" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B74" s="4">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="B75" s="4">
-        <v>8</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="B76" s="4">
-        <v>8</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B77" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B78" s="4">
-        <v>6</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B79" s="4">
-        <v>6</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="B79" s="4"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B80" s="4">
-        <v>6</v>
+        <v>33</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B81" s="4">
-        <v>5.5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="B82" s="4">
-        <v>5.5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>97</v>
+        <v>8</v>
       </c>
       <c r="B83" s="4">
-        <v>5.5</v>
+        <v>38</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="B84" s="4">
-        <v>5.5</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B85" s="4">
+        <v>33</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B86" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B86" s="4">
+        <v>38</v>
+      </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="B87" s="4">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>4</v>
+        <v>97</v>
       </c>
       <c r="B88" s="4">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="B89" s="4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B90" s="4">
         <v>38</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B91" s="4">
-        <v>38</v>
+      <c r="A91" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="B92" s="4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B93" s="4">
-        <v>38</v>
-      </c>
-    </row>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="B94" s="4">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B95" s="4">
-        <v>38</v>
-      </c>
-    </row>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="B96" s="4">
-        <v>38</v>
-      </c>
-    </row>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B99" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B101" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="A98" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B98" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B100" s="4">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B103" s="4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>11.3</v>
+      </c>
+    </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B105" s="4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>63</v>
+      </c>
+      <c r="B105" s="4"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B106" s="4">
+        <v>20</v>
+      </c>
+    </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B107" s="4">
-        <v>1.3</v>
+        <v>115</v>
+      </c>
+      <c r="B107" s="4"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B108" s="4">
+        <v>20</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="3" t="s">
-        <v>61</v>
+      <c r="A109" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B109" s="4">
+        <v>15</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B110" s="4">
-        <v>11.3</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B111" s="4">
+        <v>20</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B112" s="4"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B113" s="4">
+        <v>69</v>
+      </c>
+      <c r="B112" s="4">
         <v>20</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B114" s="4"/>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B115" s="4">
-        <v>20</v>
-      </c>
-    </row>
+        <v>70</v>
+      </c>
+      <c r="B114" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B116" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B117" s="4">
-        <v>20</v>
-      </c>
-    </row>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B118" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B119" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B121" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B123" s="4">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="119" spans="1:2" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B120" s="4">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B122" s="4">
+        <v>14.3</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B125" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B127" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B129" s="4">
-        <v>14.3</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B132" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B134" s="4">
         <v>1.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add pasture sets for pas.py germination func
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0F4910-5771-448A-8EDF-6E67710844B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6079D56-5FA6-49F0-A5C2-EDEC431F7A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,9 @@
   <definedNames>
     <definedName name="approx_hay_yield" localSheetId="3">'Mach General'!$B$3</definedName>
     <definedName name="cart_hay" localSheetId="0">Price!$B$26</definedName>
-    <definedName name="casual_cost">Price!$B$74</definedName>
-    <definedName name="casual_super">Price!$B$76</definedName>
-    <definedName name="casual_workers_comp">Price!$B$78</definedName>
+    <definedName name="casual_cost">Price!$B$76</definedName>
+    <definedName name="casual_super">Price!$B$78</definedName>
+    <definedName name="casual_workers_comp">Price!$B$80</definedName>
     <definedName name="clearing_value" localSheetId="4">'Mach 1'!$A$8:$B$21</definedName>
     <definedName name="contract_bail" localSheetId="0">Price!$B$24</definedName>
     <definedName name="contract_harv_cost" localSheetId="0">Price!$A$7:$B$17</definedName>
@@ -34,33 +34,33 @@
     <definedName name="contract_mow_hay" localSheetId="0">Price!$B$22</definedName>
     <definedName name="contract_seed_cost" localSheetId="0">Price!$B$19</definedName>
     <definedName name="credit_interest" localSheetId="1">Finance!$B$3</definedName>
-    <definedName name="crp_insurance_date">Price!$B$36</definedName>
+    <definedName name="crp_insurance_date">Price!$B$38</definedName>
     <definedName name="debit_interest" localSheetId="1">Finance!$B$5</definedName>
     <definedName name="dep_area" localSheetId="4">'Mach 1'!$B$3</definedName>
     <definedName name="diesel" localSheetId="0">Price!$B$3</definedName>
     <definedName name="diesel_rebate" localSheetId="0">Price!$B$5</definedName>
     <definedName name="draft_seeding" localSheetId="4">'Mach 1'!$B$35</definedName>
-    <definedName name="fert_cartage_cost" localSheetId="0">Price!$B$52</definedName>
-    <definedName name="fert_cost" localSheetId="0">Price!$A$54:$B$61</definedName>
+    <definedName name="fert_cartage_cost" localSheetId="0">Price!$B$54</definedName>
+    <definedName name="fert_cost" localSheetId="0">Price!$A$56:$B$63</definedName>
     <definedName name="fixed_dep" localSheetId="1">Finance!$B$8</definedName>
-    <definedName name="flagfall" localSheetId="0">Price!$B$30</definedName>
+    <definedName name="flagfall" localSheetId="0">Price!$B$32</definedName>
     <definedName name="fuel_adj_tractor" localSheetId="4">'Mach 1'!$B$37</definedName>
-    <definedName name="grain_income_date" localSheetId="0">Price!$B$32</definedName>
-    <definedName name="grain_income_length" localSheetId="0">Price!$B$34</definedName>
-    <definedName name="grain_price" localSheetId="0">Price!$A$38:$H$49</definedName>
+    <definedName name="grain_income_date" localSheetId="0">Price!$B$34</definedName>
+    <definedName name="grain_income_length" localSheetId="0">Price!$B$36</definedName>
+    <definedName name="grain_price" localSheetId="0">Price!$A$40:$H$51</definedName>
     <definedName name="harv_eff" localSheetId="4">'Mach 1'!$B$65</definedName>
     <definedName name="harv_fuel_consumption" localSheetId="4">'Mach 1'!$B$61</definedName>
     <definedName name="harvest_maint" localSheetId="4">'Mach 1'!$A$79:$B$89</definedName>
     <definedName name="harvest_speed" localSheetId="4">'Mach 1'!$A$67:$B$77</definedName>
     <definedName name="harvest_yield" localSheetId="3">'Mach General'!$A$6:$B$16</definedName>
     <definedName name="harvester_width" localSheetId="4">'Mach 1'!$B$59</definedName>
-    <definedName name="manager_cost">Price!$B$64</definedName>
+    <definedName name="manager_cost">Price!$B$66</definedName>
     <definedName name="oil_grease_factor_harv" localSheetId="4">'Mach 1'!$B$63</definedName>
     <definedName name="oil_grease_factor_tractor" localSheetId="4">'Mach 1'!$B$24</definedName>
-    <definedName name="permanent_cost">Price!$B$66</definedName>
-    <definedName name="permanent_ls_leave">Price!$B$72</definedName>
-    <definedName name="permanent_super">Price!$B$68</definedName>
-    <definedName name="permanent_workers_comp">Price!$B$70</definedName>
+    <definedName name="permanent_cost">Price!$B$68</definedName>
+    <definedName name="permanent_ls_leave">Price!$B$74</definedName>
+    <definedName name="permanent_super">Price!$B$70</definedName>
+    <definedName name="permanent_workers_comp">Price!$B$72</definedName>
     <definedName name="repair_maint_factor_tractor" localSheetId="4">'Mach 1'!$B$26</definedName>
     <definedName name="ria" localSheetId="2">'Feed Budget'!$B$3</definedName>
     <definedName name="rib" localSheetId="2">'Feed Budget'!$B$5</definedName>
@@ -86,6 +86,8 @@
     <definedName name="spreader_width" localSheetId="4">'Mach 1'!$A$105:$B$112</definedName>
     <definedName name="stubble_fuel_consumption" localSheetId="4">'Mach 1'!$B$125</definedName>
     <definedName name="stubble_maint" localSheetId="4">'Mach 1'!$B$127</definedName>
+    <definedName name="sup_feed">'Mach 1'!$A$130:$C$134</definedName>
+    <definedName name="sup_transaction">Price!$B$30</definedName>
     <definedName name="tillage_maint" localSheetId="4">'Mach 1'!$B$39</definedName>
     <definedName name="time_fill_spreader" localSheetId="4">'Mach 1'!$B$116</definedName>
     <definedName name="variable_dep" localSheetId="1">Finance!#REF!</definedName>
@@ -162,7 +164,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="A30" authorId="0" shapeId="0" xr:uid="{FB43B3C4-3E5F-4538-B4DD-6D67661C2593}">
+    <comment ref="A30" authorId="0" shapeId="0" xr:uid="{FA6C6E15-83F4-4AE8-A8CF-15029B1A298F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+transaction cost $/t incured when purchasing grain from neighbour for sup feeding</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A32" authorId="0" shapeId="0" xr:uid="{FB43B3C4-3E5F-4538-B4DD-6D67661C2593}">
       <text>
         <r>
           <rPr>
@@ -186,7 +212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A32" authorId="0" shapeId="0" xr:uid="{312CAC5D-CFCD-42F2-9462-43E28E24E6F9}">
+    <comment ref="A34" authorId="0" shapeId="0" xr:uid="{312CAC5D-CFCD-42F2-9462-43E28E24E6F9}">
       <text>
         <r>
           <rPr>
@@ -210,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A34" authorId="0" shapeId="0" xr:uid="{F82278D8-E513-428A-8E30-3FB362926223}">
+    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{F82278D8-E513-428A-8E30-3FB362926223}">
       <text>
         <r>
           <rPr>
@@ -234,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{866957A5-947F-4D3A-AA52-98FF53EFB716}">
+    <comment ref="A38" authorId="0" shapeId="0" xr:uid="{866957A5-947F-4D3A-AA52-98FF53EFB716}">
       <text>
         <r>
           <rPr>
@@ -258,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{AADA8BF6-3C74-42A3-89A9-C83C52099507}">
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{AADA8BF6-3C74-42A3-89A9-C83C52099507}">
       <text>
         <r>
           <rPr>
@@ -282,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G38" authorId="0" shapeId="0" xr:uid="{AA76DADF-BBD9-4AA9-8375-76B8BFDBE1E6}">
+    <comment ref="G40" authorId="0" shapeId="0" xr:uid="{AA76DADF-BBD9-4AA9-8375-76B8BFDBE1E6}">
       <text>
         <r>
           <rPr>
@@ -306,7 +332,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H38" authorId="0" shapeId="0" xr:uid="{4FB247CF-E152-434A-876A-FF5F0ADAA4D0}">
+    <comment ref="H40" authorId="0" shapeId="0" xr:uid="{4FB247CF-E152-434A-876A-FF5F0ADAA4D0}">
       <text>
         <r>
           <rPr>
@@ -331,7 +357,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A52" authorId="0" shapeId="0" xr:uid="{A067DE07-A282-4047-AC13-801EB51C2DD0}">
+    <comment ref="A54" authorId="0" shapeId="0" xr:uid="{A067DE07-A282-4047-AC13-801EB51C2DD0}">
       <text>
         <r>
           <rPr>
@@ -355,7 +381,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B54" authorId="0" shapeId="0" xr:uid="{AC27F3B8-73DE-4D0D-B21B-28C220A98ADC}">
+    <comment ref="B56" authorId="0" shapeId="0" xr:uid="{AC27F3B8-73DE-4D0D-B21B-28C220A98ADC}">
       <text>
         <r>
           <rPr>
@@ -379,7 +405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A64" authorId="0" shapeId="0" xr:uid="{387FDAF3-8781-41B0-A9D1-44EF18159679}">
+    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{387FDAF3-8781-41B0-A9D1-44EF18159679}">
       <text>
         <r>
           <rPr>
@@ -403,7 +429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{2FAFB650-F4A0-43AA-A1A4-FD1CE25983D6}">
+    <comment ref="A68" authorId="0" shapeId="0" xr:uid="{2FAFB650-F4A0-43AA-A1A4-FD1CE25983D6}">
       <text>
         <r>
           <rPr>
@@ -428,24 +454,24 @@
         </r>
       </text>
     </comment>
-    <comment ref="A72" authorId="0" shapeId="0" xr:uid="{04D6553C-E8DC-4A56-AAAA-8F71B24DF403}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Michael Young:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
+    <comment ref="A74" authorId="0" shapeId="0" xr:uid="{04D6553C-E8DC-4A56-AAAA-8F71B24DF403}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 LS leave</t>
@@ -1629,7 +1655,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="139">
   <si>
     <t>Machinery</t>
   </si>
@@ -2034,13 +2060,25 @@
   </si>
   <si>
     <t>insurance date</t>
+  </si>
+  <si>
+    <t>Sheep Feeding</t>
+  </si>
+  <si>
+    <t>r&amp;m</t>
+  </si>
+  <si>
+    <t>L/t</t>
+  </si>
+  <si>
+    <t>Transaction cost from neighbour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2076,20 +2114,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2102,8 +2133,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2111,11 +2148,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2128,6 +2174,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2607,10 +2658,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF2F00E-8A84-429F-9A28-0BBAA9C21CDC}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2752,6 +2803,7 @@
         <v>13</v>
       </c>
     </row>
+    <row r="20" spans="1:3" ht="4.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>18</v>
@@ -2797,148 +2849,105 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B32" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B32" s="6">
-        <v>43814</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B34" s="4">
-        <v>5</v>
+        <v>104</v>
+      </c>
+      <c r="B34" s="6">
+        <v>43814</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B36" s="6">
-        <v>43692</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
-    </row>
+        <v>105</v>
+      </c>
+      <c r="B36" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>121</v>
+        <v>134</v>
+      </c>
+      <c r="B38" s="6">
+        <v>43692</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39" s="4">
-        <v>295</v>
-      </c>
-      <c r="C39" s="4">
-        <v>280</v>
-      </c>
-      <c r="D39" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="E39" s="4">
-        <f t="shared" ref="E39:E48" si="0">1-D39</f>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="F39" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="G39" s="4">
-        <v>12.05</v>
-      </c>
-      <c r="H39" s="4">
-        <f>0.86*1.05</f>
-        <v>0.90300000000000002</v>
-      </c>
+      <c r="A39" s="3"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="4">
-        <v>295</v>
-      </c>
-      <c r="C40" s="4">
-        <v>265</v>
-      </c>
-      <c r="D40" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E40" s="4">
-        <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="F40" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="G40" s="4">
-        <v>13.45</v>
-      </c>
-      <c r="H40" s="4">
-        <f>0.86*1.05</f>
-        <v>0.90300000000000002</v>
+        <v>92</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B41" s="4">
-        <v>235</v>
-      </c>
-      <c r="C41" s="4"/>
+        <v>295</v>
+      </c>
+      <c r="C41" s="4">
+        <v>280</v>
+      </c>
       <c r="D41" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E41" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="E41:E50" si="0">1-D41</f>
+        <v>0.19999999999999996</v>
       </c>
       <c r="F41" s="4">
         <v>0.15</v>
       </c>
       <c r="G41" s="4">
-        <v>12.85</v>
+        <v>12.05</v>
       </c>
       <c r="H41" s="4">
         <f>0.86*1.05</f>
@@ -2947,24 +2956,26 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>95</v>
+        <v>4</v>
       </c>
       <c r="B42" s="4">
-        <v>150</v>
-      </c>
-      <c r="C42" s="4"/>
+        <v>295</v>
+      </c>
+      <c r="C42" s="4">
+        <v>265</v>
+      </c>
       <c r="D42" s="4">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E42" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="F42" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="G42" s="4">
-        <v>1.5</v>
+        <v>13.45</v>
       </c>
       <c r="H42" s="4">
         <f>0.86*1.05</f>
@@ -2973,10 +2984,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B43" s="4">
-        <v>550</v>
+        <v>235</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4">
@@ -2987,22 +2998,22 @@
         <v>0</v>
       </c>
       <c r="F43" s="4">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="G43" s="4">
-        <v>21.95</v>
+        <v>12.85</v>
       </c>
       <c r="H43" s="4">
-        <f>1.04*1.05</f>
-        <v>1.0920000000000001</v>
+        <f>0.86*1.05</f>
+        <v>0.90300000000000002</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="B44" s="4">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4">
@@ -3013,22 +3024,22 @@
         <v>0</v>
       </c>
       <c r="F44" s="4">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="G44" s="4">
-        <v>21.95</v>
+        <v>1.5</v>
       </c>
       <c r="H44" s="4">
-        <f>1.04*1.05</f>
-        <v>1.0920000000000001</v>
+        <f>0.86*1.05</f>
+        <v>0.90300000000000002</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B45" s="4">
-        <v>305</v>
+        <v>550</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4">
@@ -3039,10 +3050,10 @@
         <v>0</v>
       </c>
       <c r="F45" s="4">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="G45" s="4">
-        <v>12.05</v>
+        <v>21.95</v>
       </c>
       <c r="H45" s="4">
         <f>1.04*1.05</f>
@@ -3051,10 +3062,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" s="4">
-        <v>350</v>
+        <v>550</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4">
@@ -3065,10 +3076,10 @@
         <v>0</v>
       </c>
       <c r="F46" s="4">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="G46" s="4">
-        <v>15.85</v>
+        <v>21.95</v>
       </c>
       <c r="H46" s="4">
         <f>1.04*1.05</f>
@@ -3077,9 +3088,11 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B47" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="B47" s="4">
+        <v>305</v>
+      </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4">
         <v>1</v>
@@ -3092,7 +3105,7 @@
         <v>0.15</v>
       </c>
       <c r="G47" s="4">
-        <v>15.85</v>
+        <v>12.05</v>
       </c>
       <c r="H47" s="4">
         <f>1.04*1.05</f>
@@ -3101,9 +3114,11 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B48" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B48" s="4">
+        <v>350</v>
+      </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4">
         <v>1</v>
@@ -3119,13 +3134,13 @@
         <v>15.85</v>
       </c>
       <c r="H48" s="4">
-        <f t="shared" ref="H48:H49" si="1">1.04*1.05</f>
+        <f>1.04*1.05</f>
         <v>1.0920000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -3133,7 +3148,7 @@
         <v>1</v>
       </c>
       <c r="E49" s="4">
-        <f>1-D49</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F49" s="4">
@@ -3143,106 +3158,146 @@
         <v>15.85</v>
       </c>
       <c r="H49" s="4">
+        <f>1.04*1.05</f>
+        <v>1.0920000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4">
+        <v>1</v>
+      </c>
+      <c r="E50" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F50" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G50" s="4">
+        <v>15.85</v>
+      </c>
+      <c r="H50" s="4">
+        <f t="shared" ref="H50:H51" si="1">1.04*1.05</f>
+        <v>1.0920000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4">
+        <v>1</v>
+      </c>
+      <c r="E51" s="4">
+        <f>1-D51</f>
+        <v>0</v>
+      </c>
+      <c r="F51" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G51" s="4">
+        <v>15.85</v>
+      </c>
+      <c r="H51" s="4">
         <f t="shared" si="1"/>
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B52" s="4">
+      <c r="B54" s="4">
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="3"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B55" s="4">
-        <v>624</v>
-      </c>
+    <row r="55" spans="1:8" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="3"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B56" s="4">
-        <v>455</v>
+        <v>113</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="B57" s="4">
-        <v>401</v>
+        <v>624</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B58" s="4">
-        <v>440</v>
+        <v>455</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B59" s="4">
-        <v>339</v>
+        <v>401</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B60" s="4">
-        <v>541</v>
+        <v>440</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="4">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="4">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B63" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A64" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B64" s="4">
-        <v>80000</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B66" s="4">
         <v>80000</v>
@@ -3250,49 +3305,57 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B68" s="4">
-        <v>0.09</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B70" s="4">
-        <v>3.5000000000000003E-2</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B72" s="4">
-        <v>2.3E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B74" s="4">
-        <v>28</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B76" s="4">
-        <v>0.09</v>
+        <v>28</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B78" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B78" s="4">
+      <c r="B80" s="4">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
@@ -3679,10 +3742,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A689975D-2450-4766-909D-59787FB65B03}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A2:C127"/>
+  <dimension ref="A2:C134"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4443,6 +4506,64 @@
         <v>1.3</v>
       </c>
     </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A129" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A130" s="8"/>
+      <c r="B130" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C130" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A131" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B131" s="8">
+        <v>1</v>
+      </c>
+      <c r="C131" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A132" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B132" s="8">
+        <v>1</v>
+      </c>
+      <c r="C132" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A133" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B133" s="8">
+        <v>1</v>
+      </c>
+      <c r="C133" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A134" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B134" s="8">
+        <v>1</v>
+      </c>
+      <c r="C134" s="8">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added a second grain transfer to allow sup purchasing
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6079D56-5FA6-49F0-A5C2-EDEC431F7A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33DC070-C5AA-40E1-921E-D707C3505019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
@@ -22,9 +22,9 @@
   <definedNames>
     <definedName name="approx_hay_yield" localSheetId="3">'Mach General'!$B$3</definedName>
     <definedName name="cart_hay" localSheetId="0">Price!$B$26</definedName>
-    <definedName name="casual_cost">Price!$B$76</definedName>
-    <definedName name="casual_super">Price!$B$78</definedName>
-    <definedName name="casual_workers_comp">Price!$B$80</definedName>
+    <definedName name="casual_cost">Price!$B$78</definedName>
+    <definedName name="casual_super">Price!$B$80</definedName>
+    <definedName name="casual_workers_comp">Price!$B$82</definedName>
     <definedName name="clearing_value" localSheetId="4">'Mach 1'!$A$8:$B$21</definedName>
     <definedName name="contract_bail" localSheetId="0">Price!$B$24</definedName>
     <definedName name="contract_harv_cost" localSheetId="0">Price!$A$7:$B$17</definedName>
@@ -34,33 +34,33 @@
     <definedName name="contract_mow_hay" localSheetId="0">Price!$B$22</definedName>
     <definedName name="contract_seed_cost" localSheetId="0">Price!$B$19</definedName>
     <definedName name="credit_interest" localSheetId="1">Finance!$B$3</definedName>
-    <definedName name="crp_insurance_date">Price!$B$38</definedName>
+    <definedName name="crp_insurance_date">Price!$B$40</definedName>
     <definedName name="debit_interest" localSheetId="1">Finance!$B$5</definedName>
     <definedName name="dep_area" localSheetId="4">'Mach 1'!$B$3</definedName>
     <definedName name="diesel" localSheetId="0">Price!$B$3</definedName>
     <definedName name="diesel_rebate" localSheetId="0">Price!$B$5</definedName>
     <definedName name="draft_seeding" localSheetId="4">'Mach 1'!$B$35</definedName>
-    <definedName name="fert_cartage_cost" localSheetId="0">Price!$B$54</definedName>
-    <definedName name="fert_cost" localSheetId="0">Price!$A$56:$B$63</definedName>
+    <definedName name="fert_cartage_cost" localSheetId="0">Price!$B$56</definedName>
+    <definedName name="fert_cost" localSheetId="0">Price!$A$58:$B$65</definedName>
     <definedName name="fixed_dep" localSheetId="1">Finance!$B$8</definedName>
-    <definedName name="flagfall" localSheetId="0">Price!$B$32</definedName>
+    <definedName name="flagfall" localSheetId="0">Price!$B$34</definedName>
     <definedName name="fuel_adj_tractor" localSheetId="4">'Mach 1'!$B$37</definedName>
-    <definedName name="grain_income_date" localSheetId="0">Price!$B$34</definedName>
-    <definedName name="grain_income_length" localSheetId="0">Price!$B$36</definedName>
-    <definedName name="grain_price" localSheetId="0">Price!$A$40:$H$51</definedName>
+    <definedName name="grain_income_date" localSheetId="0">Price!$B$36</definedName>
+    <definedName name="grain_income_length" localSheetId="0">Price!$B$38</definedName>
+    <definedName name="grain_price" localSheetId="0">Price!$A$42:$H$53</definedName>
     <definedName name="harv_eff" localSheetId="4">'Mach 1'!$B$65</definedName>
     <definedName name="harv_fuel_consumption" localSheetId="4">'Mach 1'!$B$61</definedName>
     <definedName name="harvest_maint" localSheetId="4">'Mach 1'!$A$79:$B$89</definedName>
     <definedName name="harvest_speed" localSheetId="4">'Mach 1'!$A$67:$B$77</definedName>
     <definedName name="harvest_yield" localSheetId="3">'Mach General'!$A$6:$B$16</definedName>
     <definedName name="harvester_width" localSheetId="4">'Mach 1'!$B$59</definedName>
-    <definedName name="manager_cost">Price!$B$66</definedName>
+    <definedName name="manager_cost">Price!$B$68</definedName>
     <definedName name="oil_grease_factor_harv" localSheetId="4">'Mach 1'!$B$63</definedName>
     <definedName name="oil_grease_factor_tractor" localSheetId="4">'Mach 1'!$B$24</definedName>
-    <definedName name="permanent_cost">Price!$B$68</definedName>
-    <definedName name="permanent_ls_leave">Price!$B$74</definedName>
-    <definedName name="permanent_super">Price!$B$70</definedName>
-    <definedName name="permanent_workers_comp">Price!$B$72</definedName>
+    <definedName name="permanent_cost">Price!$B$70</definedName>
+    <definedName name="permanent_ls_leave">Price!$B$76</definedName>
+    <definedName name="permanent_super">Price!$B$72</definedName>
+    <definedName name="permanent_workers_comp">Price!$B$74</definedName>
     <definedName name="repair_maint_factor_tractor" localSheetId="4">'Mach 1'!$B$26</definedName>
     <definedName name="ria" localSheetId="2">'Feed Budget'!$B$3</definedName>
     <definedName name="rib" localSheetId="2">'Feed Budget'!$B$5</definedName>
@@ -86,8 +86,9 @@
     <definedName name="spreader_width" localSheetId="4">'Mach 1'!$A$105:$B$112</definedName>
     <definedName name="stubble_fuel_consumption" localSheetId="4">'Mach 1'!$B$125</definedName>
     <definedName name="stubble_maint" localSheetId="4">'Mach 1'!$B$127</definedName>
+    <definedName name="sup_cartage">Price!$B$29</definedName>
     <definedName name="sup_feed">'Mach 1'!$A$130:$C$134</definedName>
-    <definedName name="sup_transaction">Price!$B$30</definedName>
+    <definedName name="sup_transaction">Price!$B$31</definedName>
     <definedName name="tillage_maint" localSheetId="4">'Mach 1'!$B$39</definedName>
     <definedName name="time_fill_spreader" localSheetId="4">'Mach 1'!$B$116</definedName>
     <definedName name="variable_dep" localSheetId="1">Finance!#REF!</definedName>
@@ -164,7 +165,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="A30" authorId="0" shapeId="0" xr:uid="{FA6C6E15-83F4-4AE8-A8CF-15029B1A298F}">
+    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{CEB61729-00B6-499B-865A-E27FA99795BC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+cartage cost from a neighbour when buying sup feed ($/t)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A31" authorId="0" shapeId="0" xr:uid="{FA6C6E15-83F4-4AE8-A8CF-15029B1A298F}">
       <text>
         <r>
           <rPr>
@@ -188,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A32" authorId="0" shapeId="0" xr:uid="{FB43B3C4-3E5F-4538-B4DD-6D67661C2593}">
+    <comment ref="A34" authorId="0" shapeId="0" xr:uid="{FB43B3C4-3E5F-4538-B4DD-6D67661C2593}">
       <text>
         <r>
           <rPr>
@@ -212,31 +237,32 @@
         </r>
       </text>
     </comment>
-    <comment ref="A34" authorId="0" shapeId="0" xr:uid="{312CAC5D-CFCD-42F2-9462-43E28E24E6F9}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael Young:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-for cash period allocation</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{F82278D8-E513-428A-8E30-3FB362926223}">
+    <comment ref="A36" authorId="0" shapeId="0" xr:uid="{312CAC5D-CFCD-42F2-9462-43E28E24E6F9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+for cash period allocation
+used for the allocation of buying grain for sup feed as welll</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A38" authorId="0" shapeId="0" xr:uid="{F82278D8-E513-428A-8E30-3FB362926223}">
       <text>
         <r>
           <rPr>
@@ -260,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A38" authorId="0" shapeId="0" xr:uid="{866957A5-947F-4D3A-AA52-98FF53EFB716}">
+    <comment ref="A40" authorId="0" shapeId="0" xr:uid="{866957A5-947F-4D3A-AA52-98FF53EFB716}">
       <text>
         <r>
           <rPr>
@@ -284,7 +310,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{AADA8BF6-3C74-42A3-89A9-C83C52099507}">
+    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{AADA8BF6-3C74-42A3-89A9-C83C52099507}">
       <text>
         <r>
           <rPr>
@@ -308,7 +334,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G40" authorId="0" shapeId="0" xr:uid="{AA76DADF-BBD9-4AA9-8375-76B8BFDBE1E6}">
+    <comment ref="G42" authorId="0" shapeId="0" xr:uid="{AA76DADF-BBD9-4AA9-8375-76B8BFDBE1E6}">
       <text>
         <r>
           <rPr>
@@ -332,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H40" authorId="0" shapeId="0" xr:uid="{4FB247CF-E152-434A-876A-FF5F0ADAA4D0}">
+    <comment ref="H42" authorId="0" shapeId="0" xr:uid="{4FB247CF-E152-434A-876A-FF5F0ADAA4D0}">
       <text>
         <r>
           <rPr>
@@ -357,7 +383,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A54" authorId="0" shapeId="0" xr:uid="{A067DE07-A282-4047-AC13-801EB51C2DD0}">
+    <comment ref="A56" authorId="0" shapeId="0" xr:uid="{A067DE07-A282-4047-AC13-801EB51C2DD0}">
       <text>
         <r>
           <rPr>
@@ -381,7 +407,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B56" authorId="0" shapeId="0" xr:uid="{AC27F3B8-73DE-4D0D-B21B-28C220A98ADC}">
+    <comment ref="B58" authorId="0" shapeId="0" xr:uid="{AC27F3B8-73DE-4D0D-B21B-28C220A98ADC}">
       <text>
         <r>
           <rPr>
@@ -405,7 +431,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{387FDAF3-8781-41B0-A9D1-44EF18159679}">
+    <comment ref="A68" authorId="0" shapeId="0" xr:uid="{387FDAF3-8781-41B0-A9D1-44EF18159679}">
       <text>
         <r>
           <rPr>
@@ -429,7 +455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A68" authorId="0" shapeId="0" xr:uid="{2FAFB650-F4A0-43AA-A1A4-FD1CE25983D6}">
+    <comment ref="A70" authorId="0" shapeId="0" xr:uid="{2FAFB650-F4A0-43AA-A1A4-FD1CE25983D6}">
       <text>
         <r>
           <rPr>
@@ -454,7 +480,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A74" authorId="0" shapeId="0" xr:uid="{04D6553C-E8DC-4A56-AAAA-8F71B24DF403}">
+    <comment ref="A76" authorId="0" shapeId="0" xr:uid="{04D6553C-E8DC-4A56-AAAA-8F71B24DF403}">
       <text>
         <r>
           <rPr>
@@ -1655,7 +1681,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="141">
   <si>
     <t>Machinery</t>
   </si>
@@ -2072,6 +2098,12 @@
   </si>
   <si>
     <t>Transaction cost from neighbour</t>
+  </si>
+  <si>
+    <t>Cartage from neighbour</t>
+  </si>
+  <si>
+    <t>Sup</t>
   </si>
 </sst>
 </file>
@@ -2658,10 +2690,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF2F00E-8A84-429F-9A28-0BBAA9C21CDC}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2846,162 +2878,119 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B29" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="B30" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="5" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B34" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B34" s="6">
-        <v>43814</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B36" s="4">
-        <v>5</v>
+        <v>104</v>
+      </c>
+      <c r="B36" s="6">
+        <v>43814</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B38" s="6">
-        <v>43692</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
-    </row>
+        <v>105</v>
+      </c>
+      <c r="B38" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>121</v>
+        <v>134</v>
+      </c>
+      <c r="B40" s="6">
+        <v>43692</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41" s="4">
-        <v>295</v>
-      </c>
-      <c r="C41" s="4">
-        <v>280</v>
-      </c>
-      <c r="D41" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="E41" s="4">
-        <f t="shared" ref="E41:E50" si="0">1-D41</f>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="F41" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="G41" s="4">
-        <v>12.05</v>
-      </c>
-      <c r="H41" s="4">
-        <f>0.86*1.05</f>
-        <v>0.90300000000000002</v>
-      </c>
+      <c r="A41" s="3"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="4">
-        <v>295</v>
-      </c>
-      <c r="C42" s="4">
-        <v>265</v>
-      </c>
-      <c r="D42" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="E42" s="4">
-        <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="F42" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="G42" s="4">
-        <v>13.45</v>
-      </c>
-      <c r="H42" s="4">
-        <f>0.86*1.05</f>
-        <v>0.90300000000000002</v>
+        <v>92</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B43" s="4">
-        <v>235</v>
-      </c>
-      <c r="C43" s="4"/>
+        <v>295</v>
+      </c>
+      <c r="C43" s="4">
+        <v>280</v>
+      </c>
       <c r="D43" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E43" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="E43:E52" si="0">1-D43</f>
+        <v>0.19999999999999996</v>
       </c>
       <c r="F43" s="4">
         <v>0.15</v>
       </c>
       <c r="G43" s="4">
-        <v>12.85</v>
+        <v>12.05</v>
       </c>
       <c r="H43" s="4">
         <f>0.86*1.05</f>
@@ -3010,24 +2999,26 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>95</v>
+        <v>4</v>
       </c>
       <c r="B44" s="4">
-        <v>150</v>
-      </c>
-      <c r="C44" s="4"/>
+        <v>295</v>
+      </c>
+      <c r="C44" s="4">
+        <v>265</v>
+      </c>
       <c r="D44" s="4">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="E44" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="F44" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="G44" s="4">
-        <v>1.5</v>
+        <v>13.45</v>
       </c>
       <c r="H44" s="4">
         <f>0.86*1.05</f>
@@ -3036,10 +3027,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B45" s="4">
-        <v>550</v>
+        <v>235</v>
       </c>
       <c r="C45" s="4"/>
       <c r="D45" s="4">
@@ -3050,22 +3041,22 @@
         <v>0</v>
       </c>
       <c r="F45" s="4">
-        <v>0.12</v>
+        <v>0.15</v>
       </c>
       <c r="G45" s="4">
-        <v>21.95</v>
+        <v>12.85</v>
       </c>
       <c r="H45" s="4">
-        <f>1.04*1.05</f>
-        <v>1.0920000000000001</v>
+        <f>0.86*1.05</f>
+        <v>0.90300000000000002</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
-        <v>9</v>
+        <v>95</v>
       </c>
       <c r="B46" s="4">
-        <v>550</v>
+        <v>150</v>
       </c>
       <c r="C46" s="4"/>
       <c r="D46" s="4">
@@ -3076,22 +3067,22 @@
         <v>0</v>
       </c>
       <c r="F46" s="4">
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="G46" s="4">
-        <v>21.95</v>
+        <v>1.5</v>
       </c>
       <c r="H46" s="4">
-        <f>1.04*1.05</f>
-        <v>1.0920000000000001</v>
+        <f>0.86*1.05</f>
+        <v>0.90300000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B47" s="4">
-        <v>305</v>
+        <v>550</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="4">
@@ -3102,10 +3093,10 @@
         <v>0</v>
       </c>
       <c r="F47" s="4">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="G47" s="4">
-        <v>12.05</v>
+        <v>21.95</v>
       </c>
       <c r="H47" s="4">
         <f>1.04*1.05</f>
@@ -3114,10 +3105,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" s="4">
-        <v>350</v>
+        <v>550</v>
       </c>
       <c r="C48" s="4"/>
       <c r="D48" s="4">
@@ -3128,10 +3119,10 @@
         <v>0</v>
       </c>
       <c r="F48" s="4">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="G48" s="4">
-        <v>15.85</v>
+        <v>21.95</v>
       </c>
       <c r="H48" s="4">
         <f>1.04*1.05</f>
@@ -3140,9 +3131,11 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B49" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="B49" s="4">
+        <v>305</v>
+      </c>
       <c r="C49" s="4"/>
       <c r="D49" s="4">
         <v>1</v>
@@ -3155,7 +3148,7 @@
         <v>0.15</v>
       </c>
       <c r="G49" s="4">
-        <v>15.85</v>
+        <v>12.05</v>
       </c>
       <c r="H49" s="4">
         <f>1.04*1.05</f>
@@ -3164,9 +3157,11 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="B50" s="4">
+        <v>350</v>
+      </c>
       <c r="C50" s="4"/>
       <c r="D50" s="4">
         <v>1</v>
@@ -3182,13 +3177,13 @@
         <v>15.85</v>
       </c>
       <c r="H50" s="4">
-        <f t="shared" ref="H50:H51" si="1">1.04*1.05</f>
+        <f>1.04*1.05</f>
         <v>1.0920000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -3196,7 +3191,7 @@
         <v>1</v>
       </c>
       <c r="E51" s="4">
-        <f>1-D51</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F51" s="4">
@@ -3206,106 +3201,146 @@
         <v>15.85</v>
       </c>
       <c r="H51" s="4">
+        <f>1.04*1.05</f>
+        <v>1.0920000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4">
+        <v>1</v>
+      </c>
+      <c r="E52" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F52" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G52" s="4">
+        <v>15.85</v>
+      </c>
+      <c r="H52" s="4">
+        <f t="shared" ref="H52:H53" si="1">1.04*1.05</f>
+        <v>1.0920000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4">
+        <v>1</v>
+      </c>
+      <c r="E53" s="4">
+        <f>1-D53</f>
+        <v>0</v>
+      </c>
+      <c r="F53" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="G53" s="4">
+        <v>15.85</v>
+      </c>
+      <c r="H53" s="4">
         <f t="shared" si="1"/>
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="4">
+      <c r="B56" s="4">
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="3"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B57" s="4">
-        <v>624</v>
-      </c>
+    <row r="57" spans="1:8" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="3"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="4">
-        <v>455</v>
+        <v>113</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
       <c r="B59" s="4">
-        <v>401</v>
+        <v>624</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B60" s="4">
-        <v>440</v>
+        <v>455</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B61" s="4">
-        <v>339</v>
+        <v>401</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B62" s="4">
-        <v>541</v>
+        <v>440</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" s="4">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" s="4">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B65" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B66" s="4">
-        <v>80000</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B68" s="4">
         <v>80000</v>
@@ -3313,49 +3348,57 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B70" s="4">
-        <v>0.09</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B72" s="4">
-        <v>3.5000000000000003E-2</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B74" s="4">
-        <v>2.3E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B76" s="4">
-        <v>28</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B78" s="4">
-        <v>0.09</v>
+        <v>28</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B80" s="4">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="B80" s="4">
+      <c r="B82" s="4">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
completed sup and sup pyomo, Added dep, asset, minroe constraints, altered mach option handling, alter period functions slightly
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -8,91 +8,97 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33DC070-C5AA-40E1-921E-D707C3505019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1AFB8B-3259-4D0C-AE0E-0DE4BC4831DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
     <sheet name="Finance" sheetId="2" r:id="rId2"/>
     <sheet name="Feed Budget" sheetId="5" r:id="rId3"/>
-    <sheet name="Mach General" sheetId="4" r:id="rId4"/>
-    <sheet name="Mach 1" sheetId="3" r:id="rId5"/>
+    <sheet name="Sup Feed" sheetId="6" r:id="rId4"/>
+    <sheet name="Mach General" sheetId="4" r:id="rId5"/>
+    <sheet name="Mach 1" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="approx_hay_yield" localSheetId="3">'Mach General'!$B$3</definedName>
+    <definedName name="approx_hay_yield" localSheetId="4">'Mach General'!$B$3</definedName>
     <definedName name="cart_hay" localSheetId="0">Price!$B$26</definedName>
     <definedName name="casual_cost">Price!$B$78</definedName>
     <definedName name="casual_super">Price!$B$80</definedName>
     <definedName name="casual_workers_comp">Price!$B$82</definedName>
-    <definedName name="clearing_value" localSheetId="4">'Mach 1'!$A$8:$B$21</definedName>
+    <definedName name="clearing_value" localSheetId="5">'Mach 1'!$A$8:$B$21</definedName>
     <definedName name="contract_bail" localSheetId="0">Price!$B$24</definedName>
     <definedName name="contract_harv_cost" localSheetId="0">Price!$A$7:$B$17</definedName>
-    <definedName name="contract_harv_eff" localSheetId="3">'Mach General'!$B$21</definedName>
-    <definedName name="contract_harvest_speed" localSheetId="3">'Mach General'!$A$23:$B$33</definedName>
-    <definedName name="contract_harvester_width" localSheetId="3">'Mach General'!$B$19</definedName>
+    <definedName name="contract_harv_eff" localSheetId="4">'Mach General'!$B$21</definedName>
+    <definedName name="contract_harvest_speed" localSheetId="4">'Mach General'!$A$23:$B$33</definedName>
+    <definedName name="contract_harvester_width" localSheetId="4">'Mach General'!$B$19</definedName>
     <definedName name="contract_mow_hay" localSheetId="0">Price!$B$22</definedName>
     <definedName name="contract_seed_cost" localSheetId="0">Price!$B$19</definedName>
     <definedName name="credit_interest" localSheetId="1">Finance!$B$3</definedName>
     <definedName name="crp_insurance_date">Price!$B$40</definedName>
     <definedName name="debit_interest" localSheetId="1">Finance!$B$5</definedName>
-    <definedName name="dep_area" localSheetId="4">'Mach 1'!$B$3</definedName>
+    <definedName name="dep_area" localSheetId="5">'Mach 1'!$B$3</definedName>
     <definedName name="diesel" localSheetId="0">Price!$B$3</definedName>
     <definedName name="diesel_rebate" localSheetId="0">Price!$B$5</definedName>
-    <definedName name="draft_seeding" localSheetId="4">'Mach 1'!$B$35</definedName>
+    <definedName name="draft_seeding" localSheetId="5">'Mach 1'!$B$35</definedName>
+    <definedName name="equip_insurance">Finance!$B$11</definedName>
     <definedName name="fert_cartage_cost" localSheetId="0">Price!$B$56</definedName>
     <definedName name="fert_cost" localSheetId="0">Price!$A$58:$B$65</definedName>
     <definedName name="fixed_dep" localSheetId="1">Finance!$B$8</definedName>
     <definedName name="flagfall" localSheetId="0">Price!$B$34</definedName>
-    <definedName name="fuel_adj_tractor" localSheetId="4">'Mach 1'!$B$37</definedName>
+    <definedName name="fuel_adj_tractor" localSheetId="5">'Mach 1'!$B$37</definedName>
+    <definedName name="grain_density">'Sup Feed'!$I$26:$N$28</definedName>
     <definedName name="grain_income_date" localSheetId="0">Price!$B$36</definedName>
     <definedName name="grain_income_length" localSheetId="0">Price!$B$38</definedName>
     <definedName name="grain_price" localSheetId="0">Price!$A$42:$H$53</definedName>
-    <definedName name="harv_eff" localSheetId="4">'Mach 1'!$B$65</definedName>
-    <definedName name="harv_fuel_consumption" localSheetId="4">'Mach 1'!$B$61</definedName>
-    <definedName name="harvest_maint" localSheetId="4">'Mach 1'!$A$79:$B$89</definedName>
-    <definedName name="harvest_speed" localSheetId="4">'Mach 1'!$A$67:$B$77</definedName>
-    <definedName name="harvest_yield" localSheetId="3">'Mach General'!$A$6:$B$16</definedName>
-    <definedName name="harvester_width" localSheetId="4">'Mach 1'!$B$59</definedName>
+    <definedName name="harv_eff" localSheetId="5">'Mach 1'!$B$65</definedName>
+    <definedName name="harv_fuel_consumption" localSheetId="5">'Mach 1'!$B$61</definedName>
+    <definedName name="harvest_maint" localSheetId="5">'Mach 1'!$A$79:$B$89</definedName>
+    <definedName name="harvest_speed" localSheetId="5">'Mach 1'!$A$67:$B$77</definedName>
+    <definedName name="harvest_yield" localSheetId="4">'Mach General'!$A$6:$B$16</definedName>
+    <definedName name="harvester_width" localSheetId="5">'Mach 1'!$B$59</definedName>
     <definedName name="manager_cost">Price!$B$68</definedName>
-    <definedName name="oil_grease_factor_harv" localSheetId="4">'Mach 1'!$B$63</definedName>
-    <definedName name="oil_grease_factor_tractor" localSheetId="4">'Mach 1'!$B$24</definedName>
+    <definedName name="minroe">Finance!$B$17</definedName>
+    <definedName name="oil_grease_factor_harv" localSheetId="5">'Mach 1'!$B$63</definedName>
+    <definedName name="oil_grease_factor_tractor" localSheetId="5">'Mach 1'!$B$24</definedName>
+    <definedName name="opportunity_cost_capital">Finance!$B$14</definedName>
     <definedName name="permanent_cost">Price!$B$70</definedName>
     <definedName name="permanent_ls_leave">Price!$B$76</definedName>
     <definedName name="permanent_super">Price!$B$72</definedName>
     <definedName name="permanent_workers_comp">Price!$B$74</definedName>
-    <definedName name="repair_maint_factor_tractor" localSheetId="4">'Mach 1'!$B$26</definedName>
-    <definedName name="ria" localSheetId="2">'Feed Budget'!$B$3</definedName>
-    <definedName name="rib" localSheetId="2">'Feed Budget'!$B$5</definedName>
-    <definedName name="rid" localSheetId="2">'Feed Budget'!$B$13</definedName>
-    <definedName name="rig" localSheetId="2">'Feed Budget'!$B$11</definedName>
-    <definedName name="rih" localSheetId="2">'Feed Budget'!$B$9</definedName>
-    <definedName name="rik" localSheetId="2">'Feed Budget'!$B$7</definedName>
-    <definedName name="seeder_base_crop" localSheetId="4">'Mach 1'!#REF!</definedName>
-    <definedName name="seeder_speed_base" localSheetId="4">'Mach 1'!$B$33</definedName>
-    <definedName name="seeder_speed_crop_adj" localSheetId="4">'Mach 1'!$A$41:$B$56</definedName>
-    <definedName name="seeder_width" localSheetId="4">'Mach 1'!$B$29</definedName>
-    <definedName name="seeding_eff" localSheetId="4">'Mach 1'!$B$31</definedName>
-    <definedName name="sprayer_eff" localSheetId="4">'Mach 1'!$B$96</definedName>
-    <definedName name="sprayer_fuel_consumption" localSheetId="4">'Mach 1'!$B$98</definedName>
-    <definedName name="sprayer_maint" localSheetId="4">'Mach 1'!$B$100</definedName>
-    <definedName name="sprayer_speed" localSheetId="4">'Mach 1'!$B$94</definedName>
-    <definedName name="sprayer_width" localSheetId="4">'Mach 1'!$B$92</definedName>
-    <definedName name="spreader_cap" localSheetId="4">'Mach 1'!$B$114</definedName>
-    <definedName name="spreader_eff" localSheetId="4">'Mach 1'!$B$120</definedName>
-    <definedName name="spreader_fuel" localSheetId="4">'Mach 1'!$B$103</definedName>
-    <definedName name="spreader_maint" localSheetId="4">'Mach 1'!$B$122</definedName>
-    <definedName name="spreader_speed" localSheetId="4">'Mach 1'!$B$118</definedName>
-    <definedName name="spreader_width" localSheetId="4">'Mach 1'!$A$105:$B$112</definedName>
-    <definedName name="stubble_fuel_consumption" localSheetId="4">'Mach 1'!$B$125</definedName>
-    <definedName name="stubble_maint" localSheetId="4">'Mach 1'!$B$127</definedName>
+    <definedName name="repair_maint_factor_tractor" localSheetId="5">'Mach 1'!$B$26</definedName>
+    <definedName name="ria" localSheetId="2">'Feed Budget'!$H$3</definedName>
+    <definedName name="rib" localSheetId="2">'Feed Budget'!$H$5</definedName>
+    <definedName name="rid" localSheetId="2">'Feed Budget'!$H$13</definedName>
+    <definedName name="rig" localSheetId="2">'Feed Budget'!$H$11</definedName>
+    <definedName name="rih" localSheetId="2">'Feed Budget'!$H$9</definedName>
+    <definedName name="rik" localSheetId="2">'Feed Budget'!$H$7</definedName>
+    <definedName name="seeder_base_crop" localSheetId="5">'Mach 1'!#REF!</definedName>
+    <definedName name="seeder_speed_base" localSheetId="5">'Mach 1'!$B$33</definedName>
+    <definedName name="seeder_speed_crop_adj" localSheetId="5">'Mach 1'!$A$41:$B$56</definedName>
+    <definedName name="seeder_width" localSheetId="5">'Mach 1'!$B$29</definedName>
+    <definedName name="seeding_eff" localSheetId="5">'Mach 1'!$B$31</definedName>
+    <definedName name="sprayer_eff" localSheetId="5">'Mach 1'!$B$96</definedName>
+    <definedName name="sprayer_fuel_consumption" localSheetId="5">'Mach 1'!$B$98</definedName>
+    <definedName name="sprayer_maint" localSheetId="5">'Mach 1'!$B$100</definedName>
+    <definedName name="sprayer_speed" localSheetId="5">'Mach 1'!$B$94</definedName>
+    <definedName name="sprayer_width" localSheetId="5">'Mach 1'!$B$92</definedName>
+    <definedName name="spreader_cap" localSheetId="5">'Mach 1'!$B$114</definedName>
+    <definedName name="spreader_eff" localSheetId="5">'Mach 1'!$B$120</definedName>
+    <definedName name="spreader_fuel" localSheetId="5">'Mach 1'!$B$103</definedName>
+    <definedName name="spreader_maint" localSheetId="5">'Mach 1'!$B$122</definedName>
+    <definedName name="spreader_speed" localSheetId="5">'Mach 1'!$B$118</definedName>
+    <definedName name="spreader_width" localSheetId="5">'Mach 1'!$A$105:$B$112</definedName>
+    <definedName name="stubble_fuel_consumption" localSheetId="5">'Mach 1'!$B$125</definedName>
+    <definedName name="stubble_maint" localSheetId="5">'Mach 1'!$B$127</definedName>
     <definedName name="sup_cartage">Price!$B$29</definedName>
-    <definedName name="sup_feed">'Mach 1'!$A$130:$C$134</definedName>
+    <definedName name="sup_feed">'Mach 1'!$A$130:$C$135</definedName>
+    <definedName name="sup_md_vol">'Sup Feed'!$I$10:$N$14</definedName>
     <definedName name="sup_transaction">Price!$B$31</definedName>
-    <definedName name="tillage_maint" localSheetId="4">'Mach 1'!$B$39</definedName>
-    <definedName name="time_fill_spreader" localSheetId="4">'Mach 1'!$B$116</definedName>
+    <definedName name="tillage_maint" localSheetId="5">'Mach 1'!$B$39</definedName>
+    <definedName name="time_fill_spreader" localSheetId="5">'Mach 1'!$B$116</definedName>
     <definedName name="variable_dep" localSheetId="1">Finance!#REF!</definedName>
-    <definedName name="variable_dep" localSheetId="4">'Mach 1'!$B$5</definedName>
+    <definedName name="variable_dep" localSheetId="5">'Mach 1'!$B$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -514,7 +520,7 @@
     <author>Michael Young</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{65FB491D-FBC4-4622-9AD5-102176C7868B}">
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{65FB491D-FBC4-4622-9AD5-102176C7868B}">
       <text>
         <r>
           <rPr>
@@ -538,7 +544,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="0" shapeId="0" xr:uid="{EE45B148-27DF-494E-A581-EDAF0BCAD8F1}">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{EE45B148-27DF-494E-A581-EDAF0BCAD8F1}">
       <text>
         <r>
           <rPr>
@@ -562,7 +568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{BBBC8DDA-9EB5-4A78-AA8B-A714B120F5AA}">
+    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{BBBC8DDA-9EB5-4A78-AA8B-A714B120F5AA}">
       <text>
         <r>
           <rPr>
@@ -586,7 +592,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{70E7D073-EB49-4E92-863F-C33E4291D308}">
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{70E7D073-EB49-4E92-863F-C33E4291D308}">
       <text>
         <r>
           <rPr>
@@ -610,7 +616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{C06B083F-7BA6-4C07-97C8-C57DA19E1E4F}">
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{C06B083F-7BA6-4C07-97C8-C57DA19E1E4F}">
       <text>
         <r>
           <rPr>
@@ -634,7 +640,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{6EADF2AF-64EC-4DE3-954A-3622C455C086}">
+    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{6EADF2AF-64EC-4DE3-954A-3622C455C086}">
       <text>
         <r>
           <rPr>
@@ -668,99 +674,75 @@
     <author>Michael Young</author>
   </authors>
   <commentList>
-    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{CAED6C43-0444-4DB1-96AB-80B613C18A0E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael Young:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-used to calibrate contract hay mowing price </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{75EA64EF-7BBD-4479-A80A-FE0266829E9E}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael Young:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-crop yields that harverster speed is calibrated to (these should just be approx). Used to calc the t/hr harvested for own harv and contract</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{94CD2613-4C0E-4578-A436-C34E827BBAB0}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael Young:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-yes these inputs may vary slightly between property but I suspect they wouldn't get changed because they are low priority so that’s why they are here</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{90BB259D-A774-471C-98EA-3AA91E04E59C}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael Young:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-contract harvester speed calibrated to the aprox yields above (km/hr)</t>
+    <comment ref="I27" authorId="0" shapeId="0" xr:uid="{3DC02098-1628-4880-9C5F-57BC4ABDAA2B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+used to match up values from above</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I28" authorId="0" shapeId="0" xr:uid="{76302044-C55B-483C-9985-192E6879EAED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Conversion Factor from m3 to t</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N28" authorId="0" shapeId="0" xr:uid="{C3DF5EF6-5F7E-41B0-9113-E06058B6E139}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+already in t from above</t>
         </r>
       </text>
     </comment>
@@ -774,6 +756,112 @@
     <author>Michael Young</author>
   </authors>
   <commentList>
+    <comment ref="A3" authorId="0" shapeId="0" xr:uid="{CAED6C43-0444-4DB1-96AB-80B613C18A0E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+used to calibrate contract hay mowing price </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{75EA64EF-7BBD-4479-A80A-FE0266829E9E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+crop yields that harverster speed is calibrated to (these should just be approx). Used to calc the t/hr harvested for own harv and contract</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{94CD2613-4C0E-4578-A436-C34E827BBAB0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+yes these inputs may vary slightly between property but I suspect they wouldn't get changed because they are low priority so that’s why they are here</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{90BB259D-A774-471C-98EA-3AA91E04E59C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+contract harvester speed calibrated to the aprox yields above (km/hr)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Michael Young</author>
+  </authors>
+  <commentList>
     <comment ref="A3" authorId="0" shapeId="0" xr:uid="{AAFD58D5-AE8A-4CCB-9657-C9B138C0F600}">
       <text>
         <r>
@@ -1673,6 +1761,54 @@
           </rPr>
           <t xml:space="preserve">
 stubble handeler repairs and maint $/ha (doesn't include tractor, that is recorded in the tractor section)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B130" authorId="0" shapeId="0" xr:uid="{115DEECC-C4B6-40BD-AC87-F415E26BB0BB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+r&amp;m</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C130" authorId="0" shapeId="0" xr:uid="{735B890C-028D-403F-91EB-7DDBBB95923A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+L/t</t>
         </r>
       </text>
     </comment>
@@ -1681,7 +1817,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="167">
   <si>
     <t>Machinery</t>
   </si>
@@ -2091,12 +2227,6 @@
     <t>Sheep Feeding</t>
   </si>
   <si>
-    <t>r&amp;m</t>
-  </si>
-  <si>
-    <t>L/t</t>
-  </si>
-  <si>
     <t>Transaction cost from neighbour</t>
   </si>
   <si>
@@ -2104,13 +2234,101 @@
   </si>
   <si>
     <t>Sup</t>
+  </si>
+  <si>
+    <t>Equipment insrance rate</t>
+  </si>
+  <si>
+    <t>Insurance</t>
+  </si>
+  <si>
+    <t>«</t>
+  </si>
+  <si>
+    <t>Däta</t>
+  </si>
+  <si>
+    <t>LIVESTOCK FEED - ENERGY, VOLUMES, EATEN</t>
+  </si>
+  <si>
+    <t>Energy, Dry Matter  x  Feed Type</t>
+  </si>
+  <si>
+    <t>MJ / t DM</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>% consumed</t>
+  </si>
+  <si>
+    <t>»</t>
+  </si>
+  <si>
+    <t>maint</t>
+  </si>
+  <si>
+    <t>litres</t>
+  </si>
+  <si>
+    <t>t / m3</t>
+  </si>
+  <si>
+    <t>hay</t>
+  </si>
+  <si>
+    <t>grain</t>
+  </si>
+  <si>
+    <t>silo type</t>
+  </si>
+  <si>
+    <t>crop</t>
+  </si>
+  <si>
+    <t>Cost item  x  Feed Type</t>
+  </si>
+  <si>
+    <t>LIVESTOCK FEEDS - STORAGE COSTS</t>
+  </si>
+  <si>
+    <t>cp</t>
+  </si>
+  <si>
+    <t>dry matter content</t>
+  </si>
+  <si>
+    <t>prop consumed</t>
+  </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>ROE</t>
+  </si>
+  <si>
+    <t>opportunity cost capital</t>
+  </si>
+  <si>
+    <t>min return on expenditure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">opportunity cost </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode=";;;"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2151,8 +2369,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2171,8 +2402,43 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="29"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="27"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2189,11 +2455,125 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="9" borderId="9">
+      <alignment horizontal="right"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2211,8 +2591,87 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="8" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Formula 1" xfId="2" xr:uid="{73E7623B-26A4-407F-9297-1EB699330B2D}"/>
+    <cellStyle name="Input 2" xfId="1" xr:uid="{BBF70FE2-15FC-4036-A49C-819466437B06}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2692,7 +3151,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
@@ -2878,12 +3337,12 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B29" s="8">
         <v>15</v>
@@ -2894,7 +3353,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B31" s="8">
         <v>20</v>
@@ -3412,10 +3871,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D7B669-D46E-465D-AB74-E6E4468D232E}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:B8"/>
+  <dimension ref="A2:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3459,6 +3918,45 @@
         <v>0.02</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B14" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B17" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3467,74 +3965,80 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED9269B-34A0-4B4D-B79F-55BA46418231}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:B13"/>
+  <dimension ref="E2:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="2.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2" style="1" customWidth="1"/>
+    <col min="3" max="3" width="0.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="1.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.21875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G2" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G3" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="4">
+      <c r="H3" s="4">
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="4" spans="7:8" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B5" s="4">
+      <c r="H5" s="4">
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="6" spans="7:8" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G7" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="4">
+      <c r="H7" s="4">
         <v>1.4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="8" spans="7:8" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G9" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="4">
+      <c r="H9" s="4">
         <v>1.7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="10" spans="7:8" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G11" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B11" s="4">
+      <c r="H11" s="4">
         <v>0.17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+    <row r="12" spans="7:8" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G13" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B13" s="4">
+      <c r="H13" s="4">
         <v>0.8</v>
       </c>
     </row>
@@ -3545,6 +4049,1052 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBAE29A-401D-4B75-B63C-3693AC93217E}">
+  <dimension ref="A1:Z32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.44140625" customWidth="1"/>
+    <col min="2" max="2" width="2.21875" customWidth="1"/>
+    <col min="3" max="4" width="2.77734375" customWidth="1"/>
+    <col min="5" max="5" width="2" customWidth="1"/>
+    <col min="6" max="6" width="4.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+    </row>
+    <row r="2" spans="1:26" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+    </row>
+    <row r="3" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+    </row>
+    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="18"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="21"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+    </row>
+    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+    </row>
+    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="24">
+        <v>38576.728773148148</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="23"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="21"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+    </row>
+    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="21"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+    </row>
+    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+    </row>
+    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="26"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="21"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+    </row>
+    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="L10" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="M10" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+    </row>
+    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="28"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="J11" s="33">
+        <v>11400</v>
+      </c>
+      <c r="K11" s="33">
+        <v>12100</v>
+      </c>
+      <c r="L11" s="33">
+        <v>13300</v>
+      </c>
+      <c r="M11" s="33">
+        <v>12100</v>
+      </c>
+      <c r="N11" s="33">
+        <v>7000</v>
+      </c>
+      <c r="O11" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="P11" s="34"/>
+      <c r="Q11" s="34"/>
+      <c r="R11" s="34"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+      <c r="U11" s="34"/>
+      <c r="V11" s="31"/>
+      <c r="W11" s="21"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+    </row>
+    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="28"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="45" t="s">
+        <v>158</v>
+      </c>
+      <c r="J12" s="33">
+        <v>0.1</v>
+      </c>
+      <c r="K12" s="33">
+        <v>0.12</v>
+      </c>
+      <c r="L12" s="33">
+        <v>0.3</v>
+      </c>
+      <c r="M12" s="33">
+        <v>0.3</v>
+      </c>
+      <c r="N12" s="33">
+        <v>0.08</v>
+      </c>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="34"/>
+      <c r="U12" s="34"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+    </row>
+    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="28"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="J13" s="33">
+        <v>90</v>
+      </c>
+      <c r="K13" s="33">
+        <v>90</v>
+      </c>
+      <c r="L13" s="33">
+        <v>90</v>
+      </c>
+      <c r="M13" s="33">
+        <v>90</v>
+      </c>
+      <c r="N13" s="33">
+        <v>90</v>
+      </c>
+      <c r="O13" s="32" t="s">
+        <v>146</v>
+      </c>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="34"/>
+      <c r="R13" s="34"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="34"/>
+      <c r="U13" s="34"/>
+      <c r="V13" s="31"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+    </row>
+    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="28"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="J14" s="33">
+        <v>80</v>
+      </c>
+      <c r="K14" s="33">
+        <v>80</v>
+      </c>
+      <c r="L14" s="33">
+        <v>95</v>
+      </c>
+      <c r="M14" s="33">
+        <v>80</v>
+      </c>
+      <c r="N14" s="33">
+        <v>75</v>
+      </c>
+      <c r="O14" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="P14" s="34"/>
+      <c r="Q14" s="34"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="34"/>
+      <c r="T14" s="34"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="21"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+    </row>
+    <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
+      <c r="M15" s="36"/>
+      <c r="N15" s="34"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="34"/>
+      <c r="Q15" s="34"/>
+      <c r="R15" s="34"/>
+      <c r="S15" s="34"/>
+      <c r="T15" s="34"/>
+      <c r="U15" s="34"/>
+      <c r="V15" s="31"/>
+      <c r="W15" s="21"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+    </row>
+    <row r="16" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="39"/>
+      <c r="V16" s="31"/>
+      <c r="W16" s="21"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+    </row>
+    <row r="17" spans="1:26" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="41" t="str">
+        <f>G4</f>
+        <v>LIVESTOCK FEED - ENERGY, VOLUMES, EATEN</v>
+      </c>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="40"/>
+      <c r="W17" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+    </row>
+    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="13"/>
+    </row>
+    <row r="19" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="12"/>
+    </row>
+    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="16"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="Z20" s="13"/>
+    </row>
+    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="18"/>
+      <c r="U21" s="20"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="21"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
+    </row>
+    <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="20"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="20"/>
+      <c r="V22" s="20"/>
+      <c r="W22" s="21"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
+    </row>
+    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="24">
+        <v>43909</v>
+      </c>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="23"/>
+      <c r="U23" s="20"/>
+      <c r="V23" s="20"/>
+      <c r="W23" s="21"/>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="13"/>
+    </row>
+    <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
+      <c r="Z24" s="13"/>
+    </row>
+    <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="25"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="13"/>
+      <c r="Y25" s="13"/>
+      <c r="Z25" s="13"/>
+    </row>
+    <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="J26" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="K26" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="M26" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="N26" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="25"/>
+      <c r="T26" s="25"/>
+      <c r="U26" s="25"/>
+      <c r="V26" s="25"/>
+      <c r="W26" s="21"/>
+      <c r="X26" s="13"/>
+      <c r="Y26" s="13"/>
+      <c r="Z26" s="13"/>
+    </row>
+    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="J27" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="K27" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="L27" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="M27" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="N27" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="30"/>
+      <c r="T27" s="30"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="31"/>
+      <c r="W27" s="21"/>
+      <c r="X27" s="13"/>
+      <c r="Y27" s="13"/>
+      <c r="Z27" s="13"/>
+    </row>
+    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="11"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="28"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="J28" s="44">
+        <v>0.45</v>
+      </c>
+      <c r="K28" s="44">
+        <v>0.62</v>
+      </c>
+      <c r="L28" s="44">
+        <v>0.72</v>
+      </c>
+      <c r="M28" s="44">
+        <v>0.75</v>
+      </c>
+      <c r="N28" s="43">
+        <v>1</v>
+      </c>
+      <c r="O28" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="P28" s="34"/>
+      <c r="Q28" s="34"/>
+      <c r="R28" s="34"/>
+      <c r="S28" s="34"/>
+      <c r="T28" s="34"/>
+      <c r="U28" s="34"/>
+      <c r="V28" s="31"/>
+      <c r="W28" s="21"/>
+      <c r="X28" s="13"/>
+      <c r="Y28" s="13"/>
+      <c r="Z28" s="13"/>
+    </row>
+    <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="O29" s="31"/>
+      <c r="P29" s="31"/>
+      <c r="Q29" s="31"/>
+      <c r="R29" s="31"/>
+      <c r="S29" s="31"/>
+      <c r="T29" s="31"/>
+      <c r="U29" s="31"/>
+      <c r="V29" s="31"/>
+      <c r="W29" s="21"/>
+      <c r="X29" s="13"/>
+      <c r="Y29" s="13"/>
+      <c r="Z29" s="13"/>
+    </row>
+    <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
+      <c r="M30" s="31"/>
+      <c r="N30" s="31"/>
+      <c r="O30" s="31"/>
+      <c r="P30" s="31"/>
+      <c r="Q30" s="31"/>
+      <c r="R30" s="31"/>
+      <c r="S30" s="31"/>
+      <c r="T30" s="31"/>
+      <c r="U30" s="31"/>
+      <c r="V30" s="31"/>
+      <c r="W30" s="21"/>
+      <c r="X30" s="13"/>
+      <c r="Y30" s="13"/>
+      <c r="Z30" s="13"/>
+    </row>
+    <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="11"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="41" t="str">
+        <f>G21</f>
+        <v>LIVESTOCK FEEDS - STORAGE COSTS</v>
+      </c>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="40"/>
+      <c r="N31" s="40"/>
+      <c r="O31" s="40"/>
+      <c r="P31" s="40"/>
+      <c r="Q31" s="40"/>
+      <c r="R31" s="40"/>
+      <c r="S31" s="40"/>
+      <c r="T31" s="40"/>
+      <c r="U31" s="40"/>
+      <c r="V31" s="40"/>
+      <c r="W31" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
+      <c r="Z31" s="13"/>
+    </row>
+    <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16CCB3BF-D039-4C99-9E77-946FA99C1AAC}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:B33"/>
@@ -3782,13 +5332,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A689975D-2450-4766-909D-59787FB65B03}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A2:C134"/>
+  <dimension ref="A2:C135"/>
   <sheetViews>
     <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4557,10 +6107,10 @@
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="8"/>
       <c r="B130" s="8" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
@@ -4598,12 +6148,23 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="9" t="s">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="B134" s="8">
         <v>1</v>
       </c>
       <c r="C134" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A135" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B135" s="8">
+        <v>1</v>
+      </c>
+      <c r="C135" s="8">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
stubble pyomo, stubble inputs to xl, updates to pas pyomo, updates to sow constrain, removal of dis agregated phases set
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1AFB8B-3259-4D0C-AE0E-0DE4BC4831DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB362F9D-4FC4-4B85-93D0-11EED484EF2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -313,6 +313,30 @@
           </rPr>
           <t xml:space="preserve">
 date when crop insurance is paid</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C42" authorId="0" shapeId="0" xr:uid="{9D6EEDD7-6AB3-4544-8B80-9F0128913CFF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+need a price here so model can't buy seconds for free</t>
         </r>
       </text>
     </comment>
@@ -3151,8 +3175,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50:C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3491,7 +3515,9 @@
       <c r="B45" s="4">
         <v>235</v>
       </c>
-      <c r="C45" s="4"/>
+      <c r="C45" s="4">
+        <v>235</v>
+      </c>
       <c r="D45" s="4">
         <v>1</v>
       </c>
@@ -3517,7 +3543,9 @@
       <c r="B46" s="4">
         <v>150</v>
       </c>
-      <c r="C46" s="4"/>
+      <c r="C46" s="4">
+        <v>150</v>
+      </c>
       <c r="D46" s="4">
         <v>1</v>
       </c>
@@ -3543,7 +3571,9 @@
       <c r="B47" s="4">
         <v>550</v>
       </c>
-      <c r="C47" s="4"/>
+      <c r="C47" s="4">
+        <v>550</v>
+      </c>
       <c r="D47" s="4">
         <v>1</v>
       </c>
@@ -3569,7 +3599,9 @@
       <c r="B48" s="4">
         <v>550</v>
       </c>
-      <c r="C48" s="4"/>
+      <c r="C48" s="4">
+        <v>550</v>
+      </c>
       <c r="D48" s="4">
         <v>1</v>
       </c>
@@ -3595,7 +3627,9 @@
       <c r="B49" s="4">
         <v>305</v>
       </c>
-      <c r="C49" s="4"/>
+      <c r="C49" s="4">
+        <v>305</v>
+      </c>
       <c r="D49" s="4">
         <v>1</v>
       </c>
@@ -3621,7 +3655,9 @@
       <c r="B50" s="4">
         <v>350</v>
       </c>
-      <c r="C50" s="4"/>
+      <c r="C50" s="4">
+        <v>350</v>
+      </c>
       <c r="D50" s="4">
         <v>1</v>
       </c>
@@ -3644,8 +3680,12 @@
       <c r="A51" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
+      <c r="B51" s="4">
+        <v>350</v>
+      </c>
+      <c r="C51" s="4">
+        <v>350</v>
+      </c>
       <c r="D51" s="4">
         <v>1</v>
       </c>
@@ -3668,8 +3708,12 @@
       <c r="A52" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
+      <c r="B52" s="4">
+        <v>350</v>
+      </c>
+      <c r="C52" s="4">
+        <v>350</v>
+      </c>
       <c r="D52" s="4">
         <v>1</v>
       </c>
@@ -3692,8 +3736,12 @@
       <c r="A53" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
+      <c r="B53" s="4">
+        <v>350</v>
+      </c>
+      <c r="C53" s="4">
+        <v>350</v>
+      </c>
       <c r="D53" s="4">
         <v>1</v>
       </c>
@@ -3873,7 +3921,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -3965,7 +4013,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED9269B-34A0-4B4D-B79F-55BA46418231}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="E2:H13"/>
+  <dimension ref="G2:H13"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:XFD39"/>

</xml_diff>

<commit_message>
read results to pickle, fix erosion, add overheads, mach insurance and assettr
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB362F9D-4FC4-4B85-93D0-11EED484EF2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A2A09D-66C2-45D2-BED9-5598EED3C828}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -57,6 +57,7 @@
     <definedName name="harvest_speed" localSheetId="5">'Mach 1'!$A$67:$B$77</definedName>
     <definedName name="harvest_yield" localSheetId="4">'Mach General'!$A$6:$B$16</definedName>
     <definedName name="harvester_width" localSheetId="5">'Mach 1'!$B$59</definedName>
+    <definedName name="insurance_date">'Mach General'!$B$35</definedName>
     <definedName name="manager_cost">Price!$B$68</definedName>
     <definedName name="minroe">Finance!$B$17</definedName>
     <definedName name="oil_grease_factor_harv" localSheetId="5">'Mach 1'!$B$63</definedName>
@@ -876,6 +877,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{05C603B3-DB35-4092-8F2F-DCC28789626E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+date when mach insurance is paid</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -1841,7 +1866,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="167">
   <si>
     <t>Machinery</t>
   </si>
@@ -3175,8 +3200,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:C53"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5145,16 +5170,17 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16CCB3BF-D039-4C99-9E77-946FA99C1AAC}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A2:B33"/>
+  <dimension ref="A2:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5371,6 +5397,14 @@
       </c>
       <c r="B33" s="4">
         <v>4.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="6">
+        <v>43554</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add crop yild from sim to crop.py
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D7CE6D-358C-4C06-B6AD-EFA5D2EBB7E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F735561B-ACAD-47A7-ACF3-3D3D7F888993}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
@@ -1117,7 +1117,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-max proportion of weeds remaining at a high level of the control
+max proportion of weeds killed at a high level of the control
 </t>
         </r>
       </text>
@@ -1312,7 +1312,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-below 1 can give strange results because at high weed densities there is less weed seeds set.</t>
+below 2 can give strange results when control is optimised because at high weed densities the total weed seed set is less.</t>
         </r>
       </text>
     </comment>
@@ -1384,7 +1384,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-max proportion of weeds remaining at a high level of the control
+max proportion of weeds killed at a high level of the control
 </t>
         </r>
       </text>
@@ -4509,6 +4509,89 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>60960</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{802F92D3-E8D6-4ECC-9846-022BBA38A3FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7810500" y="6797040"/>
+          <a:ext cx="3558540" cy="960120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100"/>
+            <a:t>When calabrating</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" baseline="0"/>
+            <a:t> note the y value when x = 0. Idealy this should be close to 0 to avoid 0 control level actually decreasing the weeds. Good link below to help visualise.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU">
+              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
+            </a:rPr>
+            <a:t>https://www.desmos.com/calculator/kbjcog1c73</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-AU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5350,7 +5433,7 @@
         <v>0.7</v>
       </c>
       <c r="E49" s="95">
-        <f>1-D49</f>
+        <f t="shared" ref="E49:E58" si="4">1-D49</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="F49" s="4">
@@ -5378,7 +5461,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="95">
-        <f>1-D50</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F50" s="4">
@@ -5406,7 +5489,7 @@
         <v>1</v>
       </c>
       <c r="E51" s="95">
-        <f>1-D51</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F51" s="4">
@@ -5434,7 +5517,7 @@
         <v>1</v>
       </c>
       <c r="E52" s="95">
-        <f>1-D52</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F52" s="4">
@@ -5462,7 +5545,7 @@
         <v>1</v>
       </c>
       <c r="E53" s="95">
-        <f>1-D53</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F53" s="4">
@@ -5472,7 +5555,7 @@
         <v>15.85</v>
       </c>
       <c r="H53" s="4">
-        <f t="shared" ref="H53:H58" si="4">1.04*1.05</f>
+        <f t="shared" ref="H53:H58" si="5">1.04*1.05</f>
         <v>1.0920000000000001</v>
       </c>
     </row>
@@ -5490,7 +5573,7 @@
         <v>1</v>
       </c>
       <c r="E54" s="95">
-        <f>1-D54</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F54" s="4">
@@ -5518,7 +5601,7 @@
         <v>1</v>
       </c>
       <c r="E55" s="95">
-        <f>1-D55</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F55" s="4">
@@ -5546,7 +5629,7 @@
         <v>1</v>
       </c>
       <c r="E56" s="95">
-        <f>1-D56</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F56" s="4">
@@ -5573,7 +5656,7 @@
         <v>1</v>
       </c>
       <c r="E57" s="95">
-        <f>1-D57</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F57" s="4">
@@ -5601,7 +5684,7 @@
         <v>1</v>
       </c>
       <c r="E58" s="95">
-        <f>1-D58</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F58" s="4">
@@ -5611,7 +5694,7 @@
         <v>15.85</v>
       </c>
       <c r="H58" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0920000000000001</v>
       </c>
     </row>
@@ -5629,7 +5712,7 @@
         <v>0.8</v>
       </c>
       <c r="E59" s="95">
-        <f t="shared" ref="E59:E60" si="5">1-D59</f>
+        <f t="shared" ref="E59:E60" si="6">1-D59</f>
         <v>0.19999999999999996</v>
       </c>
       <c r="F59" s="4">
@@ -5657,7 +5740,7 @@
         <v>1</v>
       </c>
       <c r="E60" s="95">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F60" s="4">
@@ -7123,8 +7206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7975518-D56C-48E6-B20B-FB32CB5C6D50}">
   <dimension ref="A1:AT287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="G223" sqref="G223"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="Q144" sqref="Q144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -8506,22 +8589,24 @@
         <v>180</v>
       </c>
       <c r="I45" s="70">
+        <v>2.5</v>
+      </c>
+      <c r="J45" s="70">
         <v>2</v>
       </c>
-      <c r="J45" s="70">
-        <v>1</v>
-      </c>
       <c r="K45" s="70">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="L45" s="70">
+        <f>I45</f>
+        <v>2.5</v>
+      </c>
+      <c r="M45" s="70">
+        <f>J45</f>
         <v>2</v>
       </c>
-      <c r="M45" s="70">
-        <v>1</v>
-      </c>
       <c r="N45" s="70">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="O45" s="71"/>
       <c r="P45" s="71"/>
@@ -8548,22 +8633,26 @@
         <v>181</v>
       </c>
       <c r="I46" s="70">
+        <f>I45</f>
+        <v>2.5</v>
+      </c>
+      <c r="J46" s="70">
+        <f>J45</f>
         <v>2</v>
       </c>
-      <c r="J46" s="70">
-        <v>1</v>
-      </c>
       <c r="K46" s="70">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="L46" s="70">
+        <f t="shared" ref="L46:L48" si="0">I46</f>
+        <v>2.5</v>
+      </c>
+      <c r="M46" s="70">
+        <f t="shared" ref="M46:M48" si="1">J46</f>
         <v>2</v>
       </c>
-      <c r="M46" s="70">
-        <v>1</v>
-      </c>
       <c r="N46" s="70">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
       <c r="O46" s="71"/>
       <c r="P46" s="71"/>
@@ -8590,22 +8679,26 @@
         <v>182</v>
       </c>
       <c r="I47" s="70">
+        <f t="shared" ref="I47:I48" si="2">I46</f>
+        <v>2.5</v>
+      </c>
+      <c r="J47" s="70">
+        <f t="shared" ref="J47:J48" si="3">J46</f>
         <v>2</v>
       </c>
-      <c r="J47" s="70">
-        <v>1</v>
-      </c>
       <c r="K47" s="70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47" s="70">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="M47" s="70">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M47" s="70">
-        <v>1</v>
-      </c>
       <c r="N47" s="70">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="O47" s="71"/>
       <c r="P47" s="71"/>
@@ -8632,22 +8725,26 @@
         <v>183</v>
       </c>
       <c r="I48" s="70">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="J48" s="70">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="J48" s="70">
-        <v>1</v>
-      </c>
       <c r="K48" s="70">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="L48" s="70">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="M48" s="70">
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M48" s="70">
-        <v>1</v>
-      </c>
       <c r="N48" s="70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O48" s="71"/>
       <c r="P48" s="71"/>
@@ -8980,15 +9077,15 @@
         <v>100</v>
       </c>
       <c r="J58" s="89">
-        <f t="shared" ref="J58:L58" si="0">J54</f>
+        <f t="shared" ref="J58:L58" si="4">J54</f>
         <v>100</v>
       </c>
       <c r="K58" s="89">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L58" s="89">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="M58" s="72"/>
@@ -9022,15 +9119,15 @@
         <v>100</v>
       </c>
       <c r="J59" s="89">
-        <f t="shared" ref="J59:L59" si="1">J56</f>
+        <f t="shared" ref="J59:L59" si="5">J56</f>
         <v>100</v>
       </c>
       <c r="K59" s="89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="L59" s="89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M59" s="72"/>
@@ -9064,15 +9161,15 @@
         <v>100</v>
       </c>
       <c r="J60" s="89">
-        <f t="shared" ref="J60:L60" si="2">J54</f>
+        <f t="shared" ref="J60:L60" si="6">J54</f>
         <v>100</v>
       </c>
       <c r="K60" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="L60" s="89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="M60" s="72"/>
@@ -9166,15 +9263,15 @@
         <v>100</v>
       </c>
       <c r="J63" s="89">
-        <f t="shared" ref="J63:L63" si="3">J56</f>
+        <f t="shared" ref="J63:L63" si="7">J56</f>
         <v>100</v>
       </c>
       <c r="K63" s="89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>100</v>
       </c>
       <c r="L63" s="89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M63" s="72"/>
@@ -9208,15 +9305,15 @@
         <v>100</v>
       </c>
       <c r="J64" s="89">
-        <f t="shared" ref="J64:L64" si="4">J54</f>
+        <f t="shared" ref="J64:L64" si="8">J54</f>
         <v>100</v>
       </c>
       <c r="K64" s="89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L64" s="89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>100</v>
       </c>
       <c r="M64" s="72"/>
@@ -9250,15 +9347,15 @@
         <v>100</v>
       </c>
       <c r="J65" s="89">
-        <f t="shared" ref="J65:L65" si="5">J54</f>
+        <f t="shared" ref="J65:L65" si="9">J54</f>
         <v>100</v>
       </c>
       <c r="K65" s="89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L65" s="89">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="M65" s="72"/>
@@ -9292,15 +9389,15 @@
         <v>100</v>
       </c>
       <c r="J66" s="89">
-        <f t="shared" ref="J66:L66" si="6">J55</f>
+        <f t="shared" ref="J66:L66" si="10">J55</f>
         <v>100</v>
       </c>
       <c r="K66" s="89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="L66" s="89">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="M66" s="72"/>
@@ -9364,15 +9461,15 @@
         <v>100</v>
       </c>
       <c r="J68" s="89">
-        <f t="shared" ref="J68:L68" si="7">J54</f>
+        <f t="shared" ref="J68:L68" si="11">J54</f>
         <v>100</v>
       </c>
       <c r="K68" s="89">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L68" s="89">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>100</v>
       </c>
       <c r="M68" s="72"/>
@@ -9406,15 +9503,15 @@
         <v>100</v>
       </c>
       <c r="J69" s="89">
-        <f t="shared" ref="J69:L69" si="8">J55</f>
+        <f t="shared" ref="J69:L69" si="12">J55</f>
         <v>100</v>
       </c>
       <c r="K69" s="89">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>100</v>
       </c>
       <c r="L69" s="89">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="M69" s="72"/>
@@ -10093,15 +10190,15 @@
         <v>0.7</v>
       </c>
       <c r="J90" s="97">
-        <f t="shared" ref="J90:L90" si="9">J86</f>
+        <f t="shared" ref="J90:L90" si="13">J86</f>
         <v>1E-3</v>
       </c>
       <c r="K90" s="92">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0.7</v>
       </c>
       <c r="L90" s="97">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
       <c r="M90" s="71"/>
@@ -10135,15 +10232,15 @@
         <v>0.7</v>
       </c>
       <c r="J91" s="97">
-        <f t="shared" ref="J91:L91" si="10">J88</f>
+        <f t="shared" ref="J91:L91" si="14">J88</f>
         <v>1E-3</v>
       </c>
       <c r="K91" s="92">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0.7</v>
       </c>
       <c r="L91" s="97">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>1E-3</v>
       </c>
       <c r="M91" s="71"/>
@@ -10177,15 +10274,15 @@
         <v>0.7</v>
       </c>
       <c r="J92" s="97">
-        <f t="shared" ref="J92:L92" si="11">J86</f>
+        <f t="shared" ref="J92:L92" si="15">J86</f>
         <v>1E-3</v>
       </c>
       <c r="K92" s="92">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0.7</v>
       </c>
       <c r="L92" s="97">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>1E-3</v>
       </c>
       <c r="M92" s="71"/>
@@ -10215,19 +10312,19 @@
         <v>96</v>
       </c>
       <c r="I93" s="92">
-        <f t="shared" ref="I93:L93" si="12">I87</f>
+        <f t="shared" ref="I93:L93" si="16">I87</f>
         <v>0.7</v>
       </c>
       <c r="J93" s="97">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1E-3</v>
       </c>
       <c r="K93" s="92">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>0.7</v>
       </c>
       <c r="L93" s="97">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>1E-3</v>
       </c>
       <c r="M93" s="71"/>
@@ -10257,19 +10354,19 @@
         <v>97</v>
       </c>
       <c r="I94" s="92">
-        <f t="shared" ref="I94:L94" si="13">I88</f>
+        <f>I88</f>
         <v>0.7</v>
       </c>
       <c r="J94" s="97">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="I94:L94" si="17">J88</f>
         <v>1E-3</v>
       </c>
       <c r="K94" s="92">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0.7</v>
       </c>
       <c r="L94" s="97">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1E-3</v>
       </c>
       <c r="M94" s="71"/>
@@ -10299,19 +10396,19 @@
         <v>7</v>
       </c>
       <c r="I95" s="92">
-        <f t="shared" ref="I95:L95" si="14">I89</f>
+        <f t="shared" ref="I95:L95" si="18">I89</f>
         <v>0.7</v>
       </c>
       <c r="J95" s="97">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1E-3</v>
       </c>
       <c r="K95" s="92">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0.7</v>
       </c>
       <c r="L95" s="97">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1E-3</v>
       </c>
       <c r="M95" s="71"/>
@@ -10341,19 +10438,19 @@
         <v>6</v>
       </c>
       <c r="I96" s="92">
-        <f t="shared" ref="I96:L96" si="15">I90</f>
+        <f t="shared" ref="I96:L96" si="19">I90</f>
         <v>0.7</v>
       </c>
       <c r="J96" s="97">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>1E-3</v>
       </c>
       <c r="K96" s="92">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>0.7</v>
       </c>
       <c r="L96" s="97">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>1E-3</v>
       </c>
       <c r="M96" s="71"/>
@@ -10383,19 +10480,19 @@
         <v>120</v>
       </c>
       <c r="I97" s="92">
-        <f t="shared" ref="I97:L97" si="16">I91</f>
+        <f t="shared" ref="I97:L97" si="20">I91</f>
         <v>0.7</v>
       </c>
       <c r="J97" s="97">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>1E-3</v>
       </c>
       <c r="K97" s="92">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0.7</v>
       </c>
       <c r="L97" s="97">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>1E-3</v>
       </c>
       <c r="M97" s="71"/>
@@ -10425,19 +10522,19 @@
         <v>9</v>
       </c>
       <c r="I98" s="92">
-        <f t="shared" ref="I98:L98" si="17">I92</f>
+        <f t="shared" ref="I98:L98" si="21">I92</f>
         <v>0.7</v>
       </c>
       <c r="J98" s="97">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1E-3</v>
       </c>
       <c r="K98" s="92">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0.7</v>
       </c>
       <c r="L98" s="97">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1E-3</v>
       </c>
       <c r="M98" s="71"/>
@@ -10467,19 +10564,19 @@
         <v>98</v>
       </c>
       <c r="I99" s="92">
-        <f t="shared" ref="I99:L99" si="18">I93</f>
+        <f t="shared" ref="I99:L99" si="22">I93</f>
         <v>0.7</v>
       </c>
       <c r="J99" s="97">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1E-3</v>
       </c>
       <c r="K99" s="92">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0.7</v>
       </c>
       <c r="L99" s="97">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>1E-3</v>
       </c>
       <c r="M99" s="71"/>
@@ -10513,15 +10610,15 @@
         <v>0.7</v>
       </c>
       <c r="J100" s="97">
-        <f t="shared" ref="J100:L100" si="19">J86</f>
+        <f t="shared" ref="J100:L100" si="23">J86</f>
         <v>1E-3</v>
       </c>
       <c r="K100" s="92">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0.7</v>
       </c>
       <c r="L100" s="97">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>1E-3</v>
       </c>
       <c r="M100" s="71"/>
@@ -10555,15 +10652,15 @@
         <v>0.7</v>
       </c>
       <c r="J101" s="97">
-        <f t="shared" ref="J101:L101" si="20">J87</f>
+        <f t="shared" ref="J101:L101" si="24">J87</f>
         <v>1E-3</v>
       </c>
       <c r="K101" s="92">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0.7</v>
       </c>
       <c r="L101" s="97">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>1E-3</v>
       </c>
       <c r="M101" s="71"/>
@@ -11171,10 +11268,11 @@
         <v>226</v>
       </c>
       <c r="H119" s="86">
-        <v>5.0000000000000001E-3</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="I119" s="86">
-        <v>5.0000000000000001E-3</v>
+        <f>H119</f>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="K119" s="71" t="s">
         <v>192</v>
@@ -11230,10 +11328,12 @@
         <v>227</v>
       </c>
       <c r="H120" s="86">
-        <v>5.0000000000000001E-3</v>
+        <f>H119</f>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="I120" s="86">
-        <v>5.0000000000000001E-3</v>
+        <f>I119</f>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="K120" s="71" t="s">
         <v>193</v>
@@ -11383,10 +11483,10 @@
         <v>221</v>
       </c>
       <c r="L124" s="101">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="M124" s="101">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="P124" s="100"/>
       <c r="Q124" s="100"/>
@@ -11977,31 +12077,31 @@
         <v>239</v>
       </c>
       <c r="I142" s="70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J142" s="70">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K142" s="70">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="L142" s="70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M142" s="70">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="N142" s="70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O142" s="70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P142" s="70">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="Q142" s="70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R142" s="71"/>
       <c r="S142" s="71"/>
@@ -12025,31 +12125,31 @@
         <v>241</v>
       </c>
       <c r="I143" s="70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J143" s="70">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K143" s="70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L143" s="70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M143" s="70">
-        <v>1</v>
-      </c>
-      <c r="N143" s="70">
-        <v>0.25</v>
+        <v>1.5</v>
+      </c>
+      <c r="N143" s="83">
+        <v>0.4</v>
       </c>
       <c r="O143" s="70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P143" s="70">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="Q143" s="70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R143" s="71"/>
       <c r="S143" s="71"/>
@@ -12073,31 +12173,31 @@
         <v>240</v>
       </c>
       <c r="I144" s="70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J144" s="70">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="K144" s="70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L144" s="70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M144" s="70">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="N144" s="70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O144" s="70">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P144" s="70">
-        <v>1</v>
-      </c>
-      <c r="Q144" s="70">
-        <v>0.5</v>
+        <v>1.5</v>
+      </c>
+      <c r="Q144" s="83">
+        <v>0.4</v>
       </c>
       <c r="R144" s="71"/>
       <c r="S144" s="71"/>
@@ -12417,11 +12517,11 @@
         <v>100</v>
       </c>
       <c r="J154" s="89">
-        <f t="shared" ref="J154:K154" si="21">J150</f>
+        <f t="shared" ref="J154:K154" si="25">J150</f>
         <v>100</v>
       </c>
       <c r="K154" s="89">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>100</v>
       </c>
       <c r="L154" s="77"/>
@@ -12456,11 +12556,11 @@
         <v>100</v>
       </c>
       <c r="J155" s="89">
-        <f t="shared" ref="J155:K155" si="22">J152</f>
+        <f t="shared" ref="J155:K155" si="26">J152</f>
         <v>100</v>
       </c>
       <c r="K155" s="89">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>100</v>
       </c>
       <c r="L155" s="77"/>
@@ -12495,11 +12595,11 @@
         <v>100</v>
       </c>
       <c r="J156" s="89">
-        <f t="shared" ref="J156:K156" si="23">J150</f>
+        <f t="shared" ref="J156:K156" si="27">J150</f>
         <v>100</v>
       </c>
       <c r="K156" s="89">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>100</v>
       </c>
       <c r="L156" s="77"/>
@@ -12594,11 +12694,11 @@
         <v>100</v>
       </c>
       <c r="J159" s="89">
-        <f t="shared" ref="J159:K159" si="24">J152</f>
+        <f t="shared" ref="J159:K159" si="28">J152</f>
         <v>100</v>
       </c>
       <c r="K159" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>100</v>
       </c>
       <c r="L159" s="77"/>
@@ -12633,11 +12733,11 @@
         <v>100</v>
       </c>
       <c r="J160" s="89">
-        <f t="shared" ref="J160:K160" si="25">J150</f>
+        <f t="shared" ref="J160:K160" si="29">J150</f>
         <v>100</v>
       </c>
       <c r="K160" s="89">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>100</v>
       </c>
       <c r="L160" s="77"/>
@@ -12672,11 +12772,11 @@
         <v>100</v>
       </c>
       <c r="J161" s="89">
-        <f t="shared" ref="J161:K161" si="26">J150</f>
+        <f t="shared" ref="J161:K161" si="30">J150</f>
         <v>100</v>
       </c>
       <c r="K161" s="89">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>100</v>
       </c>
       <c r="L161" s="77"/>
@@ -12711,11 +12811,11 @@
         <v>100</v>
       </c>
       <c r="J162" s="89">
-        <f t="shared" ref="J162:K162" si="27">J151</f>
+        <f t="shared" ref="J162:K162" si="31">J151</f>
         <v>100</v>
       </c>
       <c r="K162" s="89">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>100</v>
       </c>
       <c r="L162" s="77"/>
@@ -12780,11 +12880,11 @@
         <v>100</v>
       </c>
       <c r="J164" s="89">
-        <f t="shared" ref="J164:K164" si="28">J150</f>
+        <f t="shared" ref="J164:K164" si="32">J150</f>
         <v>100</v>
       </c>
       <c r="K164" s="89">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>100</v>
       </c>
       <c r="L164" s="77"/>
@@ -12819,11 +12919,11 @@
         <v>100</v>
       </c>
       <c r="J165" s="89">
-        <f t="shared" ref="J165:K165" si="29">J151</f>
+        <f t="shared" ref="J165:K165" si="33">J151</f>
         <v>100</v>
       </c>
       <c r="K165" s="89">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>100</v>
       </c>
       <c r="L165" s="77"/>
@@ -13526,24 +13626,24 @@
         <f>I182</f>
         <v>0.7</v>
       </c>
-      <c r="J186" s="97">
-        <f t="shared" ref="J186:L186" si="30">J182</f>
+      <c r="J186" s="92">
+        <f t="shared" ref="J186:N186" si="34">J182</f>
         <v>0.3</v>
       </c>
       <c r="K186" s="92">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="L186" s="97">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="L186" s="92">
+        <f t="shared" si="34"/>
         <v>0.3</v>
       </c>
       <c r="M186" s="92">
-        <f t="shared" ref="M186:N186" si="31">M182</f>
-        <v>0</v>
-      </c>
-      <c r="N186" s="97">
-        <f t="shared" si="31"/>
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="N186" s="92">
+        <f t="shared" si="34"/>
         <v>0.3</v>
       </c>
       <c r="O186" s="71"/>
@@ -13574,24 +13674,24 @@
         <f>I184</f>
         <v>0</v>
       </c>
-      <c r="J187" s="97">
-        <f t="shared" ref="J187:L187" si="32">J184</f>
+      <c r="J187" s="92">
+        <f t="shared" ref="J187:N187" si="35">J184</f>
         <v>0.3</v>
       </c>
       <c r="K187" s="92">
-        <f t="shared" si="32"/>
-        <v>0</v>
-      </c>
-      <c r="L187" s="97">
-        <f t="shared" si="32"/>
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="L187" s="92">
+        <f t="shared" si="35"/>
         <v>0.3</v>
       </c>
       <c r="M187" s="92">
-        <f t="shared" ref="M187:N187" si="33">M184</f>
+        <f t="shared" si="35"/>
         <v>0.7</v>
       </c>
-      <c r="N187" s="97">
-        <f t="shared" si="33"/>
+      <c r="N187" s="92">
+        <f t="shared" si="35"/>
         <v>0.3</v>
       </c>
       <c r="O187" s="71"/>
@@ -13622,24 +13722,24 @@
         <f>I182</f>
         <v>0.7</v>
       </c>
-      <c r="J188" s="97">
-        <f t="shared" ref="J188:L188" si="34">J182</f>
+      <c r="J188" s="92">
+        <f t="shared" ref="J188:N188" si="36">J182</f>
         <v>0.3</v>
       </c>
       <c r="K188" s="92">
-        <f t="shared" si="34"/>
-        <v>0</v>
-      </c>
-      <c r="L188" s="97">
-        <f t="shared" si="34"/>
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="L188" s="92">
+        <f t="shared" si="36"/>
         <v>0.3</v>
       </c>
       <c r="M188" s="92">
-        <f t="shared" ref="M188:N188" si="35">M182</f>
-        <v>0</v>
-      </c>
-      <c r="N188" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="N188" s="92">
+        <f t="shared" si="36"/>
         <v>0.3</v>
       </c>
       <c r="O188" s="71"/>
@@ -13667,26 +13767,26 @@
         <v>96</v>
       </c>
       <c r="I189" s="92">
-        <f t="shared" ref="I189:N189" si="36">I183</f>
-        <v>0</v>
-      </c>
-      <c r="J189" s="97">
-        <f t="shared" si="36"/>
+        <f>I184</f>
+        <v>0</v>
+      </c>
+      <c r="J189" s="92">
+        <f t="shared" ref="J189:N189" si="37">J184</f>
         <v>0.3</v>
       </c>
       <c r="K189" s="92">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="L189" s="92">
+        <f t="shared" si="37"/>
+        <v>0.3</v>
+      </c>
+      <c r="M189" s="92">
+        <f t="shared" si="37"/>
         <v>0.7</v>
       </c>
-      <c r="L189" s="97">
-        <f t="shared" si="36"/>
-        <v>0.3</v>
-      </c>
-      <c r="M189" s="92">
-        <f t="shared" ref="M189:N189" si="37">M183</f>
-        <v>0</v>
-      </c>
-      <c r="N189" s="97">
+      <c r="N189" s="92">
         <f t="shared" si="37"/>
         <v>0.3</v>
       </c>
@@ -13715,27 +13815,27 @@
         <v>97</v>
       </c>
       <c r="I190" s="92">
-        <f t="shared" ref="I190:N190" si="38">I184</f>
-        <v>0</v>
-      </c>
-      <c r="J190" s="97">
+        <f>I184</f>
+        <v>0</v>
+      </c>
+      <c r="J190" s="92">
+        <f t="shared" ref="J190:N190" si="38">J184</f>
+        <v>0.3</v>
+      </c>
+      <c r="K190" s="92">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="L190" s="92">
         <f t="shared" si="38"/>
         <v>0.3</v>
       </c>
-      <c r="K190" s="92">
+      <c r="M190" s="92">
         <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
-      <c r="L190" s="97">
+        <v>0.7</v>
+      </c>
+      <c r="N190" s="92">
         <f t="shared" si="38"/>
-        <v>0.3</v>
-      </c>
-      <c r="M190" s="92">
-        <f t="shared" ref="M190:N190" si="39">M184</f>
-        <v>0.7</v>
-      </c>
-      <c r="N190" s="97">
-        <f t="shared" si="39"/>
         <v>0.3</v>
       </c>
       <c r="O190" s="71"/>
@@ -13763,27 +13863,27 @@
         <v>7</v>
       </c>
       <c r="I191" s="92">
-        <f t="shared" ref="I191:N191" si="40">I185</f>
-        <v>0</v>
-      </c>
-      <c r="J191" s="97">
-        <f t="shared" si="40"/>
+        <f>I184</f>
+        <v>0</v>
+      </c>
+      <c r="J191" s="92">
+        <f t="shared" ref="J191:N191" si="39">J184</f>
         <v>0.3</v>
       </c>
       <c r="K191" s="92">
-        <f t="shared" si="40"/>
-        <v>0</v>
-      </c>
-      <c r="L191" s="97">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="L191" s="92">
+        <f t="shared" si="39"/>
         <v>0.3</v>
       </c>
       <c r="M191" s="92">
-        <f t="shared" ref="M191:N191" si="41">M185</f>
-        <v>0</v>
-      </c>
-      <c r="N191" s="97">
-        <f t="shared" si="41"/>
+        <f t="shared" si="39"/>
+        <v>0.7</v>
+      </c>
+      <c r="N191" s="92">
+        <f t="shared" si="39"/>
         <v>0.3</v>
       </c>
       <c r="O191" s="71"/>
@@ -13811,27 +13911,27 @@
         <v>6</v>
       </c>
       <c r="I192" s="92">
-        <f t="shared" ref="I192:N192" si="42">I186</f>
+        <f>I182</f>
         <v>0.7</v>
       </c>
-      <c r="J192" s="97">
-        <f t="shared" si="42"/>
+      <c r="J192" s="92">
+        <f t="shared" ref="J192:N192" si="40">J182</f>
         <v>0.3</v>
       </c>
       <c r="K192" s="92">
-        <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="L192" s="97">
-        <f t="shared" si="42"/>
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="L192" s="92">
+        <f t="shared" si="40"/>
         <v>0.3</v>
       </c>
       <c r="M192" s="92">
-        <f t="shared" ref="M192:N192" si="43">M186</f>
-        <v>0</v>
-      </c>
-      <c r="N192" s="97">
-        <f t="shared" si="43"/>
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="N192" s="92">
+        <f t="shared" si="40"/>
         <v>0.3</v>
       </c>
       <c r="O192" s="71"/>
@@ -13859,27 +13959,27 @@
         <v>120</v>
       </c>
       <c r="I193" s="92">
-        <f t="shared" ref="I193:N193" si="44">I187</f>
-        <v>0</v>
-      </c>
-      <c r="J193" s="97">
-        <f t="shared" si="44"/>
+        <f>I182</f>
+        <v>0.7</v>
+      </c>
+      <c r="J193" s="92">
+        <f t="shared" ref="J193:N193" si="41">J182</f>
         <v>0.3</v>
       </c>
       <c r="K193" s="92">
-        <f t="shared" si="44"/>
-        <v>0</v>
-      </c>
-      <c r="L193" s="97">
-        <f t="shared" si="44"/>
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="L193" s="92">
+        <f t="shared" si="41"/>
         <v>0.3</v>
       </c>
       <c r="M193" s="92">
-        <f t="shared" ref="M193:N193" si="45">M187</f>
-        <v>0.7</v>
-      </c>
-      <c r="N193" s="97">
-        <f t="shared" si="45"/>
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="N193" s="92">
+        <f t="shared" si="41"/>
         <v>0.3</v>
       </c>
       <c r="O193" s="71"/>
@@ -13907,27 +14007,27 @@
         <v>9</v>
       </c>
       <c r="I194" s="92">
-        <f t="shared" ref="I194:N194" si="46">I188</f>
+        <f>I183</f>
+        <v>0</v>
+      </c>
+      <c r="J194" s="92">
+        <f t="shared" ref="J194:N194" si="42">J183</f>
+        <v>0.3</v>
+      </c>
+      <c r="K194" s="92">
+        <f t="shared" si="42"/>
         <v>0.7</v>
       </c>
-      <c r="J194" s="97">
-        <f t="shared" si="46"/>
+      <c r="L194" s="92">
+        <f t="shared" si="42"/>
         <v>0.3</v>
       </c>
-      <c r="K194" s="92">
-        <f t="shared" si="46"/>
-        <v>0</v>
-      </c>
-      <c r="L194" s="97">
-        <f t="shared" si="46"/>
-        <v>0.3</v>
-      </c>
       <c r="M194" s="92">
-        <f t="shared" ref="M194:N194" si="47">M188</f>
-        <v>0</v>
-      </c>
-      <c r="N194" s="97">
-        <f t="shared" si="47"/>
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="N194" s="92">
+        <f t="shared" si="42"/>
         <v>0.3</v>
       </c>
       <c r="O194" s="71"/>
@@ -13955,27 +14055,27 @@
         <v>98</v>
       </c>
       <c r="I195" s="92">
-        <f t="shared" ref="I195:N195" si="48">I189</f>
-        <v>0</v>
-      </c>
-      <c r="J195" s="97">
-        <f t="shared" si="48"/>
+        <f>I184</f>
+        <v>0</v>
+      </c>
+      <c r="J195" s="92">
+        <f t="shared" ref="J195:N195" si="43">J184</f>
         <v>0.3</v>
       </c>
       <c r="K195" s="92">
-        <f t="shared" si="48"/>
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="L195" s="92">
+        <f t="shared" si="43"/>
+        <v>0.3</v>
+      </c>
+      <c r="M195" s="92">
+        <f t="shared" si="43"/>
         <v>0.7</v>
       </c>
-      <c r="L195" s="97">
-        <f t="shared" si="48"/>
-        <v>0.3</v>
-      </c>
-      <c r="M195" s="92">
-        <f t="shared" ref="M195:N195" si="49">M189</f>
-        <v>0</v>
-      </c>
-      <c r="N195" s="97">
-        <f t="shared" si="49"/>
+      <c r="N195" s="92">
+        <f t="shared" si="43"/>
         <v>0.3</v>
       </c>
       <c r="O195" s="71"/>
@@ -14006,24 +14106,24 @@
         <f>I182</f>
         <v>0.7</v>
       </c>
-      <c r="J196" s="97">
-        <f t="shared" ref="J196:L196" si="50">J182</f>
+      <c r="J196" s="92">
+        <f t="shared" ref="J196:N196" si="44">J182</f>
         <v>0.3</v>
       </c>
       <c r="K196" s="92">
-        <f t="shared" si="50"/>
-        <v>0</v>
-      </c>
-      <c r="L196" s="97">
-        <f t="shared" si="50"/>
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="L196" s="92">
+        <f t="shared" si="44"/>
         <v>0.3</v>
       </c>
       <c r="M196" s="92">
-        <f t="shared" ref="M196:N196" si="51">M182</f>
-        <v>0</v>
-      </c>
-      <c r="N196" s="97">
-        <f t="shared" si="51"/>
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="N196" s="92">
+        <f t="shared" si="44"/>
         <v>0.3</v>
       </c>
       <c r="O196" s="71"/>
@@ -14054,24 +14154,24 @@
         <f>I183</f>
         <v>0</v>
       </c>
-      <c r="J197" s="97">
-        <f t="shared" ref="J197:N197" si="52">J183</f>
+      <c r="J197" s="92">
+        <f t="shared" ref="J197:N197" si="45">J183</f>
         <v>0.3</v>
       </c>
       <c r="K197" s="92">
-        <f t="shared" si="52"/>
+        <f t="shared" si="45"/>
         <v>0.7</v>
       </c>
-      <c r="L197" s="97">
-        <f t="shared" si="52"/>
+      <c r="L197" s="92">
+        <f t="shared" si="45"/>
         <v>0.3</v>
       </c>
       <c r="M197" s="92">
-        <f t="shared" ref="M197:N197" si="53">M183</f>
-        <v>0</v>
-      </c>
-      <c r="N197" s="97">
-        <f t="shared" si="53"/>
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="N197" s="92">
+        <f t="shared" si="45"/>
         <v>0.3</v>
       </c>
       <c r="O197" s="71"/>
@@ -15063,7 +15163,7 @@
       <c r="E226" s="58"/>
       <c r="F226" s="72"/>
       <c r="G226" s="49" t="str">
-        <f t="shared" ref="G226:G229" si="54">G217</f>
+        <f t="shared" ref="G226:G229" si="46">G217</f>
         <v>N</v>
       </c>
       <c r="H226" s="104">
@@ -15100,7 +15200,7 @@
       <c r="E227" s="58"/>
       <c r="F227" s="72"/>
       <c r="G227" s="49" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="46"/>
         <v>P</v>
       </c>
       <c r="H227" s="104">
@@ -15137,7 +15237,7 @@
       <c r="E228" s="58"/>
       <c r="F228" s="72"/>
       <c r="G228" s="49" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="46"/>
         <v>PAS</v>
       </c>
       <c r="H228" s="104">
@@ -15174,7 +15274,7 @@
       <c r="E229" s="58"/>
       <c r="F229" s="72"/>
       <c r="G229" s="49" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="46"/>
         <v>Ys</v>
       </c>
       <c r="H229" s="104">
@@ -16357,7 +16457,7 @@
         <v>0</v>
       </c>
       <c r="K266" s="90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L266" s="90">
         <v>0</v>
@@ -16489,7 +16589,7 @@
         <v>0</v>
       </c>
       <c r="K269" s="90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L269" s="90">
         <v>0</v>
@@ -16577,7 +16677,7 @@
         <v>0</v>
       </c>
       <c r="K271" s="90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L271" s="90">
         <v>0</v>
@@ -16665,7 +16765,7 @@
         <v>0</v>
       </c>
       <c r="K273" s="90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L273" s="90">
         <v>0</v>
@@ -16753,7 +16853,7 @@
         <v>0</v>
       </c>
       <c r="K275" s="90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L275" s="90">
         <v>0</v>
@@ -16841,7 +16941,7 @@
         <v>0</v>
       </c>
       <c r="K277" s="90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L277" s="90">
         <v>0</v>
@@ -16885,7 +16985,7 @@
         <v>0</v>
       </c>
       <c r="K278" s="90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L278" s="90">
         <v>0</v>
@@ -16929,7 +17029,7 @@
         <v>0</v>
       </c>
       <c r="K279" s="90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L279" s="90">
         <v>0</v>
@@ -16973,7 +17073,7 @@
         <v>0</v>
       </c>
       <c r="K280" s="90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L280" s="90">
         <v>0</v>
@@ -17017,7 +17117,7 @@
         <v>0</v>
       </c>
       <c r="K281" s="90">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L281" s="90">
         <v>0</v>

</xml_diff>

<commit_message>
added nutrient to crop.py
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DDE923-2B44-4DF7-8FD4-0EA91C44DDD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFB1172-C34D-4277-829F-2D5FCCCB1F52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -43,12 +43,14 @@
     <definedName name="diesel" localSheetId="0">Price!$B$3</definedName>
     <definedName name="diesel_rebate" localSheetId="0">Price!$B$5</definedName>
     <definedName name="draft_seeding" localSheetId="6">'Mach 1'!$B$35</definedName>
+    <definedName name="drymatter_grazed">'Crop Sim'!$S$313:$S$341</definedName>
     <definedName name="equip_insurance">Finance!$B$11</definedName>
     <definedName name="fert_bnds" localSheetId="4">'Crop Sim'!$O$247:$S$263</definedName>
     <definedName name="fert_cartage_cost" localSheetId="0">Price!$B$63</definedName>
     <definedName name="fert_control_params" localSheetId="4">'Crop Sim'!$H$247:$I$251</definedName>
     <definedName name="fert_cost" localSheetId="0">Price!$A$65:$B$69</definedName>
     <definedName name="fixed_dep" localSheetId="1">Finance!$B$8</definedName>
+    <definedName name="fixing_probability">'Crop Sim'!$O$358:$P$374</definedName>
     <definedName name="flagfall" localSheetId="0">Price!$B$34</definedName>
     <definedName name="fuel_adj_tractor" localSheetId="6">'Mach 1'!$B$37</definedName>
     <definedName name="fungi_control_bnds">'Crop Sim'!$H$150:$K$166</definedName>
@@ -77,6 +79,9 @@
     <definedName name="max_yield_gen">'Crop Sim'!$H$11:$I$15</definedName>
     <definedName name="max_yield_spec">'Crop Sim'!$K$11:$L$23</definedName>
     <definedName name="minroe">Finance!$B$17</definedName>
+    <definedName name="nitrogen_removed_grazing">'Crop Sim'!$N$313:$N$341</definedName>
+    <definedName name="nitrogen_removed_harvest">'Crop Sim'!$I$313:$I$341</definedName>
+    <definedName name="nutrient_leach">'Crop Sim'!$L$307</definedName>
     <definedName name="nutrient_yield_params">'Crop Sim'!$H$279:$J$295</definedName>
     <definedName name="oil_grease_factor_harv" localSheetId="6">'Mach 1'!$B$63</definedName>
     <definedName name="oil_grease_factor_tractor" localSheetId="6">'Mach 1'!$B$24</definedName>
@@ -105,7 +110,6 @@
     <definedName name="seeds_soften">'Crop Sim'!$O$119:$Q$120</definedName>
     <definedName name="seedset_min">'Crop Sim'!$L$125:$M$125</definedName>
     <definedName name="seedset_slope">'Crop Sim'!$L$123:$M$123</definedName>
-    <definedName name="Soil_nitrate_assimtope" localSheetId="4">'Crop Sim'!$S$389:$S$417</definedName>
     <definedName name="Soil_nitrate_slope">'Crop Sim'!$N$389:$N$417</definedName>
     <definedName name="sprayer_eff" localSheetId="6">'Mach 1'!$B$96</definedName>
     <definedName name="sprayer_fuel_consumption" localSheetId="6">'Mach 1'!$B$98</definedName>
@@ -1633,7 +1637,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-max proportion of yield</t>
+Sensitivity on proportion of yield lost. Ie yeild proportion lost at 0 nitrogen. 
+For pulses this is set to 0 ie because nitrogen doesn't effect pulse yield</t>
         </r>
       </text>
     </comment>
@@ -1706,6 +1711,30 @@
           </rPr>
           <t xml:space="preserve">
 Nitrogen level has no impact on pulse yield</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I312" authorId="0" shapeId="0" xr:uid="{09C5BB96-5D6C-4DFC-BBA0-CC93F6147E5B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+kg of N removed per kg harvested</t>
         </r>
       </text>
     </comment>
@@ -1874,7 +1903,31 @@
           </rPr>
           <t xml:space="preserve">
 this is inputted in the stubble section but I need it for all landuse types (including capitals) so I have done it again here
-Only includes crops that fix nitrogen</t>
+Includes all crops - the fixing section below accounts for N fixing of different crops.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P358" authorId="0" shapeId="0" xr:uid="{22B83CFA-B542-4817-A32E-C21F2B8E268B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+not sure this is needed if using the biomass slope below</t>
         </r>
       </text>
     </comment>
@@ -3043,7 +3096,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="255">
   <si>
     <t>Machinery</t>
   </si>
@@ -3804,7 +3857,10 @@
     <t>Soil nitrate slope</t>
   </si>
   <si>
-    <t>Soil nitrate assimtope</t>
+    <t>Fix N</t>
+  </si>
+  <si>
+    <t>leach</t>
   </si>
 </sst>
 </file>
@@ -4095,7 +4151,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4343,6 +4399,7 @@
     <xf numFmtId="2" fontId="5" fillId="8" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Formula 1" xfId="2" xr:uid="{73E7623B-26A4-407F-9297-1EB699330B2D}"/>
@@ -5325,7 +5382,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
       <selection activeCell="A65" sqref="A65:B69"/>
     </sheetView>
   </sheetViews>
@@ -6121,34 +6178,34 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B66" s="4">
-        <v>440</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B67" s="4">
-        <v>339</v>
+        <v>541</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" s="4">
-        <v>541</v>
+        <v>339</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B69" s="4">
-        <v>15</v>
+        <v>440</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -6174,7 +6231,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B74" s="4">
         <v>30</v>
@@ -6182,7 +6239,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B75" s="4">
         <v>30</v>
@@ -7531,8 +7588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7975518-D56C-48E6-B20B-FB32CB5C6D50}">
   <dimension ref="A1:AT423"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
-      <selection activeCell="S389" sqref="S389:S417"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="L292" sqref="L292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -17362,10 +17419,10 @@
         <v>177</v>
       </c>
       <c r="I282" s="81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J282" s="84">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K282" s="70"/>
       <c r="L282" s="70"/>
@@ -17429,7 +17486,8 @@
       <c r="H284" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="I284" s="81">
+      <c r="I284" s="94">
+        <f>I280</f>
         <v>1</v>
       </c>
       <c r="J284" s="94">
@@ -17464,12 +17522,13 @@
       <c r="H285" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="I285" s="81">
-        <v>1</v>
+      <c r="I285" s="94">
+        <f>I282</f>
+        <v>0</v>
       </c>
       <c r="J285" s="94">
         <f>J282</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K285" s="70"/>
       <c r="L285" s="70"/>
@@ -17499,11 +17558,12 @@
       <c r="H286" s="89" t="s">
         <v>95</v>
       </c>
-      <c r="I286" s="81">
+      <c r="I286" s="94">
+        <f t="shared" ref="I286:J286" si="58">I280</f>
         <v>1</v>
       </c>
       <c r="J286" s="94">
-        <f t="shared" ref="J286" si="58">J280</f>
+        <f t="shared" si="58"/>
         <v>0.03</v>
       </c>
       <c r="K286" s="70"/>
@@ -17534,12 +17594,13 @@
       <c r="H287" s="89" t="s">
         <v>96</v>
       </c>
-      <c r="I287" s="81">
-        <v>1</v>
+      <c r="I287" s="94">
+        <f>I282</f>
+        <v>0</v>
       </c>
       <c r="J287" s="94">
         <f>J282</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K287" s="70"/>
       <c r="L287" s="70"/>
@@ -17569,12 +17630,13 @@
       <c r="H288" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="I288" s="81">
-        <v>1</v>
+      <c r="I288" s="94">
+        <f t="shared" ref="I288:J288" si="59">I282</f>
+        <v>0</v>
       </c>
       <c r="J288" s="94">
-        <f t="shared" ref="J288" si="59">J282</f>
-        <v>100</v>
+        <f t="shared" si="59"/>
+        <v>0</v>
       </c>
       <c r="K288" s="70"/>
       <c r="L288" s="70"/>
@@ -17604,12 +17666,13 @@
       <c r="H289" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="I289" s="81">
-        <v>1</v>
+      <c r="I289" s="94">
+        <f>I282</f>
+        <v>0</v>
       </c>
       <c r="J289" s="94">
         <f>J282</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K289" s="70"/>
       <c r="L289" s="70"/>
@@ -17639,7 +17702,8 @@
       <c r="H290" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="I290" s="81">
+      <c r="I290" s="94">
+        <f>I280</f>
         <v>1</v>
       </c>
       <c r="J290" s="94">
@@ -17674,7 +17738,8 @@
       <c r="H291" s="89" t="s">
         <v>120</v>
       </c>
-      <c r="I291" s="81">
+      <c r="I291" s="94">
+        <f>I280</f>
         <v>1</v>
       </c>
       <c r="J291" s="94">
@@ -17709,7 +17774,8 @@
       <c r="H292" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="I292" s="81">
+      <c r="I292" s="94">
+        <f>I281</f>
         <v>1</v>
       </c>
       <c r="J292" s="94">
@@ -17744,12 +17810,13 @@
       <c r="H293" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="I293" s="81">
-        <v>1</v>
+      <c r="I293" s="94">
+        <f>I282</f>
+        <v>0</v>
       </c>
       <c r="J293" s="94">
         <f>J282</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K293" s="70"/>
       <c r="L293" s="70"/>
@@ -17779,7 +17846,8 @@
       <c r="H294" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="I294" s="81">
+      <c r="I294" s="94">
+        <f>I280</f>
         <v>1</v>
       </c>
       <c r="J294" s="94">
@@ -17814,11 +17882,12 @@
       <c r="H295" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="I295" s="81">
+      <c r="I295" s="94">
+        <f t="shared" ref="I295:J295" si="60">I281</f>
         <v>1</v>
       </c>
       <c r="J295" s="94">
-        <f t="shared" ref="J295" si="60">J281</f>
+        <f t="shared" si="60"/>
         <v>0.03</v>
       </c>
       <c r="K295" s="70"/>
@@ -18129,7 +18198,9 @@
       <c r="I305" s="54"/>
       <c r="J305" s="54"/>
       <c r="K305" s="54"/>
-      <c r="L305" s="54"/>
+      <c r="L305" s="55" t="s">
+        <v>254</v>
+      </c>
       <c r="M305" s="54"/>
       <c r="N305" s="54"/>
       <c r="O305" s="54"/>
@@ -18157,7 +18228,9 @@
       <c r="I306" s="54"/>
       <c r="J306" s="54"/>
       <c r="K306" s="54"/>
-      <c r="L306" s="54"/>
+      <c r="L306" s="54" t="s">
+        <v>223</v>
+      </c>
       <c r="M306" s="54"/>
       <c r="N306" s="54"/>
       <c r="O306" s="54"/>
@@ -18185,7 +18258,9 @@
       <c r="I307" s="54"/>
       <c r="J307" s="54"/>
       <c r="K307" s="54"/>
-      <c r="L307" s="54"/>
+      <c r="L307" s="109">
+        <v>0.05</v>
+      </c>
       <c r="M307" s="54"/>
       <c r="N307" s="54"/>
       <c r="O307" s="54"/>
@@ -18367,7 +18442,8 @@
         <v>176</v>
       </c>
       <c r="I313" s="88">
-        <v>0</v>
+        <f>AVERAGE(I317,I323,I327)</f>
+        <v>20</v>
       </c>
       <c r="J313" s="70"/>
       <c r="K313" s="70"/>
@@ -18376,7 +18452,8 @@
         <v>176</v>
       </c>
       <c r="N313" s="88">
-        <v>0</v>
+        <f>AVERAGE(N317,N323,N327)</f>
+        <v>17</v>
       </c>
       <c r="O313" s="70"/>
       <c r="P313" s="70"/>
@@ -18385,7 +18462,8 @@
         <v>176</v>
       </c>
       <c r="S313" s="88">
-        <v>0</v>
+        <f>AVERAGE(S317,S323,S327)</f>
+        <v>1</v>
       </c>
       <c r="T313" s="70"/>
       <c r="U313" s="70"/>
@@ -18407,7 +18485,8 @@
         <v>175</v>
       </c>
       <c r="I314" s="88">
-        <v>0</v>
+        <f>AVERAGE(I325,I328)</f>
+        <v>41</v>
       </c>
       <c r="J314" s="70"/>
       <c r="K314" s="70"/>
@@ -18416,7 +18495,8 @@
         <v>175</v>
       </c>
       <c r="N314" s="88">
-        <v>0</v>
+        <f>AVERAGE(N325,N328)</f>
+        <v>18</v>
       </c>
       <c r="O314" s="70"/>
       <c r="P314" s="70"/>
@@ -18425,7 +18505,8 @@
         <v>175</v>
       </c>
       <c r="S314" s="88">
-        <v>0</v>
+        <f>AVERAGE(S325,S328)</f>
+        <v>1</v>
       </c>
       <c r="T314" s="70"/>
       <c r="U314" s="70"/>
@@ -18447,7 +18528,8 @@
         <v>177</v>
       </c>
       <c r="I315" s="88">
-        <v>0</v>
+        <f>AVERAGE(I320:I322,I326,I318)</f>
+        <v>45.6</v>
       </c>
       <c r="J315" s="70"/>
       <c r="K315" s="70"/>
@@ -18456,7 +18538,8 @@
         <v>177</v>
       </c>
       <c r="N315" s="88">
-        <v>0</v>
+        <f>AVERAGE(N320:N322,N326,N318)</f>
+        <v>17</v>
       </c>
       <c r="O315" s="70"/>
       <c r="P315" s="70"/>
@@ -18465,7 +18548,8 @@
         <v>177</v>
       </c>
       <c r="S315" s="88">
-        <v>0</v>
+        <f>AVERAGE(S320:S322,S326,S318)</f>
+        <v>1</v>
       </c>
       <c r="T315" s="70"/>
       <c r="U315" s="70"/>
@@ -18487,7 +18571,8 @@
         <v>178</v>
       </c>
       <c r="I316" s="88">
-        <v>0</v>
+        <f>AVERAGE(I317:I328)</f>
+        <v>32.25</v>
       </c>
       <c r="J316" s="70"/>
       <c r="K316" s="70"/>
@@ -18496,7 +18581,8 @@
         <v>178</v>
       </c>
       <c r="N316" s="88">
-        <v>0</v>
+        <f>AVERAGE(N317:N328)</f>
+        <v>17.166666666666668</v>
       </c>
       <c r="O316" s="70"/>
       <c r="P316" s="70"/>
@@ -18505,7 +18591,8 @@
         <v>178</v>
       </c>
       <c r="S316" s="88">
-        <v>0</v>
+        <f>AVERAGE(S317:S328)</f>
+        <v>1.1666666666666667</v>
       </c>
       <c r="T316" s="70"/>
       <c r="U316" s="70"/>
@@ -18527,7 +18614,7 @@
         <v>4</v>
       </c>
       <c r="I317" s="88">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="J317" s="70"/>
       <c r="K317" s="70"/>
@@ -18536,7 +18623,7 @@
         <v>4</v>
       </c>
       <c r="N317" s="88">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O317" s="70"/>
       <c r="P317" s="70"/>
@@ -18545,7 +18632,7 @@
         <v>4</v>
       </c>
       <c r="S317" s="88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T317" s="70"/>
       <c r="U317" s="70"/>
@@ -18567,7 +18654,7 @@
         <v>10</v>
       </c>
       <c r="I318" s="88">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J318" s="70"/>
       <c r="K318" s="70"/>
@@ -18576,7 +18663,7 @@
         <v>10</v>
       </c>
       <c r="N318" s="88">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O318" s="70"/>
       <c r="P318" s="70"/>
@@ -18585,7 +18672,7 @@
         <v>10</v>
       </c>
       <c r="S318" s="88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T318" s="70"/>
       <c r="U318" s="70"/>
@@ -18607,7 +18694,7 @@
         <v>95</v>
       </c>
       <c r="I319" s="88">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J319" s="70"/>
       <c r="K319" s="70"/>
@@ -18616,7 +18703,7 @@
         <v>95</v>
       </c>
       <c r="N319" s="88">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O319" s="70"/>
       <c r="P319" s="70"/>
@@ -18625,7 +18712,7 @@
         <v>95</v>
       </c>
       <c r="S319" s="88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T319" s="70"/>
       <c r="U319" s="70"/>
@@ -18647,7 +18734,7 @@
         <v>96</v>
       </c>
       <c r="I320" s="88">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="J320" s="70"/>
       <c r="K320" s="70"/>
@@ -18656,7 +18743,7 @@
         <v>96</v>
       </c>
       <c r="N320" s="88">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O320" s="70"/>
       <c r="P320" s="70"/>
@@ -18665,7 +18752,7 @@
         <v>96</v>
       </c>
       <c r="S320" s="88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T320" s="70"/>
       <c r="U320" s="70"/>
@@ -18687,7 +18774,7 @@
         <v>97</v>
       </c>
       <c r="I321" s="88">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="J321" s="70"/>
       <c r="K321" s="70"/>
@@ -18696,7 +18783,7 @@
         <v>97</v>
       </c>
       <c r="N321" s="88">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O321" s="70"/>
       <c r="P321" s="70"/>
@@ -18705,7 +18792,7 @@
         <v>97</v>
       </c>
       <c r="S321" s="88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T321" s="70"/>
       <c r="U321" s="70"/>
@@ -18727,7 +18814,7 @@
         <v>7</v>
       </c>
       <c r="I322" s="88">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="J322" s="70"/>
       <c r="K322" s="70"/>
@@ -18736,7 +18823,7 @@
         <v>7</v>
       </c>
       <c r="N322" s="88">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O322" s="70"/>
       <c r="P322" s="70"/>
@@ -18745,7 +18832,7 @@
         <v>7</v>
       </c>
       <c r="S322" s="88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T322" s="70"/>
       <c r="U322" s="70"/>
@@ -18767,7 +18854,7 @@
         <v>6</v>
       </c>
       <c r="I323" s="88">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J323" s="70"/>
       <c r="K323" s="70"/>
@@ -18776,7 +18863,7 @@
         <v>6</v>
       </c>
       <c r="N323" s="88">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O323" s="70"/>
       <c r="P323" s="70"/>
@@ -18785,7 +18872,7 @@
         <v>6</v>
       </c>
       <c r="S323" s="88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T323" s="70"/>
       <c r="U323" s="70"/>
@@ -18816,7 +18903,7 @@
         <v>120</v>
       </c>
       <c r="N324" s="88">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O324" s="70"/>
       <c r="P324" s="70"/>
@@ -18825,7 +18912,7 @@
         <v>120</v>
       </c>
       <c r="S324" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T324" s="70"/>
       <c r="U324" s="70"/>
@@ -18847,7 +18934,7 @@
         <v>9</v>
       </c>
       <c r="I325" s="88">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J325" s="70"/>
       <c r="K325" s="70"/>
@@ -18856,7 +18943,7 @@
         <v>9</v>
       </c>
       <c r="N325" s="88">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O325" s="70"/>
       <c r="P325" s="70"/>
@@ -18865,7 +18952,7 @@
         <v>9</v>
       </c>
       <c r="S325" s="88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T325" s="70"/>
       <c r="U325" s="70"/>
@@ -18887,7 +18974,7 @@
         <v>98</v>
       </c>
       <c r="I326" s="88">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="J326" s="70"/>
       <c r="K326" s="70"/>
@@ -18896,7 +18983,7 @@
         <v>98</v>
       </c>
       <c r="N326" s="88">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O326" s="70"/>
       <c r="P326" s="70"/>
@@ -18905,7 +18992,7 @@
         <v>98</v>
       </c>
       <c r="S326" s="88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T326" s="70"/>
       <c r="U326" s="70"/>
@@ -18927,7 +19014,7 @@
         <v>5</v>
       </c>
       <c r="I327" s="88">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J327" s="70"/>
       <c r="K327" s="70"/>
@@ -18936,7 +19023,7 @@
         <v>5</v>
       </c>
       <c r="N327" s="88">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="O327" s="70"/>
       <c r="P327" s="70"/>
@@ -18945,7 +19032,7 @@
         <v>5</v>
       </c>
       <c r="S327" s="88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T327" s="70"/>
       <c r="U327" s="70"/>
@@ -18967,7 +19054,7 @@
         <v>8</v>
       </c>
       <c r="I328" s="88">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="J328" s="70"/>
       <c r="K328" s="70"/>
@@ -18976,7 +19063,7 @@
         <v>8</v>
       </c>
       <c r="N328" s="88">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="O328" s="70"/>
       <c r="P328" s="70"/>
@@ -18985,7 +19072,7 @@
         <v>8</v>
       </c>
       <c r="S328" s="88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T328" s="70"/>
       <c r="U328" s="70"/>
@@ -19016,7 +19103,7 @@
         <v>229</v>
       </c>
       <c r="N329" s="88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O329" s="70"/>
       <c r="P329" s="70"/>
@@ -19025,7 +19112,7 @@
         <v>229</v>
       </c>
       <c r="S329" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T329" s="70"/>
       <c r="U329" s="70"/>
@@ -19056,7 +19143,7 @@
         <v>230</v>
       </c>
       <c r="N330" s="88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O330" s="70"/>
       <c r="P330" s="70"/>
@@ -19065,7 +19152,7 @@
         <v>230</v>
       </c>
       <c r="S330" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T330" s="70"/>
       <c r="U330" s="70"/>
@@ -19096,7 +19183,7 @@
         <v>231</v>
       </c>
       <c r="N331" s="88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O331" s="70"/>
       <c r="P331" s="70"/>
@@ -19105,7 +19192,7 @@
         <v>231</v>
       </c>
       <c r="S331" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T331" s="70"/>
       <c r="U331" s="70"/>
@@ -19136,7 +19223,7 @@
         <v>232</v>
       </c>
       <c r="N332" s="88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O332" s="70"/>
       <c r="P332" s="70"/>
@@ -19145,7 +19232,7 @@
         <v>232</v>
       </c>
       <c r="S332" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T332" s="70"/>
       <c r="U332" s="70"/>
@@ -19176,7 +19263,7 @@
         <v>233</v>
       </c>
       <c r="N333" s="88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O333" s="70"/>
       <c r="P333" s="70"/>
@@ -19185,7 +19272,7 @@
         <v>233</v>
       </c>
       <c r="S333" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T333" s="70"/>
       <c r="U333" s="70"/>
@@ -19216,7 +19303,7 @@
         <v>234</v>
       </c>
       <c r="N334" s="88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O334" s="70"/>
       <c r="P334" s="70"/>
@@ -19225,7 +19312,7 @@
         <v>234</v>
       </c>
       <c r="S334" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T334" s="70"/>
       <c r="U334" s="70"/>
@@ -19256,7 +19343,7 @@
         <v>235</v>
       </c>
       <c r="N335" s="88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O335" s="70"/>
       <c r="P335" s="70"/>
@@ -19265,7 +19352,7 @@
         <v>235</v>
       </c>
       <c r="S335" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T335" s="70"/>
       <c r="U335" s="70"/>
@@ -19296,7 +19383,7 @@
         <v>236</v>
       </c>
       <c r="N336" s="88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O336" s="70"/>
       <c r="P336" s="70"/>
@@ -19305,7 +19392,7 @@
         <v>236</v>
       </c>
       <c r="S336" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T336" s="70"/>
       <c r="U336" s="70"/>
@@ -19336,7 +19423,7 @@
         <v>237</v>
       </c>
       <c r="N337" s="88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O337" s="70"/>
       <c r="P337" s="70"/>
@@ -19345,7 +19432,7 @@
         <v>237</v>
       </c>
       <c r="S337" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T337" s="70"/>
       <c r="U337" s="70"/>
@@ -19376,7 +19463,7 @@
         <v>238</v>
       </c>
       <c r="N338" s="88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O338" s="70"/>
       <c r="P338" s="70"/>
@@ -19385,7 +19472,7 @@
         <v>238</v>
       </c>
       <c r="S338" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T338" s="70"/>
       <c r="U338" s="70"/>
@@ -19416,7 +19503,7 @@
         <v>239</v>
       </c>
       <c r="N339" s="88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O339" s="70"/>
       <c r="P339" s="70"/>
@@ -19425,7 +19512,7 @@
         <v>239</v>
       </c>
       <c r="S339" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T339" s="70"/>
       <c r="U339" s="70"/>
@@ -19456,7 +19543,7 @@
         <v>240</v>
       </c>
       <c r="N340" s="88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O340" s="70"/>
       <c r="P340" s="70"/>
@@ -19465,7 +19552,7 @@
         <v>240</v>
       </c>
       <c r="S340" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T340" s="70"/>
       <c r="U340" s="70"/>
@@ -19496,7 +19583,7 @@
         <v>241</v>
       </c>
       <c r="N341" s="88">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="O341" s="70"/>
       <c r="P341" s="70"/>
@@ -19505,7 +19592,7 @@
         <v>241</v>
       </c>
       <c r="S341" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T341" s="70"/>
       <c r="U341" s="70"/>
@@ -20011,7 +20098,9 @@
       </c>
       <c r="N358" s="63"/>
       <c r="O358" s="63"/>
-      <c r="P358" s="63"/>
+      <c r="P358" s="63" t="s">
+        <v>253</v>
+      </c>
       <c r="Q358" s="63"/>
       <c r="R358" s="63"/>
       <c r="S358" s="63"/>
@@ -20044,11 +20133,16 @@
       </c>
       <c r="M359" s="108">
         <f>AVERAGE(M363,M365,M369,M370,M373)</f>
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="N359" s="70"/>
+      <c r="O359" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="P359" s="108">
+        <f>AVERAGE(P363,P365,P369,P370,P373)</f>
         <v>0</v>
       </c>
-      <c r="N359" s="70"/>
-      <c r="O359" s="70"/>
-      <c r="P359" s="70"/>
       <c r="Q359" s="70"/>
       <c r="R359" s="70"/>
       <c r="S359" s="70"/>
@@ -20081,11 +20175,16 @@
       </c>
       <c r="M360" s="108">
         <f>AVERAGE(M374,M371)</f>
+        <v>0.2</v>
+      </c>
+      <c r="N360" s="70"/>
+      <c r="O360" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="P360" s="108">
+        <f>AVERAGE(P374,P371)</f>
         <v>0</v>
       </c>
-      <c r="N360" s="70"/>
-      <c r="O360" s="70"/>
-      <c r="P360" s="70"/>
       <c r="Q360" s="70"/>
       <c r="R360" s="70"/>
       <c r="S360" s="70"/>
@@ -20121,8 +20220,13 @@
         <v>0.3</v>
       </c>
       <c r="N361" s="70"/>
-      <c r="O361" s="70"/>
-      <c r="P361" s="70"/>
+      <c r="O361" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="P361" s="108">
+        <f>AVERAGE(P368,P372,P364,P366,P367)</f>
+        <v>1</v>
+      </c>
       <c r="Q361" s="70"/>
       <c r="R361" s="70"/>
       <c r="S361" s="70"/>
@@ -20155,11 +20259,16 @@
       </c>
       <c r="M362" s="108">
         <f>AVERAGE(M363:M374)</f>
-        <v>0.125</v>
+        <v>0.32166666666666666</v>
       </c>
       <c r="N362" s="70"/>
-      <c r="O362" s="70"/>
-      <c r="P362" s="70"/>
+      <c r="O362" s="49" t="s">
+        <v>178</v>
+      </c>
+      <c r="P362" s="108">
+        <f>AVERAGE(P363:P374)</f>
+        <v>0.41666666666666669</v>
+      </c>
       <c r="Q362" s="70"/>
       <c r="R362" s="70"/>
       <c r="S362" s="70"/>
@@ -20191,11 +20300,15 @@
         <v>4</v>
       </c>
       <c r="M363" s="108">
+        <v>0.44</v>
+      </c>
+      <c r="N363" s="70"/>
+      <c r="O363" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="P363" s="108">
         <v>0</v>
       </c>
-      <c r="N363" s="70"/>
-      <c r="O363" s="70"/>
-      <c r="P363" s="70"/>
       <c r="Q363" s="70"/>
       <c r="R363" s="70"/>
       <c r="S363" s="70"/>
@@ -20230,8 +20343,12 @@
         <v>0.3</v>
       </c>
       <c r="N364" s="70"/>
-      <c r="O364" s="70"/>
-      <c r="P364" s="70"/>
+      <c r="O364" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="P364" s="108">
+        <v>1</v>
+      </c>
       <c r="Q364" s="70"/>
       <c r="R364" s="70"/>
       <c r="S364" s="70"/>
@@ -20263,11 +20380,15 @@
         <v>95</v>
       </c>
       <c r="M365" s="108">
+        <v>0.7</v>
+      </c>
+      <c r="N365" s="70"/>
+      <c r="O365" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="P365" s="108">
         <v>0</v>
       </c>
-      <c r="N365" s="70"/>
-      <c r="O365" s="70"/>
-      <c r="P365" s="70"/>
       <c r="Q365" s="70"/>
       <c r="R365" s="70"/>
       <c r="S365" s="70"/>
@@ -20302,8 +20423,12 @@
         <v>0.3</v>
       </c>
       <c r="N366" s="70"/>
-      <c r="O366" s="70"/>
-      <c r="P366" s="70"/>
+      <c r="O366" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="P366" s="108">
+        <v>1</v>
+      </c>
       <c r="Q366" s="70"/>
       <c r="R366" s="70"/>
       <c r="S366" s="70"/>
@@ -20338,8 +20463,12 @@
         <v>0.3</v>
       </c>
       <c r="N367" s="70"/>
-      <c r="O367" s="70"/>
-      <c r="P367" s="70"/>
+      <c r="O367" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="P367" s="108">
+        <v>1</v>
+      </c>
       <c r="Q367" s="70"/>
       <c r="R367" s="70"/>
       <c r="S367" s="70"/>
@@ -20374,8 +20503,12 @@
         <v>0.3</v>
       </c>
       <c r="N368" s="70"/>
-      <c r="O368" s="70"/>
-      <c r="P368" s="70"/>
+      <c r="O368" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="P368" s="108">
+        <v>1</v>
+      </c>
       <c r="Q368" s="70"/>
       <c r="R368" s="70"/>
       <c r="S368" s="70"/>
@@ -20407,11 +20540,15 @@
         <v>6</v>
       </c>
       <c r="M369" s="108">
+        <v>0.4</v>
+      </c>
+      <c r="N369" s="70"/>
+      <c r="O369" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="P369" s="108">
         <v>0</v>
       </c>
-      <c r="N369" s="70"/>
-      <c r="O369" s="70"/>
-      <c r="P369" s="70"/>
       <c r="Q369" s="70"/>
       <c r="R369" s="70"/>
       <c r="S369" s="70"/>
@@ -20446,8 +20583,12 @@
         <v>0</v>
       </c>
       <c r="N370" s="70"/>
-      <c r="O370" s="70"/>
-      <c r="P370" s="70"/>
+      <c r="O370" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="P370" s="108">
+        <v>0</v>
+      </c>
       <c r="Q370" s="70"/>
       <c r="R370" s="70"/>
       <c r="S370" s="70"/>
@@ -20479,11 +20620,15 @@
         <v>9</v>
       </c>
       <c r="M371" s="108">
+        <v>0.2</v>
+      </c>
+      <c r="N371" s="70"/>
+      <c r="O371" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="P371" s="108">
         <v>0</v>
       </c>
-      <c r="N371" s="70"/>
-      <c r="O371" s="70"/>
-      <c r="P371" s="70"/>
       <c r="Q371" s="70"/>
       <c r="R371" s="70"/>
       <c r="S371" s="70"/>
@@ -20513,8 +20658,12 @@
         <v>0.3</v>
       </c>
       <c r="N372" s="107"/>
-      <c r="O372" s="107"/>
-      <c r="P372" s="107"/>
+      <c r="O372" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="P372" s="108">
+        <v>1</v>
+      </c>
       <c r="Q372" s="107"/>
       <c r="R372" s="107"/>
       <c r="S372" s="107"/>
@@ -20542,11 +20691,15 @@
         <v>5</v>
       </c>
       <c r="M373" s="108">
+        <v>0.42</v>
+      </c>
+      <c r="N373" s="70"/>
+      <c r="O373" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="P373" s="108">
         <v>0</v>
       </c>
-      <c r="N373" s="70"/>
-      <c r="O373" s="70"/>
-      <c r="P373" s="70"/>
       <c r="Q373" s="70"/>
       <c r="R373" s="70"/>
       <c r="S373" s="70"/>
@@ -20574,11 +20727,15 @@
         <v>8</v>
       </c>
       <c r="M374" s="108">
+        <v>0.2</v>
+      </c>
+      <c r="N374" s="70"/>
+      <c r="O374" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="P374" s="108">
         <v>0</v>
       </c>
-      <c r="N374" s="70"/>
-      <c r="O374" s="70"/>
-      <c r="P374" s="70"/>
       <c r="Q374" s="70"/>
       <c r="R374" s="70"/>
       <c r="S374" s="70"/>
@@ -21005,10 +21162,8 @@
       <c r="O388" s="63"/>
       <c r="P388" s="63"/>
       <c r="Q388" s="63"/>
-      <c r="R388" s="64"/>
-      <c r="S388" s="64" t="s">
-        <v>253</v>
-      </c>
+      <c r="R388" s="63"/>
+      <c r="S388" s="63"/>
       <c r="T388" s="63"/>
       <c r="U388" s="63"/>
       <c r="V388" s="63"/>
@@ -21029,7 +21184,8 @@
         <v>176</v>
       </c>
       <c r="I389" s="88">
-        <v>20</v>
+        <f>AVERAGE(I393,I399,I403)</f>
+        <v>0</v>
       </c>
       <c r="J389" s="70"/>
       <c r="K389" s="70"/>
@@ -21043,12 +21199,8 @@
       <c r="O389" s="70"/>
       <c r="P389" s="70"/>
       <c r="Q389" s="70"/>
-      <c r="R389" s="49" t="s">
-        <v>176</v>
-      </c>
-      <c r="S389" s="88">
-        <v>170</v>
-      </c>
+      <c r="R389" s="70"/>
+      <c r="S389" s="70"/>
       <c r="T389" s="70"/>
       <c r="U389" s="70"/>
       <c r="V389" s="70"/>
@@ -21069,7 +21221,8 @@
         <v>175</v>
       </c>
       <c r="I390" s="88">
-        <v>20</v>
+        <f>AVERAGE(I401,I404)</f>
+        <v>0</v>
       </c>
       <c r="J390" s="70"/>
       <c r="K390" s="70"/>
@@ -21083,12 +21236,8 @@
       <c r="O390" s="70"/>
       <c r="P390" s="70"/>
       <c r="Q390" s="70"/>
-      <c r="R390" s="49" t="s">
-        <v>175</v>
-      </c>
-      <c r="S390" s="88">
-        <v>170</v>
-      </c>
+      <c r="R390" s="70"/>
+      <c r="S390" s="70"/>
       <c r="T390" s="70"/>
       <c r="U390" s="70"/>
       <c r="V390" s="70"/>
@@ -21109,6 +21258,7 @@
         <v>177</v>
       </c>
       <c r="I391" s="88">
+        <f>AVERAGE(I396:I398,I402,I394)</f>
         <v>20</v>
       </c>
       <c r="J391" s="70"/>
@@ -21123,12 +21273,8 @@
       <c r="O391" s="70"/>
       <c r="P391" s="70"/>
       <c r="Q391" s="70"/>
-      <c r="R391" s="49" t="s">
-        <v>177</v>
-      </c>
-      <c r="S391" s="88">
-        <v>170</v>
-      </c>
+      <c r="R391" s="70"/>
+      <c r="S391" s="70"/>
       <c r="T391" s="70"/>
       <c r="U391" s="70"/>
       <c r="V391" s="70"/>
@@ -21149,7 +21295,8 @@
         <v>178</v>
       </c>
       <c r="I392" s="88">
-        <v>20</v>
+        <f>AVERAGE(I393:I404)</f>
+        <v>8.3333333333333339</v>
       </c>
       <c r="J392" s="70"/>
       <c r="K392" s="70"/>
@@ -21163,12 +21310,8 @@
       <c r="O392" s="70"/>
       <c r="P392" s="70"/>
       <c r="Q392" s="70"/>
-      <c r="R392" s="49" t="s">
-        <v>178</v>
-      </c>
-      <c r="S392" s="88">
-        <v>170</v>
-      </c>
+      <c r="R392" s="70"/>
+      <c r="S392" s="70"/>
       <c r="T392" s="70"/>
       <c r="U392" s="70"/>
       <c r="V392" s="70"/>
@@ -21189,7 +21332,7 @@
         <v>4</v>
       </c>
       <c r="I393" s="88">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J393" s="70"/>
       <c r="K393" s="70"/>
@@ -21203,12 +21346,8 @@
       <c r="O393" s="70"/>
       <c r="P393" s="70"/>
       <c r="Q393" s="70"/>
-      <c r="R393" s="49" t="s">
-        <v>4</v>
-      </c>
-      <c r="S393" s="88">
-        <v>170</v>
-      </c>
+      <c r="R393" s="70"/>
+      <c r="S393" s="70"/>
       <c r="T393" s="70"/>
       <c r="U393" s="70"/>
       <c r="V393" s="70"/>
@@ -21243,12 +21382,8 @@
       <c r="O394" s="70"/>
       <c r="P394" s="70"/>
       <c r="Q394" s="70"/>
-      <c r="R394" s="49" t="s">
-        <v>10</v>
-      </c>
-      <c r="S394" s="88">
-        <v>170</v>
-      </c>
+      <c r="R394" s="70"/>
+      <c r="S394" s="70"/>
       <c r="T394" s="70"/>
       <c r="U394" s="70"/>
       <c r="V394" s="70"/>
@@ -21269,7 +21404,7 @@
         <v>95</v>
       </c>
       <c r="I395" s="88">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J395" s="70"/>
       <c r="K395" s="70"/>
@@ -21283,12 +21418,8 @@
       <c r="O395" s="70"/>
       <c r="P395" s="70"/>
       <c r="Q395" s="70"/>
-      <c r="R395" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="S395" s="88">
-        <v>170</v>
-      </c>
+      <c r="R395" s="70"/>
+      <c r="S395" s="70"/>
       <c r="T395" s="70"/>
       <c r="U395" s="70"/>
       <c r="V395" s="70"/>
@@ -21323,12 +21454,8 @@
       <c r="O396" s="70"/>
       <c r="P396" s="70"/>
       <c r="Q396" s="70"/>
-      <c r="R396" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="S396" s="88">
-        <v>170</v>
-      </c>
+      <c r="R396" s="70"/>
+      <c r="S396" s="70"/>
       <c r="T396" s="70"/>
       <c r="U396" s="70"/>
       <c r="V396" s="70"/>
@@ -21363,12 +21490,8 @@
       <c r="O397" s="70"/>
       <c r="P397" s="70"/>
       <c r="Q397" s="70"/>
-      <c r="R397" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="S397" s="88">
-        <v>170</v>
-      </c>
+      <c r="R397" s="70"/>
+      <c r="S397" s="70"/>
       <c r="T397" s="70"/>
       <c r="U397" s="70"/>
       <c r="V397" s="70"/>
@@ -21403,12 +21526,8 @@
       <c r="O398" s="70"/>
       <c r="P398" s="70"/>
       <c r="Q398" s="70"/>
-      <c r="R398" s="49" t="s">
-        <v>7</v>
-      </c>
-      <c r="S398" s="88">
-        <v>170</v>
-      </c>
+      <c r="R398" s="70"/>
+      <c r="S398" s="70"/>
       <c r="T398" s="70"/>
       <c r="U398" s="70"/>
       <c r="V398" s="70"/>
@@ -21429,7 +21548,7 @@
         <v>6</v>
       </c>
       <c r="I399" s="88">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J399" s="70"/>
       <c r="K399" s="70"/>
@@ -21443,12 +21562,8 @@
       <c r="O399" s="70"/>
       <c r="P399" s="70"/>
       <c r="Q399" s="70"/>
-      <c r="R399" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="S399" s="88">
-        <v>170</v>
-      </c>
+      <c r="R399" s="70"/>
+      <c r="S399" s="70"/>
       <c r="T399" s="70"/>
       <c r="U399" s="70"/>
       <c r="V399" s="70"/>
@@ -21469,7 +21584,7 @@
         <v>120</v>
       </c>
       <c r="I400" s="88">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J400" s="70"/>
       <c r="K400" s="70"/>
@@ -21483,12 +21598,8 @@
       <c r="O400" s="70"/>
       <c r="P400" s="70"/>
       <c r="Q400" s="70"/>
-      <c r="R400" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="S400" s="88">
-        <v>170</v>
-      </c>
+      <c r="R400" s="70"/>
+      <c r="S400" s="70"/>
       <c r="T400" s="70"/>
       <c r="U400" s="70"/>
       <c r="V400" s="70"/>
@@ -21509,7 +21620,7 @@
         <v>9</v>
       </c>
       <c r="I401" s="88">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J401" s="70"/>
       <c r="K401" s="70"/>
@@ -21523,12 +21634,8 @@
       <c r="O401" s="70"/>
       <c r="P401" s="70"/>
       <c r="Q401" s="70"/>
-      <c r="R401" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="S401" s="88">
-        <v>170</v>
-      </c>
+      <c r="R401" s="70"/>
+      <c r="S401" s="70"/>
       <c r="T401" s="70"/>
       <c r="U401" s="70"/>
       <c r="V401" s="70"/>
@@ -21563,12 +21670,8 @@
       <c r="O402" s="70"/>
       <c r="P402" s="70"/>
       <c r="Q402" s="70"/>
-      <c r="R402" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="S402" s="88">
-        <v>170</v>
-      </c>
+      <c r="R402" s="70"/>
+      <c r="S402" s="70"/>
       <c r="T402" s="70"/>
       <c r="U402" s="70"/>
       <c r="V402" s="70"/>
@@ -21589,7 +21692,7 @@
         <v>5</v>
       </c>
       <c r="I403" s="88">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J403" s="70"/>
       <c r="K403" s="70"/>
@@ -21603,12 +21706,8 @@
       <c r="O403" s="70"/>
       <c r="P403" s="70"/>
       <c r="Q403" s="70"/>
-      <c r="R403" s="49" t="s">
-        <v>5</v>
-      </c>
-      <c r="S403" s="88">
-        <v>170</v>
-      </c>
+      <c r="R403" s="70"/>
+      <c r="S403" s="70"/>
       <c r="T403" s="70"/>
       <c r="U403" s="70"/>
       <c r="V403" s="70"/>
@@ -21629,7 +21728,7 @@
         <v>8</v>
       </c>
       <c r="I404" s="88">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J404" s="70"/>
       <c r="K404" s="70"/>
@@ -21643,12 +21742,8 @@
       <c r="O404" s="70"/>
       <c r="P404" s="70"/>
       <c r="Q404" s="70"/>
-      <c r="R404" s="49" t="s">
-        <v>8</v>
-      </c>
-      <c r="S404" s="88">
-        <v>170</v>
-      </c>
+      <c r="R404" s="70"/>
+      <c r="S404" s="70"/>
       <c r="T404" s="70"/>
       <c r="U404" s="70"/>
       <c r="V404" s="70"/>
@@ -21683,12 +21778,8 @@
       <c r="O405" s="70"/>
       <c r="P405" s="70"/>
       <c r="Q405" s="70"/>
-      <c r="R405" s="68" t="s">
-        <v>229</v>
-      </c>
-      <c r="S405" s="88">
-        <v>170</v>
-      </c>
+      <c r="R405" s="70"/>
+      <c r="S405" s="70"/>
       <c r="T405" s="70"/>
       <c r="U405" s="70"/>
       <c r="V405" s="70"/>
@@ -21723,12 +21814,8 @@
       <c r="O406" s="70"/>
       <c r="P406" s="70"/>
       <c r="Q406" s="70"/>
-      <c r="R406" s="68" t="s">
-        <v>230</v>
-      </c>
-      <c r="S406" s="88">
-        <v>170</v>
-      </c>
+      <c r="R406" s="70"/>
+      <c r="S406" s="70"/>
       <c r="T406" s="70"/>
       <c r="U406" s="70"/>
       <c r="V406" s="70"/>
@@ -21763,12 +21850,8 @@
       <c r="O407" s="70"/>
       <c r="P407" s="70"/>
       <c r="Q407" s="70"/>
-      <c r="R407" s="68" t="s">
-        <v>231</v>
-      </c>
-      <c r="S407" s="88">
-        <v>170</v>
-      </c>
+      <c r="R407" s="70"/>
+      <c r="S407" s="70"/>
       <c r="T407" s="70"/>
       <c r="U407" s="70"/>
       <c r="V407" s="70"/>
@@ -21803,12 +21886,8 @@
       <c r="O408" s="70"/>
       <c r="P408" s="70"/>
       <c r="Q408" s="70"/>
-      <c r="R408" s="49" t="s">
-        <v>232</v>
-      </c>
-      <c r="S408" s="88">
-        <v>170</v>
-      </c>
+      <c r="R408" s="70"/>
+      <c r="S408" s="70"/>
       <c r="T408" s="70"/>
       <c r="U408" s="70"/>
       <c r="V408" s="70"/>
@@ -21843,12 +21922,8 @@
       <c r="O409" s="70"/>
       <c r="P409" s="70"/>
       <c r="Q409" s="70"/>
-      <c r="R409" s="49" t="s">
-        <v>233</v>
-      </c>
-      <c r="S409" s="88">
-        <v>170</v>
-      </c>
+      <c r="R409" s="70"/>
+      <c r="S409" s="70"/>
       <c r="T409" s="70"/>
       <c r="U409" s="70"/>
       <c r="V409" s="70"/>
@@ -21883,12 +21958,8 @@
       <c r="O410" s="70"/>
       <c r="P410" s="70"/>
       <c r="Q410" s="70"/>
-      <c r="R410" s="68" t="s">
-        <v>234</v>
-      </c>
-      <c r="S410" s="88">
-        <v>170</v>
-      </c>
+      <c r="R410" s="70"/>
+      <c r="S410" s="70"/>
       <c r="T410" s="70"/>
       <c r="U410" s="70"/>
       <c r="V410" s="70"/>
@@ -21923,12 +21994,8 @@
       <c r="O411" s="70"/>
       <c r="P411" s="70"/>
       <c r="Q411" s="70"/>
-      <c r="R411" s="68" t="s">
-        <v>235</v>
-      </c>
-      <c r="S411" s="88">
-        <v>170</v>
-      </c>
+      <c r="R411" s="70"/>
+      <c r="S411" s="70"/>
       <c r="T411" s="70"/>
       <c r="U411" s="70"/>
       <c r="V411" s="70"/>
@@ -21963,12 +22030,8 @@
       <c r="O412" s="70"/>
       <c r="P412" s="70"/>
       <c r="Q412" s="70"/>
-      <c r="R412" s="68" t="s">
-        <v>236</v>
-      </c>
-      <c r="S412" s="88">
-        <v>170</v>
-      </c>
+      <c r="R412" s="70"/>
+      <c r="S412" s="70"/>
       <c r="T412" s="70"/>
       <c r="U412" s="70"/>
       <c r="V412" s="70"/>
@@ -22003,12 +22066,8 @@
       <c r="O413" s="70"/>
       <c r="P413" s="70"/>
       <c r="Q413" s="70"/>
-      <c r="R413" s="68" t="s">
-        <v>237</v>
-      </c>
-      <c r="S413" s="88">
-        <v>170</v>
-      </c>
+      <c r="R413" s="70"/>
+      <c r="S413" s="70"/>
       <c r="T413" s="70"/>
       <c r="U413" s="70"/>
       <c r="V413" s="70"/>
@@ -22043,12 +22102,8 @@
       <c r="O414" s="70"/>
       <c r="P414" s="70"/>
       <c r="Q414" s="70"/>
-      <c r="R414" s="68" t="s">
-        <v>238</v>
-      </c>
-      <c r="S414" s="88">
-        <v>170</v>
-      </c>
+      <c r="R414" s="70"/>
+      <c r="S414" s="70"/>
       <c r="T414" s="70"/>
       <c r="U414" s="70"/>
       <c r="V414" s="70"/>
@@ -22083,12 +22138,8 @@
       <c r="O415" s="70"/>
       <c r="P415" s="70"/>
       <c r="Q415" s="70"/>
-      <c r="R415" s="66" t="s">
-        <v>239</v>
-      </c>
-      <c r="S415" s="88">
-        <v>170</v>
-      </c>
+      <c r="R415" s="70"/>
+      <c r="S415" s="70"/>
       <c r="T415" s="70"/>
       <c r="U415" s="70"/>
       <c r="V415" s="70"/>
@@ -22123,12 +22174,8 @@
       <c r="O416" s="70"/>
       <c r="P416" s="70"/>
       <c r="Q416" s="70"/>
-      <c r="R416" s="66" t="s">
-        <v>240</v>
-      </c>
-      <c r="S416" s="88">
-        <v>170</v>
-      </c>
+      <c r="R416" s="70"/>
+      <c r="S416" s="70"/>
       <c r="T416" s="70"/>
       <c r="U416" s="70"/>
       <c r="V416" s="70"/>
@@ -22163,12 +22210,8 @@
       <c r="O417" s="70"/>
       <c r="P417" s="70"/>
       <c r="Q417" s="70"/>
-      <c r="R417" s="49" t="s">
-        <v>241</v>
-      </c>
-      <c r="S417" s="88">
-        <v>170</v>
-      </c>
+      <c r="R417" s="70"/>
+      <c r="S417" s="70"/>
       <c r="T417" s="70"/>
       <c r="U417" s="70"/>
       <c r="V417" s="70"/>

</xml_diff>

<commit_message>
tidy up after crop sim - remove old inputs and make change to croplabour
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFB1172-C34D-4277-829F-2D5FCCCB1F52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E28784-DD3F-4715-ADBB-713A6BC99F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -3074,7 +3074,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -5382,7 +5382,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="A65" sqref="A65:B69"/>
     </sheetView>
   </sheetViews>
@@ -7588,8 +7588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7975518-D56C-48E6-B20B-FB32CB5C6D50}">
   <dimension ref="A1:AT423"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="L292" sqref="L292"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="P248" sqref="P248:P251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -16255,7 +16255,7 @@
       </c>
       <c r="O247" s="58"/>
       <c r="P247" s="58" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="Q247" s="58" t="s">
         <v>226</v>
@@ -16264,7 +16264,7 @@
         <v>227</v>
       </c>
       <c r="S247" s="58" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="T247" s="65"/>
       <c r="U247" s="63"/>
@@ -16283,10 +16283,10 @@
       <c r="F248" s="66"/>
       <c r="G248" s="67"/>
       <c r="H248" s="49" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="I248" s="106">
-        <v>0.46</v>
+        <v>0</v>
       </c>
       <c r="K248" s="70"/>
       <c r="L248" s="70"/>
@@ -16296,7 +16296,7 @@
         <v>176</v>
       </c>
       <c r="P248" s="87">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q248" s="87">
         <v>0</v>
@@ -16305,7 +16305,7 @@
         <v>0</v>
       </c>
       <c r="S248" s="87">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="U248" s="70"/>
       <c r="V248" s="70"/>
@@ -16336,7 +16336,7 @@
         <v>175</v>
       </c>
       <c r="P249" s="87">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q249" s="87">
         <v>0</v>
@@ -16345,7 +16345,7 @@
         <v>0</v>
       </c>
       <c r="S249" s="87">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="U249" s="70"/>
       <c r="V249" s="70"/>
@@ -16403,10 +16403,10 @@
       <c r="F251" s="66"/>
       <c r="G251" s="67"/>
       <c r="H251" s="49" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="I251" s="106">
-        <v>0</v>
+        <v>0.46</v>
       </c>
       <c r="K251" s="70"/>
       <c r="L251" s="70"/>
@@ -16416,7 +16416,7 @@
         <v>178</v>
       </c>
       <c r="P251" s="87">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q251" s="87">
         <v>0</v>
@@ -16425,7 +16425,7 @@
         <v>0</v>
       </c>
       <c r="S251" s="87">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="U251" s="70"/>
       <c r="V251" s="70"/>
@@ -16451,7 +16451,7 @@
       </c>
       <c r="P252" s="87">
         <f>P248</f>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q252" s="87">
         <f t="shared" ref="Q252:S252" si="49">Q248</f>
@@ -16462,8 +16462,8 @@
         <v>0</v>
       </c>
       <c r="S252" s="87">
-        <f t="shared" si="49"/>
-        <v>0</v>
+        <f>S248</f>
+        <v>150</v>
       </c>
       <c r="U252" s="70"/>
       <c r="V252" s="70"/>
@@ -16500,7 +16500,7 @@
         <v>0</v>
       </c>
       <c r="S253" s="87">
-        <f t="shared" si="50"/>
+        <f>S250</f>
         <v>0</v>
       </c>
       <c r="U253" s="70"/>
@@ -16527,7 +16527,7 @@
       </c>
       <c r="P254" s="87">
         <f>P248</f>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q254" s="87">
         <f t="shared" ref="Q254:S254" si="51">Q248</f>
@@ -16538,8 +16538,8 @@
         <v>0</v>
       </c>
       <c r="S254" s="87">
-        <f t="shared" si="51"/>
-        <v>0</v>
+        <f>S248</f>
+        <v>150</v>
       </c>
       <c r="U254" s="70"/>
       <c r="V254" s="70"/>
@@ -16628,7 +16628,7 @@
         <v>0</v>
       </c>
       <c r="S257" s="87">
-        <f t="shared" si="52"/>
+        <f>S250</f>
         <v>0</v>
       </c>
       <c r="U257" s="70"/>
@@ -16655,7 +16655,7 @@
       </c>
       <c r="P258" s="87">
         <f>P248</f>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q258" s="87">
         <f t="shared" ref="Q258:S258" si="53">Q248</f>
@@ -16666,8 +16666,8 @@
         <v>0</v>
       </c>
       <c r="S258" s="87">
-        <f t="shared" si="53"/>
-        <v>0</v>
+        <f>S248</f>
+        <v>150</v>
       </c>
       <c r="U258" s="70"/>
       <c r="V258" s="70"/>
@@ -16693,7 +16693,7 @@
       </c>
       <c r="P259" s="87">
         <f>P248</f>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q259" s="87">
         <f t="shared" ref="Q259:S259" si="54">Q248</f>
@@ -16704,8 +16704,8 @@
         <v>0</v>
       </c>
       <c r="S259" s="87">
-        <f t="shared" si="54"/>
-        <v>0</v>
+        <f>S248</f>
+        <v>150</v>
       </c>
       <c r="U259" s="70"/>
       <c r="V259" s="70"/>
@@ -16731,7 +16731,7 @@
       </c>
       <c r="P260" s="87">
         <f>P249</f>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q260" s="87">
         <f t="shared" ref="Q260:S260" si="55">Q249</f>
@@ -16742,8 +16742,8 @@
         <v>0</v>
       </c>
       <c r="S260" s="87">
-        <f t="shared" si="55"/>
-        <v>0</v>
+        <f>S249</f>
+        <v>150</v>
       </c>
       <c r="U260" s="70"/>
       <c r="V260" s="70"/>
@@ -16795,7 +16795,7 @@
       </c>
       <c r="P262" s="87">
         <f>P248</f>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q262" s="87">
         <f t="shared" ref="Q262:S262" si="56">Q248</f>
@@ -16806,8 +16806,8 @@
         <v>0</v>
       </c>
       <c r="S262" s="87">
-        <f t="shared" si="56"/>
-        <v>0</v>
+        <f>S248</f>
+        <v>150</v>
       </c>
       <c r="U262" s="70"/>
       <c r="V262" s="70"/>
@@ -16833,7 +16833,7 @@
       </c>
       <c r="P263" s="87">
         <f>P249</f>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q263" s="87">
         <f t="shared" ref="Q263:S263" si="57">Q249</f>
@@ -16844,8 +16844,8 @@
         <v>0</v>
       </c>
       <c r="S263" s="87">
-        <f t="shared" si="57"/>
-        <v>0</v>
+        <f>S249</f>
+        <v>150</v>
       </c>
       <c r="U263" s="70"/>
       <c r="V263" s="70"/>
@@ -17739,11 +17739,11 @@
         <v>120</v>
       </c>
       <c r="I291" s="94">
-        <f>I280</f>
+        <f t="shared" ref="I291:J293" si="60">I280</f>
         <v>1</v>
       </c>
       <c r="J291" s="94">
-        <f>J280</f>
+        <f t="shared" si="60"/>
         <v>0.03</v>
       </c>
       <c r="K291" s="70"/>
@@ -17775,11 +17775,11 @@
         <v>9</v>
       </c>
       <c r="I292" s="94">
-        <f>I281</f>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="J292" s="94">
-        <f>J281</f>
+        <f t="shared" si="60"/>
         <v>0.03</v>
       </c>
       <c r="K292" s="70"/>
@@ -17811,11 +17811,11 @@
         <v>98</v>
       </c>
       <c r="I293" s="94">
-        <f>I282</f>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="J293" s="94">
-        <f>J282</f>
+        <f t="shared" si="60"/>
         <v>0</v>
       </c>
       <c r="K293" s="70"/>
@@ -17883,11 +17883,11 @@
         <v>8</v>
       </c>
       <c r="I295" s="94">
-        <f t="shared" ref="I295:J295" si="60">I281</f>
+        <f t="shared" ref="I295:J295" si="61">I281</f>
         <v>1</v>
       </c>
       <c r="J295" s="94">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>0.03</v>
       </c>
       <c r="K295" s="70"/>

</xml_diff>

<commit_message>
interest rate changes to universal.xlsx after review
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\Dropbox\Michael\python\MUDAS\MUDAS 2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F9200B-9128-49B0-9554-6199B9897349}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06501EF0-C771-4230-B73E-B88FFAC059A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="84" windowWidth="23256" windowHeight="12576" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -45,10 +45,10 @@
     <definedName name="diesel_rebate" localSheetId="0">Price!$B$5</definedName>
     <definedName name="draft_seeding" localSheetId="5">'Mach 1'!$B$35</definedName>
     <definedName name="drymatter_grazed">'[1]Crop Sim'!$S$313:$S$341</definedName>
-    <definedName name="equip_insurance">Finance!$B$11</definedName>
+    <definedName name="equip_insurance">Finance!$B$17</definedName>
     <definedName name="fert_cartage_cost" localSheetId="0">Price!$B$63</definedName>
     <definedName name="fert_cost" localSheetId="0">Price!$A$65:$B$72</definedName>
-    <definedName name="fixed_dep" localSheetId="1">Finance!$B$8</definedName>
+    <definedName name="fixed_dep" localSheetId="1">Finance!$B$14</definedName>
     <definedName name="fixing_probability">'[1]Crop Sim'!$O$358:$P$374</definedName>
     <definedName name="flagfall" localSheetId="0">Price!$B$34</definedName>
     <definedName name="fuel_adj_tractor" localSheetId="5">'Mach 1'!$B$37</definedName>
@@ -75,14 +75,14 @@
     <definedName name="manager_cost">Price!$B$76</definedName>
     <definedName name="max_yield_gen">'[1]Crop Sim'!$H$11:$I$15</definedName>
     <definedName name="max_yield_spec">'[1]Crop Sim'!$K$11:$L$23</definedName>
-    <definedName name="minroe">Finance!$B$17</definedName>
+    <definedName name="minroe">Finance!$B$11</definedName>
     <definedName name="nitrogen_removed_grazing">'[1]Crop Sim'!$N$313:$N$341</definedName>
     <definedName name="nitrogen_removed_harvest">'[1]Crop Sim'!$I$313:$I$341</definedName>
     <definedName name="nutrient_leach">'[1]Crop Sim'!$L$307</definedName>
     <definedName name="nutrient_yield_params">'[1]Crop Sim'!$H$279:$J$295</definedName>
     <definedName name="oil_grease_factor_harv" localSheetId="5">'Mach 1'!$B$63</definedName>
     <definedName name="oil_grease_factor_tractor" localSheetId="5">'Mach 1'!$B$24</definedName>
-    <definedName name="opportunity_cost_capital">Finance!$B$14</definedName>
+    <definedName name="opportunity_cost_capital">Finance!$B$8</definedName>
     <definedName name="pasture_biomass">'[1]Crop Sim'!$H$358:$I$371</definedName>
     <definedName name="pasture_control">'[1]Crop Sim'!#REF!</definedName>
     <definedName name="permanent_cost">Price!$B$78</definedName>
@@ -139,14 +139,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -2138,9 +2130,6 @@
     <t>credit interest</t>
   </si>
   <si>
-    <t>Depriceation rates</t>
-  </si>
-  <si>
     <t>variable dep</t>
   </si>
   <si>
@@ -2489,9 +2478,6 @@
     <t>Sup</t>
   </si>
   <si>
-    <t>Equipment insrance rate</t>
-  </si>
-  <si>
     <t>Insurance</t>
   </si>
   <si>
@@ -2586,17 +2572,24 @@
   </si>
   <si>
     <t>ns31</t>
+  </si>
+  <si>
+    <t>Depreciation rates</t>
+  </si>
+  <si>
+    <t>Equipment insurance rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode=";;;"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2654,6 +2647,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2837,7 +2837,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="center"/>
@@ -2847,8 +2847,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2952,12 +2953,14 @@
     <xf numFmtId="2" fontId="5" fillId="9" borderId="9" xfId="2" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Formula 1" xfId="2" xr:uid="{73E7623B-26A4-407F-9297-1EB699330B2D}"/>
     <cellStyle name="Input 2" xfId="1" xr:uid="{BBF70FE2-15FC-4036-A49C-819466437B06}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{DB39D728-5C70-40A8-B0F9-CD829D9AC578}"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="4" xr:uid="{E49083D7-0748-4BC3-8D9E-EB900F92BB58}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6390,30 +6393,30 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A74" sqref="A74:XFD84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -6424,8 +6427,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -6436,13 +6439,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -6450,7 +6453,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -6458,7 +6461,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -6466,7 +6469,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -6474,7 +6477,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -6482,7 +6485,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -6490,7 +6493,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
@@ -6498,31 +6501,31 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="4">
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
@@ -6533,13 +6536,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="4.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
@@ -6550,8 +6553,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
@@ -6562,8 +6565,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -6574,99 +6577,99 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B29" s="8">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B31" s="8">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B34" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B36" s="6">
         <v>43814</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B38" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B40" s="6">
         <v>43692</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="D42" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="G42" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G42" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="H42" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B43" s="47">
         <f>AVERAGE(B49,B51,B59)</f>
@@ -6697,9 +6700,9 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B44" s="47">
         <f>AVERAGE(B57,B60)</f>
@@ -6730,9 +6733,9 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B45" s="47">
         <f>AVERAGE(B50,B52:B54,B58)</f>
@@ -6763,9 +6766,9 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B46" s="47">
         <f>AVERAGE(B49:B60)</f>
@@ -6796,36 +6799,36 @@
         <v>0.93800000000000028</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="D48" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="F48" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="G48" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="G48" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="H48" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>4</v>
       </c>
@@ -6853,7 +6856,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>10</v>
       </c>
@@ -6881,9 +6884,9 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B51" s="4">
         <v>150</v>
@@ -6909,9 +6912,9 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B52" s="4">
         <v>350</v>
@@ -6937,9 +6940,9 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B53" s="4">
         <v>350</v>
@@ -6965,7 +6968,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -6993,7 +6996,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>6</v>
       </c>
@@ -7021,9 +7024,9 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B56" s="4">
         <v>50</v>
@@ -7048,7 +7051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>9</v>
       </c>
@@ -7076,9 +7079,9 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B58" s="4">
         <v>350</v>
@@ -7104,7 +7107,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>5</v>
       </c>
@@ -7132,7 +7135,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>8</v>
       </c>
@@ -7160,150 +7163,150 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
-        <v>117</v>
       </c>
       <c r="B63" s="4">
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B66" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67" s="4">
         <v>541</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68" s="4">
         <v>339</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B69" s="4">
         <v>780</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B70" s="4">
         <v>550</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B71" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B72" s="4">
         <v>520</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="B76" s="4">
         <v>80000</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B78" s="4">
         <v>80000</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B80" s="4">
         <v>0.09</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B82" s="4">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B84" s="4">
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B86" s="4">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B88" s="4">
         <v>0.09</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B90" s="4">
         <v>3.5000000000000003E-2</v>
@@ -7321,87 +7324,87 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="4">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="49">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="49">
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="4">
+        <v>162</v>
+      </c>
+      <c r="B8" s="49">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="49">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="49">
         <v>0.02</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="4">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="B14" s="4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="B17" s="4">
+        <v>171</v>
+      </c>
+      <c r="B17" s="49">
         <v>0.02</v>
       </c>
     </row>
@@ -7415,76 +7418,76 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="G2:H13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="2" style="1" customWidth="1"/>
-    <col min="3" max="3" width="0.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="2.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="1.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.21875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="0.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="1.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G2" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="5" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G3" s="5" t="s">
-        <v>112</v>
       </c>
       <c r="H3" s="4">
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="7:8" ht="4.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="7:8" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G5" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H5" s="4">
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="7:8" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G7" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H7" s="4">
         <v>1.4</v>
       </c>
     </row>
-    <row r="8" spans="7:8" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G9" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H9" s="4">
         <v>1.7</v>
       </c>
     </row>
-    <row r="10" spans="7:8" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G11" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H11" s="4">
         <v>0.17</v>
       </c>
     </row>
-    <row r="12" spans="7:8" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G13" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H13" s="4">
         <v>0.8</v>
@@ -7504,16 +7507,16 @@
       <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.44140625" customWidth="1"/>
-    <col min="2" max="2" width="2.21875" customWidth="1"/>
-    <col min="3" max="4" width="2.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="2.28515625" customWidth="1"/>
+    <col min="3" max="4" width="2.7109375" customWidth="1"/>
     <col min="5" max="5" width="2" customWidth="1"/>
-    <col min="6" max="6" width="4.109375" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -7541,7 +7544,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="12"/>
     </row>
-    <row r="2" spans="1:26" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -7569,11 +7572,11 @@
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
     </row>
-    <row r="3" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -7599,17 +7602,17 @@
       <c r="Y3" s="13"/>
       <c r="Z3" s="13"/>
     </row>
-    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
@@ -7631,7 +7634,7 @@
       <c r="Y4" s="13"/>
       <c r="Z4" s="13"/>
     </row>
-    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="17"/>
@@ -7639,7 +7642,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
@@ -7661,7 +7664,7 @@
       <c r="Y5" s="13"/>
       <c r="Z5" s="13"/>
     </row>
-    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="22"/>
@@ -7691,7 +7694,7 @@
       <c r="Y6" s="13"/>
       <c r="Z6" s="13"/>
     </row>
-    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="22"/>
@@ -7719,7 +7722,7 @@
       <c r="Y7" s="13"/>
       <c r="Z7" s="13"/>
     </row>
-    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="22"/>
@@ -7747,7 +7750,7 @@
       <c r="Y8" s="13"/>
       <c r="Z8" s="13"/>
     </row>
-    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="22"/>
@@ -7775,7 +7778,7 @@
       <c r="Y9" s="13"/>
       <c r="Z9" s="13"/>
     </row>
-    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="22"/>
@@ -7798,7 +7801,7 @@
         <v>5</v>
       </c>
       <c r="N10" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O10" s="27"/>
       <c r="P10" s="27"/>
@@ -7813,7 +7816,7 @@
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
     </row>
-    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="22"/>
@@ -7822,7 +7825,7 @@
       <c r="F11" s="28"/>
       <c r="H11" s="32"/>
       <c r="I11" s="45" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J11" s="33">
         <v>11400</v>
@@ -7840,7 +7843,7 @@
         <v>7000</v>
       </c>
       <c r="O11" s="32" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="P11" s="34"/>
       <c r="Q11" s="34"/>
@@ -7854,7 +7857,7 @@
       <c r="Y11" s="13"/>
       <c r="Z11" s="13"/>
     </row>
-    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="22"/>
@@ -7863,7 +7866,7 @@
       <c r="F12" s="28"/>
       <c r="H12" s="32"/>
       <c r="I12" s="45" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J12" s="33">
         <v>0.1</v>
@@ -7893,7 +7896,7 @@
       <c r="Y12" s="13"/>
       <c r="Z12" s="13"/>
     </row>
-    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="22"/>
@@ -7902,7 +7905,7 @@
       <c r="F13" s="28"/>
       <c r="H13" s="32"/>
       <c r="I13" s="45" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J13" s="33">
         <v>90</v>
@@ -7920,7 +7923,7 @@
         <v>90</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="P13" s="34"/>
       <c r="Q13" s="34"/>
@@ -7934,7 +7937,7 @@
       <c r="Y13" s="13"/>
       <c r="Z13" s="13"/>
     </row>
-    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="12"/>
       <c r="C14" s="22"/>
@@ -7943,7 +7946,7 @@
       <c r="F14" s="28"/>
       <c r="H14" s="32"/>
       <c r="I14" s="45" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J14" s="33">
         <v>80</v>
@@ -7961,7 +7964,7 @@
         <v>75</v>
       </c>
       <c r="O14" s="32" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="P14" s="34"/>
       <c r="Q14" s="34"/>
@@ -7975,7 +7978,7 @@
       <c r="Y14" s="13"/>
       <c r="Z14" s="13"/>
     </row>
-    <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="C15" s="22"/>
@@ -8003,7 +8006,7 @@
       <c r="Y15" s="13"/>
       <c r="Z15" s="13"/>
     </row>
-    <row r="16" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="22"/>
@@ -8031,7 +8034,7 @@
       <c r="Y16" s="13"/>
       <c r="Z16" s="13"/>
     </row>
-    <row r="17" spans="1:26" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="C17" s="40"/>
@@ -8058,13 +8061,13 @@
       <c r="U17" s="40"/>
       <c r="V17" s="40"/>
       <c r="W17" s="42" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
       <c r="Z17" s="13"/>
     </row>
-    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -8092,7 +8095,7 @@
       <c r="Y18" s="13"/>
       <c r="Z18" s="13"/>
     </row>
-    <row r="19" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -8120,11 +8123,11 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
@@ -8150,17 +8153,17 @@
       <c r="Y20" s="13"/>
       <c r="Z20" s="13"/>
     </row>
-    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
@@ -8182,7 +8185,7 @@
       <c r="Y21" s="13"/>
       <c r="Z21" s="13"/>
     </row>
-    <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="17"/>
@@ -8190,7 +8193,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
@@ -8212,7 +8215,7 @@
       <c r="Y22" s="13"/>
       <c r="Z22" s="13"/>
     </row>
-    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="12"/>
       <c r="C23" s="22"/>
@@ -8242,7 +8245,7 @@
       <c r="Y23" s="13"/>
       <c r="Z23" s="13"/>
     </row>
-    <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="22"/>
@@ -8270,7 +8273,7 @@
       <c r="Y24" s="13"/>
       <c r="Z24" s="13"/>
     </row>
-    <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="C25" s="22"/>
@@ -8298,7 +8301,7 @@
       <c r="Y25" s="13"/>
       <c r="Z25" s="13"/>
     </row>
-    <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="22"/>
@@ -8308,7 +8311,7 @@
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J26" s="26" t="s">
         <v>6</v>
@@ -8323,7 +8326,7 @@
         <v>5</v>
       </c>
       <c r="N26" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O26" s="27"/>
       <c r="P26" s="27"/>
@@ -8338,7 +8341,7 @@
       <c r="Y26" s="13"/>
       <c r="Z26" s="13"/>
     </row>
-    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="22"/>
@@ -8348,22 +8351,22 @@
       <c r="G27" s="29"/>
       <c r="H27" s="29"/>
       <c r="I27" s="29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J27" s="30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K27" s="30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L27" s="30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M27" s="30" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N27" s="30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="O27" s="30"/>
       <c r="P27" s="30"/>
@@ -8378,7 +8381,7 @@
       <c r="Y27" s="13"/>
       <c r="Z27" s="13"/>
     </row>
-    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="22"/>
@@ -8387,7 +8390,7 @@
       <c r="F28" s="28"/>
       <c r="H28" s="32"/>
       <c r="I28" s="45" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J28" s="44">
         <v>0.45</v>
@@ -8405,7 +8408,7 @@
         <v>1</v>
       </c>
       <c r="O28" s="32" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="P28" s="34"/>
       <c r="Q28" s="34"/>
@@ -8419,7 +8422,7 @@
       <c r="Y28" s="13"/>
       <c r="Z28" s="13"/>
     </row>
-    <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="22"/>
@@ -8447,7 +8450,7 @@
       <c r="Y29" s="13"/>
       <c r="Z29" s="13"/>
     </row>
-    <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="22"/>
@@ -8475,7 +8478,7 @@
       <c r="Y30" s="13"/>
       <c r="Z30" s="13"/>
     </row>
-    <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
       <c r="C31" s="40"/>
@@ -8502,13 +8505,13 @@
       <c r="U31" s="40"/>
       <c r="V31" s="40"/>
       <c r="W31" s="42" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="X31" s="13"/>
       <c r="Y31" s="13"/>
       <c r="Z31" s="13"/>
     </row>
-    <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -8551,41 +8554,41 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="B3" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="9.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -8593,7 +8596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -8601,7 +8604,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -8609,7 +8612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -8617,7 +8620,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -8625,7 +8628,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -8633,7 +8636,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -8641,60 +8644,60 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="B19" s="4">
         <v>12.2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B21" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
@@ -8702,7 +8705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>4</v>
       </c>
@@ -8710,7 +8713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>6</v>
       </c>
@@ -8718,7 +8721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
@@ -8726,7 +8729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
@@ -8734,7 +8737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
@@ -8742,7 +8745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>10</v>
       </c>
@@ -8750,33 +8753,33 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B31" s="4">
         <v>4.5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B32" s="4">
         <v>4.5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B33" s="4">
         <v>4.5</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B35" s="6">
         <v>43554</v>
@@ -8798,268 +8801,268 @@
       <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="19.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="4">
         <v>1000</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4">
         <v>0.08</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="4">
         <v>188000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="4">
         <v>87000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="4">
         <v>297000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="4">
         <v>90000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="4">
         <v>35000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="4">
         <v>15000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="4">
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B16" s="4">
         <v>75000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="4">
         <v>36000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="4">
         <v>78000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="4">
         <v>22000</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="4">
         <v>110000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="4">
         <v>36000</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="4">
         <v>1.25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="B29" s="4">
         <v>12.2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="4">
         <v>0.6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="4.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B33" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35">
         <v>5.41</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37">
         <v>1.08</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B39">
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>5</v>
       </c>
@@ -9067,7 +9070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>4</v>
       </c>
@@ -9075,7 +9078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>6</v>
       </c>
@@ -9083,23 +9086,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B49" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>8</v>
       </c>
@@ -9107,7 +9110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>9</v>
       </c>
@@ -9115,7 +9118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>7</v>
       </c>
@@ -9123,7 +9126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>10</v>
       </c>
@@ -9131,78 +9134,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B55" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B56" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
-        <v>50</v>
       </c>
       <c r="B59" s="4">
         <v>12.2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B61" s="4">
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B63" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B65" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B67" s="4"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>5</v>
       </c>
@@ -9210,7 +9213,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>4</v>
       </c>
@@ -9218,7 +9221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>6</v>
       </c>
@@ -9226,7 +9229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>8</v>
       </c>
@@ -9234,7 +9237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>9</v>
       </c>
@@ -9242,7 +9245,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>7</v>
       </c>
@@ -9250,7 +9253,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>10</v>
       </c>
@@ -9258,37 +9261,37 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B75" s="4">
         <v>5.5</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B76" s="4">
         <v>5.5</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B77" s="4">
         <v>5.5</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B79" s="4"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>5</v>
       </c>
@@ -9296,7 +9299,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>4</v>
       </c>
@@ -9304,7 +9307,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>6</v>
       </c>
@@ -9312,7 +9315,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>8</v>
       </c>
@@ -9320,7 +9323,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>9</v>
       </c>
@@ -9328,7 +9331,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>7</v>
       </c>
@@ -9336,7 +9339,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>10</v>
       </c>
@@ -9344,233 +9347,233 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B87" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B88" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B89" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="4" t="s">
-        <v>56</v>
       </c>
       <c r="B92" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B94" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B96" s="4">
         <v>0.6</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="4.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B98" s="4">
         <v>0.6</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="3" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B100" s="4">
         <v>1.3</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="B103" s="4">
         <v>11.3</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B105" s="4"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="B105" s="4"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="B106" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B107" s="4"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B108" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B109" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B110" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B111" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B112" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B114" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="7.2" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B116" s="4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B118" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="5.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B120" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B122" s="4">
         <v>14.3</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="4" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="4" t="s">
-        <v>76</v>
       </c>
       <c r="B125" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B127" s="4">
         <v>1.3</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="8"/>
       <c r="B130" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>6</v>
       </c>
@@ -9581,7 +9584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="9" t="s">
         <v>4</v>
       </c>
@@ -9592,7 +9595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>7</v>
       </c>
@@ -9603,7 +9606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="9" t="s">
         <v>5</v>
       </c>
@@ -9614,9 +9617,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B135" s="8">
         <v>1</v>

</xml_diff>

<commit_message>
fix offs day per period alter sup feed formula alter sup feed inputs
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06501EF0-C771-4230-B73E-B88FFAC059A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5DBDC5-562A-43E0-B41F-400848D0FDD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -138,6 +138,14 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2849,7 +2857,7 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2954,6 +2962,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="5" fillId="8" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Formula 1" xfId="2" xr:uid="{73E7623B-26A4-407F-9297-1EB699330B2D}"/>
@@ -6397,26 +6406,26 @@
       <selection activeCell="A74" sqref="A74:XFD84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -6427,8 +6436,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -6439,13 +6448,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -6453,7 +6462,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -6461,7 +6470,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -6469,7 +6478,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -6477,7 +6486,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -6485,7 +6494,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -6493,7 +6502,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
@@ -6501,7 +6510,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>95</v>
       </c>
@@ -6509,7 +6518,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>96</v>
       </c>
@@ -6517,7 +6526,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>97</v>
       </c>
@@ -6525,7 +6534,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
@@ -6536,13 +6545,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
@@ -6553,8 +6562,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
@@ -6565,8 +6574,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -6577,12 +6586,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>136</v>
       </c>
@@ -6590,10 +6599,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="6.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>135</v>
       </c>
@@ -6601,13 +6610,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>102</v>
       </c>
@@ -6615,7 +6624,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>103</v>
       </c>
@@ -6623,8 +6632,8 @@
         <v>43814</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>104</v>
       </c>
@@ -6632,8 +6641,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>133</v>
       </c>
@@ -6641,7 +6650,7 @@
         <v>43692</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>91</v>
       </c>
@@ -6667,7 +6676,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="46" t="s">
         <v>166</v>
       </c>
@@ -6700,7 +6709,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="46" t="s">
         <v>165</v>
       </c>
@@ -6733,7 +6742,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="46" t="s">
         <v>167</v>
       </c>
@@ -6766,7 +6775,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="46" t="s">
         <v>168</v>
       </c>
@@ -6799,10 +6808,10 @@
         <v>0.93800000000000028</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>91</v>
       </c>
@@ -6828,7 +6837,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>4</v>
       </c>
@@ -6856,7 +6865,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>10</v>
       </c>
@@ -6884,7 +6893,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>94</v>
       </c>
@@ -6912,7 +6921,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>95</v>
       </c>
@@ -6940,7 +6949,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>96</v>
       </c>
@@ -6968,7 +6977,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -6996,7 +7005,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>6</v>
       </c>
@@ -7024,7 +7033,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>119</v>
       </c>
@@ -7051,7 +7060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>9</v>
       </c>
@@ -7079,7 +7088,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>97</v>
       </c>
@@ -7107,7 +7116,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>5</v>
       </c>
@@ -7135,7 +7144,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>8</v>
       </c>
@@ -7163,12 +7172,12 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>116</v>
       </c>
@@ -7176,10 +7185,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="9.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>112</v>
       </c>
@@ -7187,7 +7196,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>68</v>
       </c>
@@ -7195,7 +7204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>67</v>
       </c>
@@ -7203,7 +7212,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>66</v>
       </c>
@@ -7211,7 +7220,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
         <v>114</v>
       </c>
@@ -7219,7 +7228,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>63</v>
       </c>
@@ -7227,7 +7236,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>169</v>
       </c>
@@ -7235,7 +7244,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>65</v>
       </c>
@@ -7243,12 +7252,12 @@
         <v>520</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>122</v>
       </c>
@@ -7256,7 +7265,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>123</v>
       </c>
@@ -7264,7 +7273,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>124</v>
       </c>
@@ -7272,7 +7281,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>125</v>
       </c>
@@ -7280,7 +7289,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>126</v>
       </c>
@@ -7288,7 +7297,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>127</v>
       </c>
@@ -7296,7 +7305,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>128</v>
       </c>
@@ -7304,7 +7313,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>129</v>
       </c>
@@ -7324,22 +7333,22 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -7347,8 +7356,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -7356,12 +7365,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>162</v>
       </c>
@@ -7369,12 +7378,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>163</v>
       </c>
@@ -7382,12 +7391,12 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
@@ -7395,12 +7404,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>171</v>
       </c>
@@ -7422,23 +7431,23 @@
       <selection activeCell="A15" sqref="A15:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="2" style="1" customWidth="1"/>
-    <col min="3" max="3" width="0.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="2.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="1.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="0.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="1.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.26953125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G2" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G3" s="5" t="s">
         <v>111</v>
       </c>
@@ -7446,10 +7455,10 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="7:8" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="7:8" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G5" s="4" t="s">
         <v>105</v>
       </c>
@@ -7457,8 +7466,8 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G7" s="4" t="s">
         <v>106</v>
       </c>
@@ -7466,8 +7475,8 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="8" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G9" s="4" t="s">
         <v>107</v>
       </c>
@@ -7475,8 +7484,8 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="10" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G11" s="4" t="s">
         <v>108</v>
       </c>
@@ -7484,8 +7493,8 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="12" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G13" s="4" t="s">
         <v>109</v>
       </c>
@@ -7503,20 +7512,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBAE29A-401D-4B75-B63C-3693AC93217E}">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14:N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="2.28515625" customWidth="1"/>
-    <col min="3" max="4" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" customWidth="1"/>
+    <col min="2" max="2" width="2.26953125" customWidth="1"/>
+    <col min="3" max="4" width="2.7265625" customWidth="1"/>
     <col min="5" max="5" width="2" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="4.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -7544,7 +7553,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="12"/>
     </row>
-    <row r="2" spans="1:26" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -7572,7 +7581,7 @@
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
     </row>
-    <row r="3" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="14" t="s">
@@ -7602,7 +7611,7 @@
       <c r="Y3" s="13"/>
       <c r="Z3" s="13"/>
     </row>
-    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="17"/>
@@ -7634,7 +7643,7 @@
       <c r="Y4" s="13"/>
       <c r="Z4" s="13"/>
     </row>
-    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="17"/>
@@ -7664,7 +7673,7 @@
       <c r="Y5" s="13"/>
       <c r="Z5" s="13"/>
     </row>
-    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="22"/>
@@ -7694,7 +7703,7 @@
       <c r="Y6" s="13"/>
       <c r="Z6" s="13"/>
     </row>
-    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="22"/>
@@ -7722,7 +7731,7 @@
       <c r="Y7" s="13"/>
       <c r="Z7" s="13"/>
     </row>
-    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="22"/>
@@ -7750,7 +7759,7 @@
       <c r="Y8" s="13"/>
       <c r="Z8" s="13"/>
     </row>
-    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="22"/>
@@ -7778,7 +7787,7 @@
       <c r="Y9" s="13"/>
       <c r="Z9" s="13"/>
     </row>
-    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="22"/>
@@ -7816,7 +7825,7 @@
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
     </row>
-    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="22"/>
@@ -7857,7 +7866,7 @@
       <c r="Y11" s="13"/>
       <c r="Z11" s="13"/>
     </row>
-    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="22"/>
@@ -7896,7 +7905,7 @@
       <c r="Y12" s="13"/>
       <c r="Z12" s="13"/>
     </row>
-    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="22"/>
@@ -7907,20 +7916,20 @@
       <c r="I13" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="J13" s="33">
-        <v>90</v>
-      </c>
-      <c r="K13" s="33">
-        <v>90</v>
-      </c>
-      <c r="L13" s="33">
-        <v>90</v>
-      </c>
-      <c r="M13" s="33">
-        <v>90</v>
-      </c>
-      <c r="N13" s="33">
-        <v>90</v>
+      <c r="J13" s="50">
+        <v>0.9</v>
+      </c>
+      <c r="K13" s="50">
+        <v>0.9</v>
+      </c>
+      <c r="L13" s="50">
+        <v>0.9</v>
+      </c>
+      <c r="M13" s="50">
+        <v>0.9</v>
+      </c>
+      <c r="N13" s="50">
+        <v>0.9</v>
       </c>
       <c r="O13" s="32" t="s">
         <v>144</v>
@@ -7937,7 +7946,7 @@
       <c r="Y13" s="13"/>
       <c r="Z13" s="13"/>
     </row>
-    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11"/>
       <c r="B14" s="12"/>
       <c r="C14" s="22"/>
@@ -7948,20 +7957,20 @@
       <c r="I14" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="J14" s="33">
-        <v>80</v>
-      </c>
-      <c r="K14" s="33">
-        <v>80</v>
-      </c>
-      <c r="L14" s="33">
-        <v>95</v>
-      </c>
-      <c r="M14" s="33">
-        <v>80</v>
-      </c>
-      <c r="N14" s="33">
-        <v>75</v>
+      <c r="J14" s="50">
+        <v>0.8</v>
+      </c>
+      <c r="K14" s="50">
+        <v>0.8</v>
+      </c>
+      <c r="L14" s="50">
+        <v>0.95</v>
+      </c>
+      <c r="M14" s="50">
+        <v>0.8</v>
+      </c>
+      <c r="N14" s="50">
+        <v>0.75</v>
       </c>
       <c r="O14" s="32" t="s">
         <v>145</v>
@@ -7978,7 +7987,7 @@
       <c r="Y14" s="13"/>
       <c r="Z14" s="13"/>
     </row>
-    <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="C15" s="22"/>
@@ -8006,7 +8015,7 @@
       <c r="Y15" s="13"/>
       <c r="Z15" s="13"/>
     </row>
-    <row r="16" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="22"/>
@@ -8034,7 +8043,7 @@
       <c r="Y16" s="13"/>
       <c r="Z16" s="13"/>
     </row>
-    <row r="17" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="C17" s="40"/>
@@ -8067,7 +8076,7 @@
       <c r="Y17" s="13"/>
       <c r="Z17" s="13"/>
     </row>
-    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -8095,7 +8104,7 @@
       <c r="Y18" s="13"/>
       <c r="Z18" s="13"/>
     </row>
-    <row r="19" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -8123,7 +8132,7 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="14" t="s">
@@ -8153,7 +8162,7 @@
       <c r="Y20" s="13"/>
       <c r="Z20" s="13"/>
     </row>
-    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="C21" s="17"/>
@@ -8185,7 +8194,7 @@
       <c r="Y21" s="13"/>
       <c r="Z21" s="13"/>
     </row>
-    <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="17"/>
@@ -8215,7 +8224,7 @@
       <c r="Y22" s="13"/>
       <c r="Z22" s="13"/>
     </row>
-    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
       <c r="B23" s="12"/>
       <c r="C23" s="22"/>
@@ -8245,7 +8254,7 @@
       <c r="Y23" s="13"/>
       <c r="Z23" s="13"/>
     </row>
-    <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="22"/>
@@ -8273,7 +8282,7 @@
       <c r="Y24" s="13"/>
       <c r="Z24" s="13"/>
     </row>
-    <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="C25" s="22"/>
@@ -8301,7 +8310,7 @@
       <c r="Y25" s="13"/>
       <c r="Z25" s="13"/>
     </row>
-    <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="22"/>
@@ -8341,7 +8350,7 @@
       <c r="Y26" s="13"/>
       <c r="Z26" s="13"/>
     </row>
-    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="22"/>
@@ -8381,7 +8390,7 @@
       <c r="Y27" s="13"/>
       <c r="Z27" s="13"/>
     </row>
-    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="22"/>
@@ -8422,7 +8431,7 @@
       <c r="Y28" s="13"/>
       <c r="Z28" s="13"/>
     </row>
-    <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="22"/>
@@ -8450,7 +8459,7 @@
       <c r="Y29" s="13"/>
       <c r="Z29" s="13"/>
     </row>
-    <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="22"/>
@@ -8478,7 +8487,7 @@
       <c r="Y30" s="13"/>
       <c r="Z30" s="13"/>
     </row>
-    <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
       <c r="C31" s="40"/>
@@ -8511,7 +8520,7 @@
       <c r="Y31" s="13"/>
       <c r="Z31" s="13"/>
     </row>
-    <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -8554,19 +8563,19 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>89</v>
       </c>
@@ -8574,21 +8583,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="9.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -8596,7 +8605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -8604,7 +8613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -8612,7 +8621,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -8620,7 +8629,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -8628,7 +8637,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -8636,7 +8645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -8644,7 +8653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>95</v>
       </c>
@@ -8652,7 +8661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>96</v>
       </c>
@@ -8660,7 +8669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>97</v>
       </c>
@@ -8668,12 +8677,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>83</v>
       </c>
@@ -8681,8 +8690,8 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>87</v>
       </c>
@@ -8690,14 +8699,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
@@ -8705,7 +8714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>4</v>
       </c>
@@ -8713,7 +8722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>6</v>
       </c>
@@ -8721,7 +8730,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
@@ -8729,7 +8738,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
@@ -8737,7 +8746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
@@ -8745,7 +8754,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>10</v>
       </c>
@@ -8753,7 +8762,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>95</v>
       </c>
@@ -8761,7 +8770,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>96</v>
       </c>
@@ -8769,7 +8778,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>97</v>
       </c>
@@ -8777,7 +8786,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>133</v>
       </c>
@@ -8801,19 +8810,19 @@
       <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="19.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -8824,8 +8833,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
@@ -8834,12 +8843,12 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>117</v>
       </c>
@@ -8847,7 +8856,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -8855,7 +8864,7 @@
         <v>188000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
@@ -8863,7 +8872,7 @@
         <v>87000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
@@ -8871,7 +8880,7 @@
         <v>297000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
@@ -8879,7 +8888,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
@@ -8887,7 +8896,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -8895,7 +8904,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
@@ -8903,7 +8912,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
@@ -8911,7 +8920,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
@@ -8919,7 +8928,7 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
@@ -8927,7 +8936,7 @@
         <v>78000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>37</v>
       </c>
@@ -8935,7 +8944,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
@@ -8943,7 +8952,7 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
@@ -8951,12 +8960,12 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
@@ -8964,8 +8973,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>41</v>
       </c>
@@ -8973,12 +8982,12 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>43</v>
       </c>
@@ -8986,8 +8995,8 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
@@ -8995,8 +9004,8 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>77</v>
       </c>
@@ -9004,8 +9013,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -9013,8 +9022,8 @@
         <v>5.41</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -9022,8 +9031,8 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -9031,14 +9040,14 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>130</v>
       </c>
@@ -9046,7 +9055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>131</v>
       </c>
@@ -9054,7 +9063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>132</v>
       </c>
@@ -9062,7 +9071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>5</v>
       </c>
@@ -9070,7 +9079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>4</v>
       </c>
@@ -9078,7 +9087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>6</v>
       </c>
@@ -9086,7 +9095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>94</v>
       </c>
@@ -9094,7 +9103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>119</v>
       </c>
@@ -9102,7 +9111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>8</v>
       </c>
@@ -9110,7 +9119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>9</v>
       </c>
@@ -9118,7 +9127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>7</v>
       </c>
@@ -9126,7 +9135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>10</v>
       </c>
@@ -9134,7 +9143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>95</v>
       </c>
@@ -9142,7 +9151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>96</v>
       </c>
@@ -9150,7 +9159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>97</v>
       </c>
@@ -9158,12 +9167,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>49</v>
       </c>
@@ -9171,8 +9180,8 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>50</v>
       </c>
@@ -9180,8 +9189,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>51</v>
       </c>
@@ -9189,8 +9198,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>86</v>
       </c>
@@ -9198,14 +9207,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B67" s="4"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>5</v>
       </c>
@@ -9213,7 +9222,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
         <v>4</v>
       </c>
@@ -9221,7 +9230,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>6</v>
       </c>
@@ -9229,7 +9238,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>8</v>
       </c>
@@ -9237,7 +9246,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>9</v>
       </c>
@@ -9245,7 +9254,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
         <v>7</v>
       </c>
@@ -9253,7 +9262,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>10</v>
       </c>
@@ -9261,7 +9270,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
         <v>95</v>
       </c>
@@ -9269,7 +9278,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>96</v>
       </c>
@@ -9277,7 +9286,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
         <v>97</v>
       </c>
@@ -9285,13 +9294,13 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B79" s="4"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>5</v>
       </c>
@@ -9299,7 +9308,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>4</v>
       </c>
@@ -9307,7 +9316,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>6</v>
       </c>
@@ -9315,7 +9324,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>8</v>
       </c>
@@ -9323,7 +9332,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>9</v>
       </c>
@@ -9331,7 +9340,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>7</v>
       </c>
@@ -9339,7 +9348,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>10</v>
       </c>
@@ -9347,7 +9356,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>95</v>
       </c>
@@ -9355,7 +9364,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>96</v>
       </c>
@@ -9363,7 +9372,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>97</v>
       </c>
@@ -9371,12 +9380,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
         <v>55</v>
       </c>
@@ -9384,8 +9393,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
         <v>56</v>
       </c>
@@ -9393,8 +9402,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
         <v>57</v>
       </c>
@@ -9402,8 +9411,8 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
         <v>58</v>
       </c>
@@ -9411,8 +9420,8 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" ht="3" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>59</v>
       </c>
@@ -9420,12 +9429,12 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="4" t="s">
         <v>61</v>
       </c>
@@ -9433,13 +9442,13 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B105" s="4"/>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="4" t="s">
         <v>63</v>
       </c>
@@ -9447,13 +9456,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B107" s="4"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="4" t="s">
         <v>64</v>
       </c>
@@ -9461,7 +9470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
         <v>65</v>
       </c>
@@ -9469,7 +9478,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
         <v>66</v>
       </c>
@@ -9477,7 +9486,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
         <v>67</v>
       </c>
@@ -9485,7 +9494,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="s">
         <v>68</v>
       </c>
@@ -9493,7 +9502,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>69</v>
       </c>
@@ -9501,8 +9510,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
         <v>70</v>
       </c>
@@ -9510,8 +9519,8 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
         <v>71</v>
       </c>
@@ -9519,8 +9528,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" ht="5.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
         <v>72</v>
       </c>
@@ -9528,8 +9537,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>73</v>
       </c>
@@ -9537,12 +9546,12 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
         <v>75</v>
       </c>
@@ -9550,8 +9559,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
         <v>76</v>
       </c>
@@ -9559,12 +9568,12 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="8"/>
       <c r="B130" s="8" t="s">
         <v>147</v>
@@ -9573,7 +9582,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="9" t="s">
         <v>6</v>
       </c>
@@ -9584,7 +9593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="9" t="s">
         <v>4</v>
       </c>
@@ -9595,7 +9604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133" s="9" t="s">
         <v>7</v>
       </c>
@@ -9606,7 +9615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="9" t="s">
         <v>5</v>
       </c>
@@ -9617,7 +9626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135" s="9" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
update pasture sowing to have all landuses. to improve detail and compatability
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5DBDC5-562A-43E0-B41F-400848D0FDD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C50C5F-607E-411D-8240-065738270651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -62,13 +62,13 @@
     <definedName name="grain_income_length" localSheetId="0">Price!$B$38</definedName>
     <definedName name="grain_price" localSheetId="0">Price!$A$48:$H$60</definedName>
     <definedName name="grain_price_grouped">Price!$A$42:$H$46</definedName>
-    <definedName name="harv_eff" localSheetId="5">'Mach 1'!$B$65</definedName>
-    <definedName name="harv_fuel_consumption" localSheetId="5">'Mach 1'!$B$61</definedName>
+    <definedName name="harv_eff" localSheetId="5">'Mach 1'!$B$72</definedName>
+    <definedName name="harv_fuel_consumption" localSheetId="5">'Mach 1'!$B$68</definedName>
     <definedName name="harvest_index">'[1]Crop Sim'!$L$358:$M$374</definedName>
-    <definedName name="harvest_maint" localSheetId="5">'Mach 1'!$A$79:$B$89</definedName>
-    <definedName name="harvest_speed" localSheetId="5">'Mach 1'!$A$67:$B$77</definedName>
+    <definedName name="harvest_maint" localSheetId="5">'Mach 1'!$A$86:$B$96</definedName>
+    <definedName name="harvest_speed" localSheetId="5">'Mach 1'!$A$74:$B$84</definedName>
     <definedName name="harvest_yield" localSheetId="4">'Mach General'!$A$6:$B$16</definedName>
-    <definedName name="harvester_width" localSheetId="5">'Mach 1'!$B$59</definedName>
+    <definedName name="harvester_width" localSheetId="5">'Mach 1'!$B$66</definedName>
     <definedName name="initial_fungus">'[1]Crop Sim'!#REF!</definedName>
     <definedName name="initial_weed">'[1]Crop Sim'!#REF!</definedName>
     <definedName name="insurance_date">'Mach General'!$B$35</definedName>
@@ -80,7 +80,7 @@
     <definedName name="nitrogen_removed_harvest">'[1]Crop Sim'!$I$313:$I$341</definedName>
     <definedName name="nutrient_leach">'[1]Crop Sim'!$L$307</definedName>
     <definedName name="nutrient_yield_params">'[1]Crop Sim'!$H$279:$J$295</definedName>
-    <definedName name="oil_grease_factor_harv" localSheetId="5">'Mach 1'!$B$63</definedName>
+    <definedName name="oil_grease_factor_harv" localSheetId="5">'Mach 1'!$B$70</definedName>
     <definedName name="oil_grease_factor_tractor" localSheetId="5">'Mach 1'!$B$24</definedName>
     <definedName name="opportunity_cost_capital">Finance!$B$8</definedName>
     <definedName name="pasture_biomass">'[1]Crop Sim'!$H$358:$I$371</definedName>
@@ -100,7 +100,7 @@
     <definedName name="seedbank_value">'[1]Crop Sim'!$G$119:$I$121</definedName>
     <definedName name="seeder_base_crop" localSheetId="5">'Mach 1'!#REF!</definedName>
     <definedName name="seeder_speed_base" localSheetId="5">'Mach 1'!$B$33</definedName>
-    <definedName name="seeder_speed_crop_adj" localSheetId="5">'Mach 1'!$A$41:$B$56</definedName>
+    <definedName name="seeder_speed_crop_adj" localSheetId="5">'Mach 1'!$A$41:$B$63</definedName>
     <definedName name="seeder_width" localSheetId="5">'Mach 1'!$B$29</definedName>
     <definedName name="seeding_eff" localSheetId="5">'Mach 1'!$B$31</definedName>
     <definedName name="seeds_die">'[1]Crop Sim'!$W$119:$Y$121</definedName>
@@ -108,25 +108,25 @@
     <definedName name="seedset_min">'[1]Crop Sim'!$L$125:$M$125</definedName>
     <definedName name="seedset_slope">'[1]Crop Sim'!$L$123:$M$123</definedName>
     <definedName name="Soil_nitrate_slope">'[1]Crop Sim'!$N$389:$N$417</definedName>
-    <definedName name="sprayer_eff" localSheetId="5">'Mach 1'!$B$96</definedName>
-    <definedName name="sprayer_fuel_consumption" localSheetId="5">'Mach 1'!$B$98</definedName>
-    <definedName name="sprayer_maint" localSheetId="5">'Mach 1'!$B$100</definedName>
-    <definedName name="sprayer_speed" localSheetId="5">'Mach 1'!$B$94</definedName>
-    <definedName name="sprayer_width" localSheetId="5">'Mach 1'!$B$92</definedName>
-    <definedName name="spreader_cap" localSheetId="5">'Mach 1'!$B$114</definedName>
-    <definedName name="spreader_eff" localSheetId="5">'Mach 1'!$B$120</definedName>
-    <definedName name="spreader_fuel" localSheetId="5">'Mach 1'!$B$103</definedName>
-    <definedName name="spreader_maint" localSheetId="5">'Mach 1'!$B$122</definedName>
-    <definedName name="spreader_speed" localSheetId="5">'Mach 1'!$B$118</definedName>
-    <definedName name="spreader_width" localSheetId="5">'Mach 1'!$A$105:$B$112</definedName>
-    <definedName name="stubble_fuel_consumption" localSheetId="5">'Mach 1'!$B$125</definedName>
-    <definedName name="stubble_maint" localSheetId="5">'Mach 1'!$B$127</definedName>
+    <definedName name="sprayer_eff" localSheetId="5">'Mach 1'!$B$103</definedName>
+    <definedName name="sprayer_fuel_consumption" localSheetId="5">'Mach 1'!$B$105</definedName>
+    <definedName name="sprayer_maint" localSheetId="5">'Mach 1'!$B$107</definedName>
+    <definedName name="sprayer_speed" localSheetId="5">'Mach 1'!$B$101</definedName>
+    <definedName name="sprayer_width" localSheetId="5">'Mach 1'!$B$99</definedName>
+    <definedName name="spreader_cap" localSheetId="5">'Mach 1'!$B$121</definedName>
+    <definedName name="spreader_eff" localSheetId="5">'Mach 1'!$B$127</definedName>
+    <definedName name="spreader_fuel" localSheetId="5">'Mach 1'!$B$110</definedName>
+    <definedName name="spreader_maint" localSheetId="5">'Mach 1'!$B$129</definedName>
+    <definedName name="spreader_speed" localSheetId="5">'Mach 1'!$B$125</definedName>
+    <definedName name="spreader_width" localSheetId="5">'Mach 1'!$A$112:$B$119</definedName>
+    <definedName name="stubble_fuel_consumption" localSheetId="5">'Mach 1'!$B$132</definedName>
+    <definedName name="stubble_maint" localSheetId="5">'Mach 1'!$B$134</definedName>
     <definedName name="sup_cartage">Price!$B$29</definedName>
-    <definedName name="sup_feed">'Mach 1'!$A$130:$C$135</definedName>
+    <definedName name="sup_feed">'Mach 1'!$A$137:$C$142</definedName>
     <definedName name="sup_md_vol">'Sup Feed'!$I$10:$N$14</definedName>
     <definedName name="sup_transaction">Price!$B$31</definedName>
     <definedName name="tillage_maint" localSheetId="5">'Mach 1'!$B$39</definedName>
-    <definedName name="time_fill_spreader" localSheetId="5">'Mach 1'!$B$116</definedName>
+    <definedName name="time_fill_spreader" localSheetId="5">'Mach 1'!$B$123</definedName>
     <definedName name="variable_dep" localSheetId="1">Finance!#REF!</definedName>
     <definedName name="variable_dep" localSheetId="5">'Mach 1'!$B$5</definedName>
     <definedName name="weed_control_bnds">'[1]Crop Sim'!$H$54:$M$70</definedName>
@@ -1505,11 +1505,11 @@
           </rPr>
           <t xml:space="preserve">
 seeding speed of other crops relative to wheat (wheat should be 1)
-</t>
+Note - cont pasture needs to be included here if resown</t>
         </r>
       </text>
     </comment>
-    <comment ref="A59" authorId="0" shapeId="0" xr:uid="{EB3EC863-815A-4F07-ADF1-BACEDBEA528E}">
+    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{EB3EC863-815A-4F07-ADF1-BACEDBEA528E}">
       <text>
         <r>
           <rPr>
@@ -1533,7 +1533,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A61" authorId="0" shapeId="0" xr:uid="{3377AFBB-BAF8-4184-9D43-0D43F3CF0BCD}">
+    <comment ref="A68" authorId="0" shapeId="0" xr:uid="{3377AFBB-BAF8-4184-9D43-0D43F3CF0BCD}">
       <text>
         <r>
           <rPr>
@@ -1557,7 +1557,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B61" authorId="0" shapeId="0" xr:uid="{8F650DD9-B6D6-4B19-A197-CD333C815375}">
+    <comment ref="B68" authorId="0" shapeId="0" xr:uid="{8F650DD9-B6D6-4B19-A197-CD333C815375}">
       <text>
         <r>
           <rPr>
@@ -1582,7 +1582,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A63" authorId="0" shapeId="0" xr:uid="{1F923DBF-9E7F-4464-8708-2B0AF1340A76}">
+    <comment ref="A70" authorId="0" shapeId="0" xr:uid="{1F923DBF-9E7F-4464-8708-2B0AF1340A76}">
       <text>
         <r>
           <rPr>
@@ -1606,7 +1606,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A65" authorId="0" shapeId="0" xr:uid="{925041D9-BB4A-4730-BA16-A60ED3E49090}">
+    <comment ref="A72" authorId="0" shapeId="0" xr:uid="{925041D9-BB4A-4730-BA16-A60ED3E49090}">
       <text>
         <r>
           <rPr>
@@ -1630,7 +1630,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A67" authorId="0" shapeId="0" xr:uid="{83C78BD9-1F45-41C1-83A8-FF872B400F8F}">
+    <comment ref="A74" authorId="0" shapeId="0" xr:uid="{83C78BD9-1F45-41C1-83A8-FF872B400F8F}">
       <text>
         <r>
           <rPr>
@@ -1655,7 +1655,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A79" authorId="0" shapeId="0" xr:uid="{03C07A35-AAEB-46EF-9545-55B9E522D28F}">
+    <comment ref="A86" authorId="0" shapeId="0" xr:uid="{03C07A35-AAEB-46EF-9545-55B9E522D28F}">
       <text>
         <r>
           <rPr>
@@ -1680,7 +1680,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A92" authorId="0" shapeId="0" xr:uid="{821E0CE2-6A9B-42C2-9F86-0C81A466AB82}">
+    <comment ref="A99" authorId="0" shapeId="0" xr:uid="{821E0CE2-6A9B-42C2-9F86-0C81A466AB82}">
       <text>
         <r>
           <rPr>
@@ -1704,7 +1704,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A94" authorId="0" shapeId="0" xr:uid="{D25B8429-9410-44C7-8574-A6DC0E08A456}">
+    <comment ref="A101" authorId="0" shapeId="0" xr:uid="{D25B8429-9410-44C7-8574-A6DC0E08A456}">
       <text>
         <r>
           <rPr>
@@ -1728,7 +1728,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A96" authorId="0" shapeId="0" xr:uid="{BB9ACD3C-8B60-44E6-911C-6ADC9B17BEE9}">
+    <comment ref="A103" authorId="0" shapeId="0" xr:uid="{BB9ACD3C-8B60-44E6-911C-6ADC9B17BEE9}">
       <text>
         <r>
           <rPr>
@@ -1752,7 +1752,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A98" authorId="0" shapeId="0" xr:uid="{8AE1C4AE-C9A6-42B8-87F4-4B73EC5E1B5E}">
+    <comment ref="A105" authorId="0" shapeId="0" xr:uid="{8AE1C4AE-C9A6-42B8-87F4-4B73EC5E1B5E}">
       <text>
         <r>
           <rPr>
@@ -1776,7 +1776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A100" authorId="0" shapeId="0" xr:uid="{64BD9D49-D5FD-46A7-90EB-ABA6BC4DD5BF}">
+    <comment ref="A107" authorId="0" shapeId="0" xr:uid="{64BD9D49-D5FD-46A7-90EB-ABA6BC4DD5BF}">
       <text>
         <r>
           <rPr>
@@ -1800,7 +1800,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A103" authorId="0" shapeId="0" xr:uid="{B3CC4513-8BFF-4910-ABF7-F746405E57E7}">
+    <comment ref="A110" authorId="0" shapeId="0" xr:uid="{B3CC4513-8BFF-4910-ABF7-F746405E57E7}">
       <text>
         <r>
           <rPr>
@@ -1824,7 +1824,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A105" authorId="0" shapeId="0" xr:uid="{4922BC00-7562-4251-AF4D-B71E622B07C0}">
+    <comment ref="A112" authorId="0" shapeId="0" xr:uid="{4922BC00-7562-4251-AF4D-B71E622B07C0}">
       <text>
         <r>
           <rPr>
@@ -1849,7 +1849,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A114" authorId="0" shapeId="0" xr:uid="{22E62F09-30E0-4CD0-81DE-F02394555AD3}">
+    <comment ref="A121" authorId="0" shapeId="0" xr:uid="{22E62F09-30E0-4CD0-81DE-F02394555AD3}">
       <text>
         <r>
           <rPr>
@@ -1873,7 +1873,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A116" authorId="0" shapeId="0" xr:uid="{AF9CD173-26D1-4803-84AA-A1C88C31B999}">
+    <comment ref="A123" authorId="0" shapeId="0" xr:uid="{AF9CD173-26D1-4803-84AA-A1C88C31B999}">
       <text>
         <r>
           <rPr>
@@ -1897,7 +1897,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A118" authorId="0" shapeId="0" xr:uid="{B466F8A9-62FF-4035-B41F-6123131A64B2}">
+    <comment ref="A125" authorId="0" shapeId="0" xr:uid="{B466F8A9-62FF-4035-B41F-6123131A64B2}">
       <text>
         <r>
           <rPr>
@@ -1921,7 +1921,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A120" authorId="0" shapeId="0" xr:uid="{D36EEB6F-4421-421C-BD2B-38C8EED80323}">
+    <comment ref="A127" authorId="0" shapeId="0" xr:uid="{D36EEB6F-4421-421C-BD2B-38C8EED80323}">
       <text>
         <r>
           <rPr>
@@ -1945,7 +1945,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A122" authorId="0" shapeId="0" xr:uid="{476F3EA8-18FE-4BF1-857E-DB0233D5DFAB}">
+    <comment ref="A129" authorId="0" shapeId="0" xr:uid="{476F3EA8-18FE-4BF1-857E-DB0233D5DFAB}">
       <text>
         <r>
           <rPr>
@@ -1969,7 +1969,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A125" authorId="0" shapeId="0" xr:uid="{9163A97B-97F8-4781-A636-98B9A4B8C98E}">
+    <comment ref="A132" authorId="0" shapeId="0" xr:uid="{9163A97B-97F8-4781-A636-98B9A4B8C98E}">
       <text>
         <r>
           <rPr>
@@ -1993,7 +1993,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A127" authorId="0" shapeId="0" xr:uid="{30ECEA2E-A5CE-459D-8EC2-C4E59BCFCA95}">
+    <comment ref="A134" authorId="0" shapeId="0" xr:uid="{30ECEA2E-A5CE-459D-8EC2-C4E59BCFCA95}">
       <text>
         <r>
           <rPr>
@@ -2017,7 +2017,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B130" authorId="0" shapeId="0" xr:uid="{115DEECC-C4B6-40BD-AC87-F415E26BB0BB}">
+    <comment ref="B137" authorId="0" shapeId="0" xr:uid="{115DEECC-C4B6-40BD-AC87-F415E26BB0BB}">
       <text>
         <r>
           <rPr>
@@ -2041,7 +2041,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C130" authorId="0" shapeId="0" xr:uid="{735B890C-028D-403F-91EB-7DDBBB95923A}">
+    <comment ref="C137" authorId="0" shapeId="0" xr:uid="{735B890C-028D-403F-91EB-7DDBBB95923A}">
       <text>
         <r>
           <rPr>
@@ -2070,7 +2070,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="179">
   <si>
     <t>Machinery</t>
   </si>
@@ -2462,15 +2462,6 @@
     <t>casual_workers_comp</t>
   </si>
   <si>
-    <t>annual</t>
-  </si>
-  <si>
-    <t>tedera</t>
-  </si>
-  <si>
-    <t>lucerne</t>
-  </si>
-  <si>
     <t>insurance date</t>
   </si>
   <si>
@@ -2586,6 +2577,36 @@
   </si>
   <si>
     <t>Equipment insurance rate</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>sr</t>
+  </si>
+  <si>
+    <t>tr</t>
+  </si>
+  <si>
+    <t>jr</t>
+  </si>
+  <si>
+    <t>tc</t>
+  </si>
+  <si>
+    <t>jc</t>
+  </si>
+  <si>
+    <t>ur</t>
+  </si>
+  <si>
+    <t>xr</t>
+  </si>
+  <si>
+    <t>uc</t>
+  </si>
+  <si>
+    <t>xc</t>
   </si>
 </sst>
 </file>
@@ -6406,26 +6427,26 @@
       <selection activeCell="A74" sqref="A74:XFD84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -6436,8 +6457,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -6448,13 +6469,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -6462,7 +6483,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -6470,7 +6491,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -6478,7 +6499,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -6486,7 +6507,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -6494,7 +6515,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -6502,7 +6523,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
@@ -6510,7 +6531,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>95</v>
       </c>
@@ -6518,7 +6539,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>96</v>
       </c>
@@ -6526,7 +6547,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>97</v>
       </c>
@@ -6534,7 +6555,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
@@ -6545,13 +6566,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
@@ -6562,8 +6583,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
@@ -6574,8 +6595,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -6586,37 +6607,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B29" s="8">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="6.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B31" s="8">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>102</v>
       </c>
@@ -6624,7 +6645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>103</v>
       </c>
@@ -6632,8 +6653,8 @@
         <v>43814</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>104</v>
       </c>
@@ -6641,16 +6662,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B40" s="6">
         <v>43692</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>91</v>
       </c>
@@ -6676,9 +6697,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="46" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B43" s="47">
         <f>AVERAGE(B49,B51,B59)</f>
@@ -6709,9 +6730,9 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B44" s="47">
         <f>AVERAGE(B57,B60)</f>
@@ -6742,9 +6763,9 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="46" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B45" s="47">
         <f>AVERAGE(B50,B52:B54,B58)</f>
@@ -6775,9 +6796,9 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="46" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B46" s="47">
         <f>AVERAGE(B49:B60)</f>
@@ -6808,10 +6829,10 @@
         <v>0.93800000000000028</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>91</v>
       </c>
@@ -6837,7 +6858,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>4</v>
       </c>
@@ -6865,7 +6886,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>10</v>
       </c>
@@ -6893,7 +6914,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>94</v>
       </c>
@@ -6921,7 +6942,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>95</v>
       </c>
@@ -6949,7 +6970,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>96</v>
       </c>
@@ -6977,7 +6998,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -7005,7 +7026,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>6</v>
       </c>
@@ -7033,7 +7054,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>119</v>
       </c>
@@ -7060,7 +7081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>9</v>
       </c>
@@ -7088,7 +7109,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>97</v>
       </c>
@@ -7116,7 +7137,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>5</v>
       </c>
@@ -7144,7 +7165,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>8</v>
       </c>
@@ -7172,12 +7193,12 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>116</v>
       </c>
@@ -7185,10 +7206,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="9.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>112</v>
       </c>
@@ -7196,7 +7217,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>68</v>
       </c>
@@ -7204,7 +7225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>67</v>
       </c>
@@ -7212,7 +7233,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>66</v>
       </c>
@@ -7220,7 +7241,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>114</v>
       </c>
@@ -7228,7 +7249,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>63</v>
       </c>
@@ -7236,15 +7257,15 @@
         <v>550</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B71" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>65</v>
       </c>
@@ -7252,12 +7273,12 @@
         <v>520</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>122</v>
       </c>
@@ -7265,7 +7286,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>123</v>
       </c>
@@ -7273,7 +7294,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>124</v>
       </c>
@@ -7281,7 +7302,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>125</v>
       </c>
@@ -7289,7 +7310,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>126</v>
       </c>
@@ -7297,7 +7318,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>127</v>
       </c>
@@ -7305,7 +7326,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>128</v>
       </c>
@@ -7313,7 +7334,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>129</v>
       </c>
@@ -7337,18 +7358,18 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.81640625" style="1"/>
+    <col min="2" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -7356,8 +7377,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -7365,38 +7386,38 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B8" s="49">
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B11" s="49">
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
@@ -7404,14 +7425,14 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B17" s="49">
         <v>0.02</v>
@@ -7431,23 +7452,23 @@
       <selection activeCell="A15" sqref="A15:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="2" style="1" customWidth="1"/>
-    <col min="3" max="3" width="0.1796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="2.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="1.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.26953125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="1"/>
+    <col min="3" max="3" width="0.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="1.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G2" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G3" s="5" t="s">
         <v>111</v>
       </c>
@@ -7455,10 +7476,10 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="7:8" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="7:8" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G5" s="4" t="s">
         <v>105</v>
       </c>
@@ -7466,8 +7487,8 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G7" s="4" t="s">
         <v>106</v>
       </c>
@@ -7475,8 +7496,8 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="8" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G9" s="4" t="s">
         <v>107</v>
       </c>
@@ -7484,8 +7505,8 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="10" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G11" s="4" t="s">
         <v>108</v>
       </c>
@@ -7493,8 +7514,8 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="12" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G13" s="4" t="s">
         <v>109</v>
       </c>
@@ -7512,20 +7533,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBAE29A-401D-4B75-B63C-3693AC93217E}">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14:N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.453125" customWidth="1"/>
-    <col min="2" max="2" width="2.26953125" customWidth="1"/>
-    <col min="3" max="4" width="2.7265625" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="2.28515625" customWidth="1"/>
+    <col min="3" max="4" width="2.7109375" customWidth="1"/>
     <col min="5" max="5" width="2" customWidth="1"/>
-    <col min="6" max="6" width="4.1796875" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -7553,7 +7574,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="12"/>
     </row>
-    <row r="2" spans="1:26" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -7581,11 +7602,11 @@
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
     </row>
-    <row r="3" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="14" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -7611,17 +7632,17 @@
       <c r="Y3" s="13"/>
       <c r="Z3" s="13"/>
     </row>
-    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
@@ -7643,7 +7664,7 @@
       <c r="Y4" s="13"/>
       <c r="Z4" s="13"/>
     </row>
-    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="17"/>
@@ -7651,7 +7672,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
@@ -7673,7 +7694,7 @@
       <c r="Y5" s="13"/>
       <c r="Z5" s="13"/>
     </row>
-    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="22"/>
@@ -7703,7 +7724,7 @@
       <c r="Y6" s="13"/>
       <c r="Z6" s="13"/>
     </row>
-    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="22"/>
@@ -7731,7 +7752,7 @@
       <c r="Y7" s="13"/>
       <c r="Z7" s="13"/>
     </row>
-    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="22"/>
@@ -7759,7 +7780,7 @@
       <c r="Y8" s="13"/>
       <c r="Z8" s="13"/>
     </row>
-    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="22"/>
@@ -7787,7 +7808,7 @@
       <c r="Y9" s="13"/>
       <c r="Z9" s="13"/>
     </row>
-    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="22"/>
@@ -7825,7 +7846,7 @@
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
     </row>
-    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="22"/>
@@ -7834,7 +7855,7 @@
       <c r="F11" s="28"/>
       <c r="H11" s="32"/>
       <c r="I11" s="45" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J11" s="33">
         <v>11400</v>
@@ -7852,7 +7873,7 @@
         <v>7000</v>
       </c>
       <c r="O11" s="32" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="P11" s="34"/>
       <c r="Q11" s="34"/>
@@ -7866,7 +7887,7 @@
       <c r="Y11" s="13"/>
       <c r="Z11" s="13"/>
     </row>
-    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="22"/>
@@ -7875,7 +7896,7 @@
       <c r="F12" s="28"/>
       <c r="H12" s="32"/>
       <c r="I12" s="45" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J12" s="33">
         <v>0.1</v>
@@ -7905,7 +7926,7 @@
       <c r="Y12" s="13"/>
       <c r="Z12" s="13"/>
     </row>
-    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="22"/>
@@ -7914,7 +7935,7 @@
       <c r="F13" s="28"/>
       <c r="H13" s="32"/>
       <c r="I13" s="45" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J13" s="50">
         <v>0.9</v>
@@ -7932,7 +7953,7 @@
         <v>0.9</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="P13" s="34"/>
       <c r="Q13" s="34"/>
@@ -7946,7 +7967,7 @@
       <c r="Y13" s="13"/>
       <c r="Z13" s="13"/>
     </row>
-    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="12"/>
       <c r="C14" s="22"/>
@@ -7955,7 +7976,7 @@
       <c r="F14" s="28"/>
       <c r="H14" s="32"/>
       <c r="I14" s="45" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="J14" s="50">
         <v>0.8</v>
@@ -7973,7 +7994,7 @@
         <v>0.75</v>
       </c>
       <c r="O14" s="32" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="P14" s="34"/>
       <c r="Q14" s="34"/>
@@ -7987,7 +8008,7 @@
       <c r="Y14" s="13"/>
       <c r="Z14" s="13"/>
     </row>
-    <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="C15" s="22"/>
@@ -8015,7 +8036,7 @@
       <c r="Y15" s="13"/>
       <c r="Z15" s="13"/>
     </row>
-    <row r="16" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="22"/>
@@ -8043,7 +8064,7 @@
       <c r="Y16" s="13"/>
       <c r="Z16" s="13"/>
     </row>
-    <row r="17" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="C17" s="40"/>
@@ -8070,13 +8091,13 @@
       <c r="U17" s="40"/>
       <c r="V17" s="40"/>
       <c r="W17" s="42" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
       <c r="Z17" s="13"/>
     </row>
-    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -8104,7 +8125,7 @@
       <c r="Y18" s="13"/>
       <c r="Z18" s="13"/>
     </row>
-    <row r="19" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -8132,11 +8153,11 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="14" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
@@ -8162,17 +8183,17 @@
       <c r="Y20" s="13"/>
       <c r="Z20" s="13"/>
     </row>
-    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="19" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
@@ -8194,7 +8215,7 @@
       <c r="Y21" s="13"/>
       <c r="Z21" s="13"/>
     </row>
-    <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="17"/>
@@ -8202,7 +8223,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
@@ -8224,7 +8245,7 @@
       <c r="Y22" s="13"/>
       <c r="Z22" s="13"/>
     </row>
-    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="12"/>
       <c r="C23" s="22"/>
@@ -8254,7 +8275,7 @@
       <c r="Y23" s="13"/>
       <c r="Z23" s="13"/>
     </row>
-    <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="22"/>
@@ -8282,7 +8303,7 @@
       <c r="Y24" s="13"/>
       <c r="Z24" s="13"/>
     </row>
-    <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="C25" s="22"/>
@@ -8310,7 +8331,7 @@
       <c r="Y25" s="13"/>
       <c r="Z25" s="13"/>
     </row>
-    <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="22"/>
@@ -8320,7 +8341,7 @@
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J26" s="26" t="s">
         <v>6</v>
@@ -8350,7 +8371,7 @@
       <c r="Y26" s="13"/>
       <c r="Z26" s="13"/>
     </row>
-    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="22"/>
@@ -8360,22 +8381,22 @@
       <c r="G27" s="29"/>
       <c r="H27" s="29"/>
       <c r="I27" s="29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="J27" s="30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="K27" s="30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="L27" s="30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="M27" s="30" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="N27" s="30" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="O27" s="30"/>
       <c r="P27" s="30"/>
@@ -8390,7 +8411,7 @@
       <c r="Y27" s="13"/>
       <c r="Z27" s="13"/>
     </row>
-    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="22"/>
@@ -8399,7 +8420,7 @@
       <c r="F28" s="28"/>
       <c r="H28" s="32"/>
       <c r="I28" s="45" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J28" s="44">
         <v>0.45</v>
@@ -8417,7 +8438,7 @@
         <v>1</v>
       </c>
       <c r="O28" s="32" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="P28" s="34"/>
       <c r="Q28" s="34"/>
@@ -8431,7 +8452,7 @@
       <c r="Y28" s="13"/>
       <c r="Z28" s="13"/>
     </row>
-    <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="22"/>
@@ -8459,7 +8480,7 @@
       <c r="Y29" s="13"/>
       <c r="Z29" s="13"/>
     </row>
-    <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="22"/>
@@ -8487,7 +8508,7 @@
       <c r="Y30" s="13"/>
       <c r="Z30" s="13"/>
     </row>
-    <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
       <c r="C31" s="40"/>
@@ -8514,13 +8535,13 @@
       <c r="U31" s="40"/>
       <c r="V31" s="40"/>
       <c r="W31" s="42" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="X31" s="13"/>
       <c r="Y31" s="13"/>
       <c r="Z31" s="13"/>
     </row>
-    <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -8563,19 +8584,19 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>89</v>
       </c>
@@ -8583,21 +8604,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="9.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -8605,7 +8626,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -8613,7 +8634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -8621,7 +8642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -8629,7 +8650,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -8637,7 +8658,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -8645,7 +8666,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -8653,7 +8674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>95</v>
       </c>
@@ -8661,7 +8682,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>96</v>
       </c>
@@ -8669,7 +8690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>97</v>
       </c>
@@ -8677,12 +8698,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>83</v>
       </c>
@@ -8690,8 +8711,8 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>87</v>
       </c>
@@ -8699,14 +8720,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
@@ -8714,7 +8735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>4</v>
       </c>
@@ -8722,7 +8743,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>6</v>
       </c>
@@ -8730,7 +8751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
@@ -8738,7 +8759,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
@@ -8746,7 +8767,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
@@ -8754,7 +8775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>10</v>
       </c>
@@ -8762,7 +8783,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>95</v>
       </c>
@@ -8770,7 +8791,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>96</v>
       </c>
@@ -8778,7 +8799,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>97</v>
       </c>
@@ -8786,9 +8807,9 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B35" s="6">
         <v>43554</v>
@@ -8804,25 +8825,25 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A689975D-2450-4766-909D-59787FB65B03}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A2:C135"/>
+  <dimension ref="A2:C142"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="19.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -8833,8 +8854,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
@@ -8843,12 +8864,12 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>117</v>
       </c>
@@ -8856,7 +8877,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -8864,7 +8885,7 @@
         <v>188000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
@@ -8872,7 +8893,7 @@
         <v>87000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
@@ -8880,7 +8901,7 @@
         <v>297000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
@@ -8888,7 +8909,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
@@ -8896,7 +8917,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -8904,7 +8925,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
@@ -8912,7 +8933,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
@@ -8920,7 +8941,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
@@ -8928,7 +8949,7 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
@@ -8936,7 +8957,7 @@
         <v>78000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>37</v>
       </c>
@@ -8944,7 +8965,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
@@ -8952,7 +8973,7 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
@@ -8960,12 +8981,12 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
@@ -8973,8 +8994,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>41</v>
       </c>
@@ -8982,12 +9003,12 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>43</v>
       </c>
@@ -8995,8 +9016,8 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
@@ -9004,8 +9025,8 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>77</v>
       </c>
@@ -9013,8 +9034,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -9022,8 +9043,8 @@
         <v>5.41</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -9031,8 +9052,8 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -9040,600 +9061,656 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>130</v>
+        <v>169</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>131</v>
+        <v>170</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>132</v>
+        <v>171</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>5</v>
+        <v>172</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>94</v>
+        <v>175</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
       <c r="B49" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>8</v>
+        <v>177</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>9</v>
+        <v>178</v>
       </c>
       <c r="B51" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B52" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B53" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>95</v>
+        <v>6</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B55" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="B56" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="3" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B61" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B63" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="4" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B59" s="4">
+      <c r="B66" s="4">
         <v>12.2</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="4" t="s">
+    <row r="67" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B61" s="4">
+      <c r="B68" s="4">
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="4" t="s">
+    <row r="69" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B63" s="4">
+      <c r="B70" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="4" t="s">
+    <row r="71" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B72" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" s="4" t="s">
+    <row r="73" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B67" s="4"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" s="4" t="s">
+      <c r="B74" s="4"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B68" s="4">
+      <c r="B75" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" s="4" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B76" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" s="4" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B70" s="4">
+      <c r="B77" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" s="4" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B71" s="4">
+      <c r="B78" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" s="4" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B72" s="4">
+      <c r="B79" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" s="4" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B73" s="4">
+      <c r="B80" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" s="4" t="s">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B74" s="4">
+      <c r="B81" s="4">
         <v>5.5</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" s="4" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B75" s="4">
+      <c r="B82" s="4">
         <v>5.5</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" s="4" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B76" s="4">
+      <c r="B83" s="4">
         <v>5.5</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" s="4" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B77" s="4">
+      <c r="B84" s="4">
         <v>5.5</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79" s="4" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B79" s="4"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80" s="4" t="s">
+      <c r="B86" s="4"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B80" s="4">
+      <c r="B87" s="4">
         <v>33</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" s="4" t="s">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B81" s="4">
+      <c r="B88" s="4">
         <v>33</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" s="4" t="s">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B82" s="4">
+      <c r="B89" s="4">
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" s="4" t="s">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B83" s="4">
+      <c r="B90" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="4" t="s">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B84" s="4">
+      <c r="B91" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" s="4" t="s">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="4">
+      <c r="B92" s="4">
         <v>33</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" s="4" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B86" s="4">
+      <c r="B93" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" s="4" t="s">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B87" s="4">
+      <c r="B94" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" s="4" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B88" s="4">
+      <c r="B95" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" s="4" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B89" s="4">
+      <c r="B96" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" s="3" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" s="4" t="s">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B92" s="4">
+      <c r="B99" s="4">
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="4" t="s">
+    <row r="100" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B94" s="4">
+      <c r="B101" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" s="4" t="s">
+    <row r="102" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B96" s="4">
+      <c r="B103" s="4">
         <v>0.6</v>
       </c>
     </row>
-    <row r="97" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" s="4" t="s">
+    <row r="104" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B98" s="4">
+      <c r="B105" s="4">
         <v>0.6</v>
       </c>
     </row>
-    <row r="99" spans="1:2" ht="3" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" s="4" t="s">
+    <row r="106" spans="1:2" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B100" s="4">
+      <c r="B107" s="4">
         <v>1.3</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" s="3" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" s="4" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B103" s="4">
+      <c r="B110" s="4">
         <v>11.3</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" s="4" t="s">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B105" s="4"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" s="4" t="s">
+      <c r="B112" s="4"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B106" s="4">
+      <c r="B113" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" s="4" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B107" s="4"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" s="4" t="s">
+      <c r="B114" s="4"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B108" s="4">
+      <c r="B115" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" s="4" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B109" s="4">
+      <c r="B116" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" s="4" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B110" s="4">
+      <c r="B117" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" s="4" t="s">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="B111" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B112" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="B114" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B116" s="4">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="B118" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="5.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" s="4" t="s">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B119" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B121" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B123" s="4">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B125" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B120" s="4">
+      <c r="B127" s="4">
         <v>0.3</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" s="4" t="s">
+    <row r="128" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B122" s="4">
+      <c r="B129" s="4">
         <v>14.3</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" s="3" t="s">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" s="4" t="s">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B125" s="4">
+      <c r="B132" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" s="4" t="s">
+    <row r="133" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B127" s="4">
+      <c r="B134" s="4">
         <v>1.3</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A129" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A130" s="8"/>
-      <c r="B130" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C130" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A131" s="9" t="s">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="8"/>
+      <c r="B137" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="C137" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B131" s="8">
+      <c r="B138" s="8">
         <v>1</v>
       </c>
-      <c r="C131" s="8">
+      <c r="C138" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A132" s="9" t="s">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B132" s="8">
+      <c r="B139" s="8">
         <v>1</v>
       </c>
-      <c r="C132" s="8">
+      <c r="C139" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A133" s="9" t="s">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B133" s="8">
+      <c r="B140" s="8">
         <v>1</v>
       </c>
-      <c r="C133" s="8">
+      <c r="C140" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A134" s="9" t="s">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B134" s="8">
+      <c r="B141" s="8">
         <v>1</v>
       </c>
-      <c r="C134" s="8">
+      <c r="C141" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A135" s="9" t="s">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B135" s="8">
+      <c r="B142" s="8">
         <v>1</v>
       </c>
-      <c r="C135" s="8">
+      <c r="C142" s="8">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reporting fix pas mask
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28C50C5F-607E-411D-8240-065738270651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B77CC8-7E43-4FA9-8951-963A38663CD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -593,31 +593,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="A56" authorId="0" shapeId="0" xr:uid="{1F236855-DB12-4A56-81DF-9D55DDDB3E64}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Michael Young:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-a value is needed for the crop sim.
--currently fodder is not sold, therefore this value is dropped in the grain price section</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="A63" authorId="0" shapeId="0" xr:uid="{A067DE07-A282-4047-AC13-801EB51C2DD0}">
       <text>
         <r>
@@ -2070,7 +2045,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="180">
   <si>
     <t>Machinery</t>
   </si>
@@ -2607,6 +2582,9 @@
   </si>
   <si>
     <t>xc</t>
+  </si>
+  <si>
+    <t>*not used, can probs remove</t>
   </si>
 </sst>
 </file>
@@ -2618,7 +2596,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2683,6 +2661,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2878,7 +2869,7 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2973,17 +2964,21 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="9" borderId="9" xfId="2">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="9" borderId="9" xfId="2" applyNumberFormat="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="5" fillId="8" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="9" borderId="9" xfId="2" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="9" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Formula 1" xfId="2" xr:uid="{73E7623B-26A4-407F-9297-1EB699330B2D}"/>
@@ -6421,32 +6416,32 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF2F00E-8A84-429F-9A28-0BBAA9C21CDC}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:XFD84"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -6457,8 +6452,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -6469,13 +6464,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -6483,7 +6478,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -6491,7 +6486,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -6499,7 +6494,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -6507,7 +6502,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -6515,7 +6510,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -6523,7 +6518,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
@@ -6531,7 +6526,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>95</v>
       </c>
@@ -6539,7 +6534,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>96</v>
       </c>
@@ -6547,7 +6542,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>97</v>
       </c>
@@ -6555,7 +6550,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
@@ -6566,13 +6561,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
@@ -6583,8 +6578,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
@@ -6595,8 +6590,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -6607,12 +6602,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>133</v>
       </c>
@@ -6620,10 +6615,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="6.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>132</v>
       </c>
@@ -6631,13 +6626,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>102</v>
       </c>
@@ -6645,7 +6640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>103</v>
       </c>
@@ -6653,8 +6648,8 @@
         <v>43814</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>104</v>
       </c>
@@ -6662,8 +6657,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>130</v>
       </c>
@@ -6671,168 +6666,171 @@
         <v>43692</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="F42" s="4" t="s">
+      <c r="F42" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="G42" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="H42" s="4" t="s">
+      <c r="H42" s="49" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="46" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="50" t="s">
         <v>163</v>
       </c>
-      <c r="B43" s="47">
+      <c r="B43" s="51">
         <f>AVERAGE(B49,B51,B59)</f>
         <v>246.66666666666666</v>
       </c>
-      <c r="C43" s="47">
+      <c r="C43" s="51">
         <f t="shared" ref="C43:H43" si="0">AVERAGE(C49,C51,C59)</f>
         <v>231.66666666666666</v>
       </c>
-      <c r="D43" s="48">
+      <c r="D43" s="52">
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="E43" s="48">
+      <c r="E43" s="52">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="F43" s="47">
+      <c r="F43" s="51">
         <f t="shared" si="0"/>
         <v>0.26666666666666666</v>
       </c>
-      <c r="G43" s="47">
+      <c r="G43" s="51">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H43" s="47">
+      <c r="H43" s="51">
         <f t="shared" si="0"/>
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="46" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="B44" s="47">
+      <c r="B44" s="51">
         <f>AVERAGE(B57,B60)</f>
         <v>550</v>
       </c>
-      <c r="C44" s="47">
+      <c r="C44" s="51">
         <f t="shared" ref="C44:H44" si="1">AVERAGE(C57,C60)</f>
         <v>550</v>
       </c>
-      <c r="D44" s="48">
+      <c r="D44" s="52">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E44" s="48">
+      <c r="E44" s="52">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F44" s="47">
+      <c r="F44" s="51">
         <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
-      <c r="G44" s="47">
+      <c r="G44" s="51">
         <f t="shared" si="1"/>
         <v>21.95</v>
       </c>
-      <c r="H44" s="47">
+      <c r="H44" s="51">
         <f t="shared" si="1"/>
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="46" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="B45" s="47">
+      <c r="B45" s="51">
         <f>AVERAGE(B50,B52:B54,B58)</f>
         <v>341</v>
       </c>
-      <c r="C45" s="47">
+      <c r="C45" s="51">
         <f t="shared" ref="C45:H45" si="2">AVERAGE(C50,C52:C54,C58)</f>
         <v>341</v>
       </c>
-      <c r="D45" s="48">
+      <c r="D45" s="52">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E45" s="48">
+      <c r="E45" s="52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F45" s="47">
+      <c r="F45" s="51">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="G45" s="47">
+      <c r="G45" s="51">
         <f t="shared" si="2"/>
         <v>15.089999999999998</v>
       </c>
-      <c r="H45" s="47">
+      <c r="H45" s="51">
         <f t="shared" si="2"/>
         <v>1.0920000000000001</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="46" t="s">
+      <c r="I45" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="50" t="s">
         <v>165</v>
       </c>
-      <c r="B46" s="47">
+      <c r="B46" s="51">
         <f>AVERAGE(B49:B60)</f>
-        <v>319.16666666666669</v>
-      </c>
-      <c r="C46" s="47">
+        <v>315</v>
+      </c>
+      <c r="C46" s="51">
         <f t="shared" ref="C46:H46" si="3">AVERAGE(C49:C60)</f>
-        <v>315.41666666666669</v>
-      </c>
-      <c r="D46" s="48">
+        <v>311.25</v>
+      </c>
+      <c r="D46" s="52">
         <f>AVERAGE(D49:D60)</f>
         <v>0.95833333333333337</v>
       </c>
-      <c r="E46" s="48">
+      <c r="E46" s="52">
         <f t="shared" si="3"/>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F46" s="47">
+      <c r="F46" s="51">
         <f t="shared" si="3"/>
         <v>0.16166666666666665</v>
       </c>
-      <c r="G46" s="47">
+      <c r="G46" s="51">
         <f t="shared" si="3"/>
         <v>13.266666666666666</v>
       </c>
-      <c r="H46" s="47">
+      <c r="H46" s="51">
         <f t="shared" si="3"/>
         <v>0.93800000000000028</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>91</v>
       </c>
@@ -6858,7 +6856,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>4</v>
       </c>
@@ -6871,7 +6869,7 @@
       <c r="D49" s="4">
         <v>0.7</v>
       </c>
-      <c r="E49" s="47">
+      <c r="E49" s="46">
         <f t="shared" ref="E49:E58" si="4">1-D49</f>
         <v>0.30000000000000004</v>
       </c>
@@ -6886,7 +6884,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>10</v>
       </c>
@@ -6899,7 +6897,7 @@
       <c r="D50" s="4">
         <v>1</v>
       </c>
-      <c r="E50" s="47">
+      <c r="E50" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -6914,7 +6912,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>94</v>
       </c>
@@ -6927,7 +6925,7 @@
       <c r="D51" s="4">
         <v>1</v>
       </c>
-      <c r="E51" s="47">
+      <c r="E51" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -6942,7 +6940,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>95</v>
       </c>
@@ -6955,7 +6953,7 @@
       <c r="D52" s="4">
         <v>1</v>
       </c>
-      <c r="E52" s="47">
+      <c r="E52" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -6970,7 +6968,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>96</v>
       </c>
@@ -6983,7 +6981,7 @@
       <c r="D53" s="4">
         <v>1</v>
       </c>
-      <c r="E53" s="47">
+      <c r="E53" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -6998,7 +6996,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -7011,7 +7009,7 @@
       <c r="D54" s="4">
         <v>1</v>
       </c>
-      <c r="E54" s="47">
+      <c r="E54" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -7026,7 +7024,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>6</v>
       </c>
@@ -7039,7 +7037,7 @@
       <c r="D55" s="4">
         <v>1</v>
       </c>
-      <c r="E55" s="47">
+      <c r="E55" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -7054,20 +7052,20 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>119</v>
       </c>
       <c r="B56" s="4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C56" s="4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D56" s="4">
         <v>1</v>
       </c>
-      <c r="E56" s="47">
+      <c r="E56" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -7081,7 +7079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>9</v>
       </c>
@@ -7094,7 +7092,7 @@
       <c r="D57" s="4">
         <v>1</v>
       </c>
-      <c r="E57" s="47">
+      <c r="E57" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -7109,7 +7107,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>97</v>
       </c>
@@ -7122,7 +7120,7 @@
       <c r="D58" s="4">
         <v>1</v>
       </c>
-      <c r="E58" s="47">
+      <c r="E58" s="46">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -7137,7 +7135,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>5</v>
       </c>
@@ -7150,7 +7148,7 @@
       <c r="D59" s="4">
         <v>0.8</v>
       </c>
-      <c r="E59" s="47">
+      <c r="E59" s="46">
         <f t="shared" ref="E59:E60" si="6">1-D59</f>
         <v>0.19999999999999996</v>
       </c>
@@ -7165,7 +7163,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>8</v>
       </c>
@@ -7178,7 +7176,7 @@
       <c r="D60" s="4">
         <v>1</v>
       </c>
-      <c r="E60" s="47">
+      <c r="E60" s="46">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -7193,12 +7191,12 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>116</v>
       </c>
@@ -7206,10 +7204,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="9.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>112</v>
       </c>
@@ -7217,7 +7215,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>68</v>
       </c>
@@ -7225,7 +7223,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>67</v>
       </c>
@@ -7233,7 +7231,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>66</v>
       </c>
@@ -7241,7 +7239,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
         <v>114</v>
       </c>
@@ -7249,7 +7247,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>63</v>
       </c>
@@ -7257,7 +7255,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>166</v>
       </c>
@@ -7265,7 +7263,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>65</v>
       </c>
@@ -7273,12 +7271,12 @@
         <v>520</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>122</v>
       </c>
@@ -7286,7 +7284,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>123</v>
       </c>
@@ -7294,7 +7292,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>124</v>
       </c>
@@ -7302,7 +7300,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>125</v>
       </c>
@@ -7310,7 +7308,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>126</v>
       </c>
@@ -7318,7 +7316,7 @@
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>127</v>
       </c>
@@ -7326,7 +7324,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>128</v>
       </c>
@@ -7334,7 +7332,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>129</v>
       </c>
@@ -7358,83 +7356,83 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="49">
+      <c r="B3" s="47">
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="49">
+      <c r="B5" s="47">
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B8" s="49">
+      <c r="B8" s="47">
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B11" s="49">
+      <c r="B11" s="47">
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="49">
+      <c r="B14" s="47">
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B17" s="49">
+      <c r="B17" s="47">
         <v>0.02</v>
       </c>
     </row>
@@ -7452,23 +7450,23 @@
       <selection activeCell="A15" sqref="A15:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="2" style="1" customWidth="1"/>
-    <col min="3" max="3" width="0.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="2.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="1.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="0.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="1.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.26953125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G2" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G3" s="5" t="s">
         <v>111</v>
       </c>
@@ -7476,10 +7474,10 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="7:8" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="7:8" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G5" s="4" t="s">
         <v>105</v>
       </c>
@@ -7487,8 +7485,8 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G7" s="4" t="s">
         <v>106</v>
       </c>
@@ -7496,8 +7494,8 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="8" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G9" s="4" t="s">
         <v>107</v>
       </c>
@@ -7505,8 +7503,8 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="10" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G11" s="4" t="s">
         <v>108</v>
       </c>
@@ -7514,8 +7512,8 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="12" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G13" s="4" t="s">
         <v>109</v>
       </c>
@@ -7537,16 +7535,16 @@
       <selection activeCell="J14" sqref="J14:N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="2.28515625" customWidth="1"/>
-    <col min="3" max="4" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" customWidth="1"/>
+    <col min="2" max="2" width="2.26953125" customWidth="1"/>
+    <col min="3" max="4" width="2.7265625" customWidth="1"/>
     <col min="5" max="5" width="2" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="4.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -7574,7 +7572,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="12"/>
     </row>
-    <row r="2" spans="1:26" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -7602,7 +7600,7 @@
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
     </row>
-    <row r="3" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="14" t="s">
@@ -7632,7 +7630,7 @@
       <c r="Y3" s="13"/>
       <c r="Z3" s="13"/>
     </row>
-    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="17"/>
@@ -7664,7 +7662,7 @@
       <c r="Y4" s="13"/>
       <c r="Z4" s="13"/>
     </row>
-    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="17"/>
@@ -7694,7 +7692,7 @@
       <c r="Y5" s="13"/>
       <c r="Z5" s="13"/>
     </row>
-    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="22"/>
@@ -7724,7 +7722,7 @@
       <c r="Y6" s="13"/>
       <c r="Z6" s="13"/>
     </row>
-    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="22"/>
@@ -7752,7 +7750,7 @@
       <c r="Y7" s="13"/>
       <c r="Z7" s="13"/>
     </row>
-    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="22"/>
@@ -7780,7 +7778,7 @@
       <c r="Y8" s="13"/>
       <c r="Z8" s="13"/>
     </row>
-    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="22"/>
@@ -7808,7 +7806,7 @@
       <c r="Y9" s="13"/>
       <c r="Z9" s="13"/>
     </row>
-    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="22"/>
@@ -7846,7 +7844,7 @@
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
     </row>
-    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="22"/>
@@ -7887,7 +7885,7 @@
       <c r="Y11" s="13"/>
       <c r="Z11" s="13"/>
     </row>
-    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="22"/>
@@ -7926,7 +7924,7 @@
       <c r="Y12" s="13"/>
       <c r="Z12" s="13"/>
     </row>
-    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="22"/>
@@ -7937,19 +7935,19 @@
       <c r="I13" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="J13" s="50">
+      <c r="J13" s="48">
         <v>0.9</v>
       </c>
-      <c r="K13" s="50">
+      <c r="K13" s="48">
         <v>0.9</v>
       </c>
-      <c r="L13" s="50">
+      <c r="L13" s="48">
         <v>0.9</v>
       </c>
-      <c r="M13" s="50">
+      <c r="M13" s="48">
         <v>0.9</v>
       </c>
-      <c r="N13" s="50">
+      <c r="N13" s="48">
         <v>0.9</v>
       </c>
       <c r="O13" s="32" t="s">
@@ -7967,7 +7965,7 @@
       <c r="Y13" s="13"/>
       <c r="Z13" s="13"/>
     </row>
-    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11"/>
       <c r="B14" s="12"/>
       <c r="C14" s="22"/>
@@ -7978,19 +7976,19 @@
       <c r="I14" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="J14" s="50">
+      <c r="J14" s="48">
         <v>0.8</v>
       </c>
-      <c r="K14" s="50">
+      <c r="K14" s="48">
         <v>0.8</v>
       </c>
-      <c r="L14" s="50">
+      <c r="L14" s="48">
         <v>0.95</v>
       </c>
-      <c r="M14" s="50">
+      <c r="M14" s="48">
         <v>0.8</v>
       </c>
-      <c r="N14" s="50">
+      <c r="N14" s="48">
         <v>0.75</v>
       </c>
       <c r="O14" s="32" t="s">
@@ -8008,7 +8006,7 @@
       <c r="Y14" s="13"/>
       <c r="Z14" s="13"/>
     </row>
-    <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="C15" s="22"/>
@@ -8036,7 +8034,7 @@
       <c r="Y15" s="13"/>
       <c r="Z15" s="13"/>
     </row>
-    <row r="16" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="22"/>
@@ -8064,7 +8062,7 @@
       <c r="Y16" s="13"/>
       <c r="Z16" s="13"/>
     </row>
-    <row r="17" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="C17" s="40"/>
@@ -8097,7 +8095,7 @@
       <c r="Y17" s="13"/>
       <c r="Z17" s="13"/>
     </row>
-    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -8125,7 +8123,7 @@
       <c r="Y18" s="13"/>
       <c r="Z18" s="13"/>
     </row>
-    <row r="19" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -8153,7 +8151,7 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="14" t="s">
@@ -8183,7 +8181,7 @@
       <c r="Y20" s="13"/>
       <c r="Z20" s="13"/>
     </row>
-    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="C21" s="17"/>
@@ -8215,7 +8213,7 @@
       <c r="Y21" s="13"/>
       <c r="Z21" s="13"/>
     </row>
-    <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="17"/>
@@ -8245,7 +8243,7 @@
       <c r="Y22" s="13"/>
       <c r="Z22" s="13"/>
     </row>
-    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
       <c r="B23" s="12"/>
       <c r="C23" s="22"/>
@@ -8275,7 +8273,7 @@
       <c r="Y23" s="13"/>
       <c r="Z23" s="13"/>
     </row>
-    <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="22"/>
@@ -8303,7 +8301,7 @@
       <c r="Y24" s="13"/>
       <c r="Z24" s="13"/>
     </row>
-    <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="C25" s="22"/>
@@ -8331,7 +8329,7 @@
       <c r="Y25" s="13"/>
       <c r="Z25" s="13"/>
     </row>
-    <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="22"/>
@@ -8371,7 +8369,7 @@
       <c r="Y26" s="13"/>
       <c r="Z26" s="13"/>
     </row>
-    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="22"/>
@@ -8411,7 +8409,7 @@
       <c r="Y27" s="13"/>
       <c r="Z27" s="13"/>
     </row>
-    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="22"/>
@@ -8452,7 +8450,7 @@
       <c r="Y28" s="13"/>
       <c r="Z28" s="13"/>
     </row>
-    <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="22"/>
@@ -8480,7 +8478,7 @@
       <c r="Y29" s="13"/>
       <c r="Z29" s="13"/>
     </row>
-    <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="22"/>
@@ -8508,7 +8506,7 @@
       <c r="Y30" s="13"/>
       <c r="Z30" s="13"/>
     </row>
-    <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
       <c r="C31" s="40"/>
@@ -8541,7 +8539,7 @@
       <c r="Y31" s="13"/>
       <c r="Z31" s="13"/>
     </row>
-    <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -8584,19 +8582,19 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="15.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>89</v>
       </c>
@@ -8604,21 +8602,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="9.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -8626,7 +8624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -8634,7 +8632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -8642,7 +8640,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -8650,7 +8648,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -8658,7 +8656,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -8666,7 +8664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -8674,7 +8672,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>95</v>
       </c>
@@ -8682,7 +8680,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>96</v>
       </c>
@@ -8690,7 +8688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>97</v>
       </c>
@@ -8698,12 +8696,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>83</v>
       </c>
@@ -8711,8 +8709,8 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>87</v>
       </c>
@@ -8720,14 +8718,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
@@ -8735,7 +8733,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>4</v>
       </c>
@@ -8743,7 +8741,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>6</v>
       </c>
@@ -8751,7 +8749,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
@@ -8759,7 +8757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
@@ -8767,7 +8765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
@@ -8775,7 +8773,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>10</v>
       </c>
@@ -8783,7 +8781,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>95</v>
       </c>
@@ -8791,7 +8789,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>96</v>
       </c>
@@ -8799,7 +8797,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>97</v>
       </c>
@@ -8807,7 +8805,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>130</v>
       </c>
@@ -8827,23 +8825,23 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A2:C142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="19.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -8854,8 +8852,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
@@ -8864,12 +8862,12 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>117</v>
       </c>
@@ -8877,7 +8875,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -8885,7 +8883,7 @@
         <v>188000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
@@ -8893,7 +8891,7 @@
         <v>87000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
@@ -8901,7 +8899,7 @@
         <v>297000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
@@ -8909,7 +8907,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
@@ -8917,7 +8915,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -8925,7 +8923,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
@@ -8933,7 +8931,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
@@ -8941,7 +8939,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
@@ -8949,7 +8947,7 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
@@ -8957,7 +8955,7 @@
         <v>78000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>37</v>
       </c>
@@ -8965,7 +8963,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
@@ -8973,7 +8971,7 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
@@ -8981,12 +8979,12 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
@@ -8994,8 +8992,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>41</v>
       </c>
@@ -9003,12 +9001,12 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>43</v>
       </c>
@@ -9016,8 +9014,8 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
@@ -9025,8 +9023,8 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>77</v>
       </c>
@@ -9034,8 +9032,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -9043,8 +9041,8 @@
         <v>5.41</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -9052,8 +9050,8 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -9061,14 +9059,14 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>169</v>
       </c>
@@ -9076,7 +9074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>170</v>
       </c>
@@ -9084,7 +9082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>171</v>
       </c>
@@ -9092,7 +9090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>172</v>
       </c>
@@ -9100,7 +9098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>173</v>
       </c>
@@ -9108,7 +9106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>174</v>
       </c>
@@ -9116,7 +9114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>175</v>
       </c>
@@ -9124,7 +9122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>176</v>
       </c>
@@ -9132,7 +9130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>177</v>
       </c>
@@ -9140,7 +9138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>178</v>
       </c>
@@ -9148,7 +9146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>5</v>
       </c>
@@ -9156,7 +9154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>4</v>
       </c>
@@ -9164,7 +9162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>6</v>
       </c>
@@ -9172,7 +9170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>94</v>
       </c>
@@ -9180,7 +9178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>119</v>
       </c>
@@ -9188,7 +9186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>8</v>
       </c>
@@ -9196,7 +9194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>9</v>
       </c>
@@ -9204,7 +9202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>7</v>
       </c>
@@ -9212,7 +9210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>10</v>
       </c>
@@ -9220,7 +9218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>95</v>
       </c>
@@ -9228,7 +9226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>96</v>
       </c>
@@ -9236,7 +9234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>97</v>
       </c>
@@ -9244,12 +9242,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>49</v>
       </c>
@@ -9257,8 +9255,8 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>50</v>
       </c>
@@ -9266,8 +9264,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>51</v>
       </c>
@@ -9275,8 +9273,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>86</v>
       </c>
@@ -9284,14 +9282,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B74" s="4"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
         <v>5</v>
       </c>
@@ -9299,7 +9297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>4</v>
       </c>
@@ -9307,7 +9305,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
         <v>6</v>
       </c>
@@ -9315,7 +9313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
         <v>8</v>
       </c>
@@ -9323,7 +9321,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>9</v>
       </c>
@@ -9331,7 +9329,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>7</v>
       </c>
@@ -9339,7 +9337,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>10</v>
       </c>
@@ -9347,7 +9345,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>95</v>
       </c>
@@ -9355,7 +9353,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>96</v>
       </c>
@@ -9363,7 +9361,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>97</v>
       </c>
@@ -9371,13 +9369,13 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B86" s="4"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>5</v>
       </c>
@@ -9385,7 +9383,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>4</v>
       </c>
@@ -9393,7 +9391,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>6</v>
       </c>
@@ -9401,7 +9399,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
         <v>8</v>
       </c>
@@ -9409,7 +9407,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>9</v>
       </c>
@@ -9417,7 +9415,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
         <v>7</v>
       </c>
@@ -9425,7 +9423,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
         <v>10</v>
       </c>
@@ -9433,7 +9431,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
         <v>95</v>
       </c>
@@ -9441,7 +9439,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
         <v>96</v>
       </c>
@@ -9449,7 +9447,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
         <v>97</v>
       </c>
@@ -9457,12 +9455,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>55</v>
       </c>
@@ -9470,8 +9468,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
         <v>56</v>
       </c>
@@ -9479,8 +9477,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="4" t="s">
         <v>57</v>
       </c>
@@ -9488,8 +9486,8 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="4" t="s">
         <v>58</v>
       </c>
@@ -9497,8 +9495,8 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="106" spans="1:2" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="3" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="4" t="s">
         <v>59</v>
       </c>
@@ -9506,12 +9504,12 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
         <v>61</v>
       </c>
@@ -9519,13 +9517,13 @@
         <v>11.3</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B112" s="4"/>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="4" t="s">
         <v>63</v>
       </c>
@@ -9533,13 +9531,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B114" s="4"/>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="4" t="s">
         <v>64</v>
       </c>
@@ -9547,7 +9545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
         <v>65</v>
       </c>
@@ -9555,7 +9553,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
         <v>66</v>
       </c>
@@ -9563,7 +9561,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
         <v>67</v>
       </c>
@@ -9571,7 +9569,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>68</v>
       </c>
@@ -9579,7 +9577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>69</v>
       </c>
@@ -9587,8 +9585,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>70</v>
       </c>
@@ -9596,8 +9594,8 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
         <v>71</v>
       </c>
@@ -9605,8 +9603,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" ht="5.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
         <v>72</v>
       </c>
@@ -9614,8 +9612,8 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
         <v>73</v>
       </c>
@@ -9623,12 +9621,12 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="s">
         <v>75</v>
       </c>
@@ -9636,8 +9634,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="s">
         <v>76</v>
       </c>
@@ -9645,12 +9643,12 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137" s="8"/>
       <c r="B137" s="8" t="s">
         <v>144</v>
@@ -9659,7 +9657,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138" s="9" t="s">
         <v>6</v>
       </c>
@@ -9670,7 +9668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139" s="9" t="s">
         <v>4</v>
       </c>
@@ -9681,7 +9679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140" s="9" t="s">
         <v>7</v>
       </c>
@@ -9692,7 +9690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="9" t="s">
         <v>5</v>
       </c>
@@ -9703,7 +9701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="9" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
Adjust spreader field efficiency (from 0.3 to 5) and spraying speed (from 15 to 20)
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B77CC8-7E43-4FA9-8951-963A38663CD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A353993A-29D2-4369-A394-B723662B7121}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,6 @@
     <definedName name="grain_income_date" localSheetId="0">Price!$B$36</definedName>
     <definedName name="grain_income_length" localSheetId="0">Price!$B$38</definedName>
     <definedName name="grain_price" localSheetId="0">Price!$A$48:$H$60</definedName>
-    <definedName name="grain_price_grouped">Price!$A$42:$H$46</definedName>
     <definedName name="harv_eff" localSheetId="5">'Mach 1'!$B$72</definedName>
     <definedName name="harv_fuel_consumption" localSheetId="5">'Mach 1'!$B$68</definedName>
     <definedName name="harvest_index">'[1]Crop Sim'!$L$358:$M$374</definedName>
@@ -139,14 +138,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -875,10 +866,35 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>John</author>
     <author>Michael Young</author>
   </authors>
   <commentList>
-    <comment ref="I27" authorId="0" shapeId="0" xr:uid="{3DC02098-1628-4880-9C5F-57BC4ABDAA2B}">
+    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{40E4A487-40A1-4E14-AC15-C25613895007}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>John:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+To represent the grain that the animals do not find</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I27" authorId="1" shapeId="0" xr:uid="{3DC02098-1628-4880-9C5F-57BC4ABDAA2B}">
       <text>
         <r>
           <rPr>
@@ -902,7 +918,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I28" authorId="0" shapeId="0" xr:uid="{76302044-C55B-483C-9985-192E6879EAED}">
+    <comment ref="I28" authorId="1" shapeId="0" xr:uid="{76302044-C55B-483C-9985-192E6879EAED}">
       <text>
         <r>
           <rPr>
@@ -926,7 +942,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N28" authorId="0" shapeId="0" xr:uid="{C3DF5EF6-5F7E-41B0-9113-E06058B6E139}">
+    <comment ref="N28" authorId="1" shapeId="0" xr:uid="{C3DF5EF6-5F7E-41B0-9113-E06058B6E139}">
       <text>
         <r>
           <rPr>
@@ -1940,7 +1956,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-fert spreder repairs and maint $/hr (doesn't include tractor, that is recorded in the tractor section)</t>
+fert spreader repairs and maint $/hr (doesn't include tractor, that is recorded in the tractor section)</t>
         </r>
       </text>
     </comment>
@@ -1988,7 +2004,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-stubble handeler repairs and maint $/ha (doesn't include tractor, that is recorded in the tractor section)</t>
+stubble handler repairs and maint $/ha (doesn't include tractor, that is recorded in the tractor section)</t>
         </r>
       </text>
     </comment>
@@ -2045,7 +2061,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="188">
   <si>
     <t>Machinery</t>
   </si>
@@ -2413,12 +2429,6 @@
     <t>Labour</t>
   </si>
   <si>
-    <t>manager_cost</t>
-  </si>
-  <si>
-    <t>permanent_cost</t>
-  </si>
-  <si>
     <t>permanent_super</t>
   </si>
   <si>
@@ -2428,9 +2438,6 @@
     <t>permanent_ls_leave</t>
   </si>
   <si>
-    <t>casual_cost</t>
-  </si>
-  <si>
     <t>casual_super</t>
   </si>
   <si>
@@ -2585,6 +2592,39 @@
   </si>
   <si>
     <t>*not used, can probs remove</t>
+  </si>
+  <si>
+    <t>manager_cost ($/yr)</t>
+  </si>
+  <si>
+    <t>permanent_cost ($/yr)</t>
+  </si>
+  <si>
+    <t>casual_cost ($/hr)</t>
+  </si>
+  <si>
+    <t>Might not be used anymore</t>
+  </si>
+  <si>
+    <t>proportion of fuel cost</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>km/hr</t>
+  </si>
+  <si>
+    <t>L/ha</t>
+  </si>
+  <si>
+    <t>L/hr</t>
+  </si>
+  <si>
+    <t>hr</t>
+  </si>
+  <si>
+    <t>$/hr</t>
   </si>
 </sst>
 </file>
@@ -2596,7 +2636,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2674,6 +2714,19 @@
       <color theme="2"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2869,7 +2922,7 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2964,9 +3017,6 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="9" borderId="9" xfId="2">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="5" fillId="8" borderId="7" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2977,6 +3027,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="9" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="5" fillId="9" borderId="9" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -6418,30 +6472,30 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="31" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -6452,8 +6506,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -6464,93 +6518,123 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="4">
         <v>300</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="4">
         <v>300</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="4">
         <v>300</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="4">
         <v>300</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="4">
         <v>300</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="4">
         <v>300</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="4">
         <v>300</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>95</v>
       </c>
       <c r="B15" s="4">
         <v>300</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C15" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>96</v>
       </c>
       <c r="B16" s="4">
         <v>300</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B17" s="4">
         <v>300</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
@@ -6561,13 +6645,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
@@ -6578,8 +6662,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
@@ -6590,8 +6674,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -6602,37 +6686,43 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B29" s="8">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="6.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C29" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B31" s="8">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>102</v>
       </c>
@@ -6640,7 +6730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>103</v>
       </c>
@@ -6648,8 +6738,8 @@
         <v>43814</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>104</v>
       </c>
@@ -6657,180 +6747,180 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B40" s="6">
         <v>43692</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A42" s="49" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="49" t="s">
+      <c r="B42" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="49" t="s">
+      <c r="C42" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="D42" s="49" t="s">
+      <c r="D42" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="E42" s="49" t="s">
+      <c r="E42" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="F42" s="49" t="s">
+      <c r="F42" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="G42" s="49" t="s">
+      <c r="G42" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="H42" s="49" t="s">
+      <c r="H42" s="48" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="50" t="s">
-        <v>163</v>
-      </c>
-      <c r="B43" s="51">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="49" t="s">
+        <v>160</v>
+      </c>
+      <c r="B43" s="50">
         <f>AVERAGE(B49,B51,B59)</f>
         <v>246.66666666666666</v>
       </c>
-      <c r="C43" s="51">
+      <c r="C43" s="50">
         <f t="shared" ref="C43:H43" si="0">AVERAGE(C49,C51,C59)</f>
         <v>231.66666666666666</v>
       </c>
-      <c r="D43" s="52">
+      <c r="D43" s="51">
         <f t="shared" si="0"/>
         <v>0.83333333333333337</v>
       </c>
-      <c r="E43" s="52">
+      <c r="E43" s="51">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="F43" s="51">
+      <c r="F43" s="50">
         <f t="shared" si="0"/>
         <v>0.26666666666666666</v>
       </c>
-      <c r="G43" s="51">
+      <c r="G43" s="50">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="H43" s="51">
+      <c r="H43" s="50">
         <f t="shared" si="0"/>
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="50" t="s">
-        <v>162</v>
-      </c>
-      <c r="B44" s="51">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="49" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" s="50">
         <f>AVERAGE(B57,B60)</f>
         <v>550</v>
       </c>
-      <c r="C44" s="51">
+      <c r="C44" s="50">
         <f t="shared" ref="C44:H44" si="1">AVERAGE(C57,C60)</f>
         <v>550</v>
       </c>
-      <c r="D44" s="52">
+      <c r="D44" s="51">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="E44" s="52">
+      <c r="E44" s="51">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F44" s="51">
+      <c r="F44" s="50">
         <f t="shared" si="1"/>
         <v>0.12</v>
       </c>
-      <c r="G44" s="51">
+      <c r="G44" s="50">
         <f t="shared" si="1"/>
         <v>21.95</v>
       </c>
-      <c r="H44" s="51">
+      <c r="H44" s="50">
         <f t="shared" si="1"/>
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" s="50" t="s">
-        <v>164</v>
-      </c>
-      <c r="B45" s="51">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" s="50">
         <f>AVERAGE(B50,B52:B54,B58)</f>
         <v>341</v>
       </c>
-      <c r="C45" s="51">
+      <c r="C45" s="50">
         <f t="shared" ref="C45:H45" si="2">AVERAGE(C50,C52:C54,C58)</f>
         <v>341</v>
       </c>
-      <c r="D45" s="52">
+      <c r="D45" s="51">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="E45" s="52">
+      <c r="E45" s="51">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="F45" s="51">
+      <c r="F45" s="50">
         <f t="shared" si="2"/>
         <v>0.15</v>
       </c>
-      <c r="G45" s="51">
+      <c r="G45" s="50">
         <f t="shared" si="2"/>
         <v>15.089999999999998</v>
       </c>
-      <c r="H45" s="51">
+      <c r="H45" s="50">
         <f t="shared" si="2"/>
         <v>1.0920000000000001</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A46" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="B46" s="51">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46" s="50">
         <f>AVERAGE(B49:B60)</f>
         <v>315</v>
       </c>
-      <c r="C46" s="51">
+      <c r="C46" s="50">
         <f t="shared" ref="C46:H46" si="3">AVERAGE(C49:C60)</f>
         <v>311.25</v>
       </c>
-      <c r="D46" s="52">
+      <c r="D46" s="51">
         <f>AVERAGE(D49:D60)</f>
         <v>0.95833333333333337</v>
       </c>
-      <c r="E46" s="52">
+      <c r="E46" s="51">
         <f t="shared" si="3"/>
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F46" s="51">
+      <c r="F46" s="50">
         <f t="shared" si="3"/>
         <v>0.16166666666666665</v>
       </c>
-      <c r="G46" s="51">
+      <c r="G46" s="50">
         <f t="shared" si="3"/>
         <v>13.266666666666666</v>
       </c>
-      <c r="H46" s="51">
+      <c r="H46" s="50">
         <f t="shared" si="3"/>
         <v>0.93800000000000028</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>91</v>
       </c>
@@ -6856,7 +6946,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>4</v>
       </c>
@@ -6866,10 +6956,10 @@
       <c r="C49" s="4">
         <v>265</v>
       </c>
-      <c r="D49" s="4">
+      <c r="D49" s="52">
         <v>0.7</v>
       </c>
-      <c r="E49" s="46">
+      <c r="E49" s="53">
         <f t="shared" ref="E49:E58" si="4">1-D49</f>
         <v>0.30000000000000004</v>
       </c>
@@ -6884,7 +6974,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>10</v>
       </c>
@@ -6894,10 +6984,10 @@
       <c r="C50" s="4">
         <v>350</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D50" s="52">
         <v>1</v>
       </c>
-      <c r="E50" s="46">
+      <c r="E50" s="53">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -6912,7 +7002,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>94</v>
       </c>
@@ -6922,10 +7012,10 @@
       <c r="C51" s="4">
         <v>150</v>
       </c>
-      <c r="D51" s="4">
+      <c r="D51" s="52">
         <v>1</v>
       </c>
-      <c r="E51" s="46">
+      <c r="E51" s="53">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -6940,7 +7030,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>95</v>
       </c>
@@ -6950,10 +7040,10 @@
       <c r="C52" s="4">
         <v>350</v>
       </c>
-      <c r="D52" s="4">
+      <c r="D52" s="52">
         <v>1</v>
       </c>
-      <c r="E52" s="46">
+      <c r="E52" s="53">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -6968,7 +7058,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>96</v>
       </c>
@@ -6978,10 +7068,10 @@
       <c r="C53" s="4">
         <v>350</v>
       </c>
-      <c r="D53" s="4">
+      <c r="D53" s="52">
         <v>1</v>
       </c>
-      <c r="E53" s="46">
+      <c r="E53" s="53">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -6996,7 +7086,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -7006,10 +7096,10 @@
       <c r="C54" s="4">
         <v>305</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D54" s="52">
         <v>1</v>
       </c>
-      <c r="E54" s="46">
+      <c r="E54" s="53">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -7024,7 +7114,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>6</v>
       </c>
@@ -7034,10 +7124,10 @@
       <c r="C55" s="4">
         <v>235</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D55" s="52">
         <v>1</v>
       </c>
-      <c r="E55" s="46">
+      <c r="E55" s="53">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -7052,7 +7142,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>119</v>
       </c>
@@ -7062,10 +7152,10 @@
       <c r="C56" s="4">
         <v>0</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D56" s="52">
         <v>1</v>
       </c>
-      <c r="E56" s="46">
+      <c r="E56" s="53">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -7079,7 +7169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>9</v>
       </c>
@@ -7089,10 +7179,10 @@
       <c r="C57" s="4">
         <v>550</v>
       </c>
-      <c r="D57" s="4">
+      <c r="D57" s="52">
         <v>1</v>
       </c>
-      <c r="E57" s="46">
+      <c r="E57" s="53">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -7107,7 +7197,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>97</v>
       </c>
@@ -7117,10 +7207,10 @@
       <c r="C58" s="4">
         <v>350</v>
       </c>
-      <c r="D58" s="4">
+      <c r="D58" s="52">
         <v>1</v>
       </c>
-      <c r="E58" s="46">
+      <c r="E58" s="53">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -7135,7 +7225,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>5</v>
       </c>
@@ -7145,10 +7235,10 @@
       <c r="C59" s="4">
         <v>280</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D59" s="52">
         <v>0.8</v>
       </c>
-      <c r="E59" s="46">
+      <c r="E59" s="53">
         <f t="shared" ref="E59:E60" si="6">1-D59</f>
         <v>0.19999999999999996</v>
       </c>
@@ -7163,7 +7253,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>8</v>
       </c>
@@ -7173,10 +7263,10 @@
       <c r="C60" s="4">
         <v>550</v>
       </c>
-      <c r="D60" s="4">
+      <c r="D60" s="52">
         <v>1</v>
       </c>
-      <c r="E60" s="46">
+      <c r="E60" s="53">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -7191,12 +7281,12 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>116</v>
       </c>
@@ -7204,10 +7294,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="9.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>112</v>
       </c>
@@ -7215,7 +7305,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>68</v>
       </c>
@@ -7223,7 +7313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>67</v>
       </c>
@@ -7231,7 +7321,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>66</v>
       </c>
@@ -7239,7 +7329,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>114</v>
       </c>
@@ -7247,7 +7337,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>63</v>
       </c>
@@ -7255,15 +7345,15 @@
         <v>550</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B71" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>65</v>
       </c>
@@ -7271,72 +7361,72 @@
         <v>520</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>122</v>
+        <v>177</v>
       </c>
       <c r="B76" s="4">
         <v>80000</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>123</v>
+        <v>178</v>
       </c>
       <c r="B78" s="4">
         <v>80000</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B80" s="52">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B82" s="52">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="B80" s="4">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B82" s="4">
-        <v>3.5000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="B84" s="4">
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>127</v>
+        <v>179</v>
       </c>
       <c r="B86" s="4">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B88" s="4">
+        <v>125</v>
+      </c>
+      <c r="B88" s="52">
         <v>0.09</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B90" s="4">
+        <v>126</v>
+      </c>
+      <c r="B90" s="52">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
@@ -7356,83 +7446,83 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.81640625" style="1"/>
+    <col min="2" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="46">
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="47">
+      <c r="B5" s="46">
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="B8" s="47">
+        <v>156</v>
+      </c>
+      <c r="B8" s="46">
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B11" s="47">
+        <v>157</v>
+      </c>
+      <c r="B11" s="46">
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="46">
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B17" s="47">
+        <v>165</v>
+      </c>
+      <c r="B17" s="46">
         <v>0.02</v>
       </c>
     </row>
@@ -7444,29 +7534,34 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DED9269B-34A0-4B4D-B79F-55BA46418231}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="G2:H13"/>
+  <dimension ref="G1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD39"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="2" style="1" customWidth="1"/>
-    <col min="3" max="3" width="0.1796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="2.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="1.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.26953125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="1"/>
+    <col min="3" max="3" width="0.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="1.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G2" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G3" s="5" t="s">
         <v>111</v>
       </c>
@@ -7474,10 +7569,10 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="7:8" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="7:8" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G5" s="4" t="s">
         <v>105</v>
       </c>
@@ -7485,8 +7580,8 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G7" s="4" t="s">
         <v>106</v>
       </c>
@@ -7494,8 +7589,8 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="8" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G9" s="4" t="s">
         <v>107</v>
       </c>
@@ -7503,8 +7598,8 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="10" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G11" s="4" t="s">
         <v>108</v>
       </c>
@@ -7512,8 +7607,8 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="12" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="7:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G13" s="4" t="s">
         <v>109</v>
       </c>
@@ -7532,19 +7627,19 @@
   <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14:N14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.453125" customWidth="1"/>
-    <col min="2" max="2" width="2.26953125" customWidth="1"/>
-    <col min="3" max="4" width="2.7265625" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="2.28515625" customWidth="1"/>
+    <col min="3" max="4" width="2.7109375" customWidth="1"/>
     <col min="5" max="5" width="2" customWidth="1"/>
-    <col min="6" max="6" width="4.1796875" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -7572,7 +7667,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="12"/>
     </row>
-    <row r="2" spans="1:26" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:26" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -7600,11 +7695,11 @@
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
     </row>
-    <row r="3" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -7630,17 +7725,17 @@
       <c r="Y3" s="13"/>
       <c r="Z3" s="13"/>
     </row>
-    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="19" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
@@ -7662,7 +7757,7 @@
       <c r="Y4" s="13"/>
       <c r="Z4" s="13"/>
     </row>
-    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="17"/>
@@ -7670,7 +7765,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
@@ -7692,7 +7787,7 @@
       <c r="Y5" s="13"/>
       <c r="Z5" s="13"/>
     </row>
-    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="22"/>
@@ -7722,7 +7817,7 @@
       <c r="Y6" s="13"/>
       <c r="Z6" s="13"/>
     </row>
-    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="22"/>
@@ -7750,7 +7845,7 @@
       <c r="Y7" s="13"/>
       <c r="Z7" s="13"/>
     </row>
-    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="22"/>
@@ -7778,7 +7873,7 @@
       <c r="Y8" s="13"/>
       <c r="Z8" s="13"/>
     </row>
-    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="22"/>
@@ -7806,7 +7901,7 @@
       <c r="Y9" s="13"/>
       <c r="Z9" s="13"/>
     </row>
-    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="22"/>
@@ -7844,7 +7939,7 @@
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
     </row>
-    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="22"/>
@@ -7853,7 +7948,7 @@
       <c r="F11" s="28"/>
       <c r="H11" s="32"/>
       <c r="I11" s="45" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J11" s="33">
         <v>11400</v>
@@ -7871,7 +7966,7 @@
         <v>7000</v>
       </c>
       <c r="O11" s="32" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="P11" s="34"/>
       <c r="Q11" s="34"/>
@@ -7885,7 +7980,7 @@
       <c r="Y11" s="13"/>
       <c r="Z11" s="13"/>
     </row>
-    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="22"/>
@@ -7894,7 +7989,7 @@
       <c r="F12" s="28"/>
       <c r="H12" s="32"/>
       <c r="I12" s="45" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J12" s="33">
         <v>0.1</v>
@@ -7924,7 +8019,7 @@
       <c r="Y12" s="13"/>
       <c r="Z12" s="13"/>
     </row>
-    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="22"/>
@@ -7933,25 +8028,25 @@
       <c r="F13" s="28"/>
       <c r="H13" s="32"/>
       <c r="I13" s="45" t="s">
-        <v>154</v>
-      </c>
-      <c r="J13" s="48">
+        <v>151</v>
+      </c>
+      <c r="J13" s="47">
         <v>0.9</v>
       </c>
-      <c r="K13" s="48">
+      <c r="K13" s="47">
         <v>0.9</v>
       </c>
-      <c r="L13" s="48">
+      <c r="L13" s="47">
         <v>0.9</v>
       </c>
-      <c r="M13" s="48">
+      <c r="M13" s="47">
         <v>0.9</v>
       </c>
-      <c r="N13" s="48">
+      <c r="N13" s="47">
         <v>0.9</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="P13" s="34"/>
       <c r="Q13" s="34"/>
@@ -7965,7 +8060,7 @@
       <c r="Y13" s="13"/>
       <c r="Z13" s="13"/>
     </row>
-    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="12"/>
       <c r="C14" s="22"/>
@@ -7974,25 +8069,25 @@
       <c r="F14" s="28"/>
       <c r="H14" s="32"/>
       <c r="I14" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="J14" s="48">
+        <v>152</v>
+      </c>
+      <c r="J14" s="47">
         <v>0.8</v>
       </c>
-      <c r="K14" s="48">
+      <c r="K14" s="47">
         <v>0.8</v>
       </c>
-      <c r="L14" s="48">
+      <c r="L14" s="47">
         <v>0.95</v>
       </c>
-      <c r="M14" s="48">
+      <c r="M14" s="47">
         <v>0.8</v>
       </c>
-      <c r="N14" s="48">
+      <c r="N14" s="47">
         <v>0.75</v>
       </c>
       <c r="O14" s="32" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="P14" s="34"/>
       <c r="Q14" s="34"/>
@@ -8006,7 +8101,7 @@
       <c r="Y14" s="13"/>
       <c r="Z14" s="13"/>
     </row>
-    <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="C15" s="22"/>
@@ -8034,7 +8129,7 @@
       <c r="Y15" s="13"/>
       <c r="Z15" s="13"/>
     </row>
-    <row r="16" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="22"/>
@@ -8062,7 +8157,7 @@
       <c r="Y16" s="13"/>
       <c r="Z16" s="13"/>
     </row>
-    <row r="17" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="C17" s="40"/>
@@ -8089,13 +8184,13 @@
       <c r="U17" s="40"/>
       <c r="V17" s="40"/>
       <c r="W17" s="42" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
       <c r="Z17" s="13"/>
     </row>
-    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -8123,7 +8218,7 @@
       <c r="Y18" s="13"/>
       <c r="Z18" s="13"/>
     </row>
-    <row r="19" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -8151,11 +8246,11 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
@@ -8181,17 +8276,17 @@
       <c r="Y20" s="13"/>
       <c r="Z20" s="13"/>
     </row>
-    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
@@ -8213,7 +8308,7 @@
       <c r="Y21" s="13"/>
       <c r="Z21" s="13"/>
     </row>
-    <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="17"/>
@@ -8221,7 +8316,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
@@ -8243,7 +8338,7 @@
       <c r="Y22" s="13"/>
       <c r="Z22" s="13"/>
     </row>
-    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="12"/>
       <c r="C23" s="22"/>
@@ -8273,7 +8368,7 @@
       <c r="Y23" s="13"/>
       <c r="Z23" s="13"/>
     </row>
-    <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="22"/>
@@ -8301,7 +8396,7 @@
       <c r="Y24" s="13"/>
       <c r="Z24" s="13"/>
     </row>
-    <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="C25" s="22"/>
@@ -8329,7 +8424,7 @@
       <c r="Y25" s="13"/>
       <c r="Z25" s="13"/>
     </row>
-    <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="22"/>
@@ -8339,7 +8434,7 @@
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J26" s="26" t="s">
         <v>6</v>
@@ -8369,7 +8464,7 @@
       <c r="Y26" s="13"/>
       <c r="Z26" s="13"/>
     </row>
-    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="22"/>
@@ -8379,22 +8474,22 @@
       <c r="G27" s="29"/>
       <c r="H27" s="29"/>
       <c r="I27" s="29" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J27" s="30" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="K27" s="30" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="L27" s="30" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="M27" s="30" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="N27" s="30" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="O27" s="30"/>
       <c r="P27" s="30"/>
@@ -8409,7 +8504,7 @@
       <c r="Y27" s="13"/>
       <c r="Z27" s="13"/>
     </row>
-    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="22"/>
@@ -8418,7 +8513,7 @@
       <c r="F28" s="28"/>
       <c r="H28" s="32"/>
       <c r="I28" s="45" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="J28" s="44">
         <v>0.45</v>
@@ -8436,7 +8531,7 @@
         <v>1</v>
       </c>
       <c r="O28" s="32" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="P28" s="34"/>
       <c r="Q28" s="34"/>
@@ -8450,7 +8545,7 @@
       <c r="Y28" s="13"/>
       <c r="Z28" s="13"/>
     </row>
-    <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="22"/>
@@ -8478,7 +8573,7 @@
       <c r="Y29" s="13"/>
       <c r="Z29" s="13"/>
     </row>
-    <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="22"/>
@@ -8506,7 +8601,7 @@
       <c r="Y30" s="13"/>
       <c r="Z30" s="13"/>
     </row>
-    <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
       <c r="C31" s="40"/>
@@ -8533,13 +8628,13 @@
       <c r="U31" s="40"/>
       <c r="V31" s="40"/>
       <c r="W31" s="42" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="X31" s="13"/>
       <c r="Y31" s="13"/>
       <c r="Z31" s="13"/>
     </row>
-    <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -8579,22 +8674,22 @@
   <dimension ref="A2:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>89</v>
       </c>
@@ -8602,21 +8697,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="9.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -8624,7 +8719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -8632,7 +8727,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -8640,7 +8735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -8648,7 +8743,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -8656,7 +8751,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -8664,7 +8759,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -8672,7 +8767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>95</v>
       </c>
@@ -8680,7 +8775,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>96</v>
       </c>
@@ -8688,7 +8783,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>97</v>
       </c>
@@ -8696,12 +8791,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>83</v>
       </c>
@@ -8709,8 +8804,8 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>87</v>
       </c>
@@ -8718,14 +8813,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="23" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
@@ -8733,7 +8828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>4</v>
       </c>
@@ -8741,7 +8836,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>6</v>
       </c>
@@ -8749,7 +8844,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
@@ -8757,7 +8852,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
@@ -8765,7 +8860,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
@@ -8773,7 +8868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>10</v>
       </c>
@@ -8781,7 +8876,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>95</v>
       </c>
@@ -8789,7 +8884,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>96</v>
       </c>
@@ -8797,7 +8892,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>97</v>
       </c>
@@ -8805,9 +8900,9 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B35" s="6">
         <v>43554</v>
@@ -8825,23 +8920,23 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A2:C142"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="B127" sqref="B127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.81640625" style="1"/>
+    <col min="1" max="1" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -8852,22 +8947,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="52">
         <v>0.08</v>
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>117</v>
       </c>
@@ -8875,7 +8970,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>27</v>
       </c>
@@ -8883,7 +8978,7 @@
         <v>188000</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
@@ -8891,7 +8986,7 @@
         <v>87000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
@@ -8899,7 +8994,7 @@
         <v>297000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>30</v>
       </c>
@@ -8907,7 +9002,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>31</v>
       </c>
@@ -8915,7 +9010,7 @@
         <v>35000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -8923,7 +9018,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
@@ -8931,7 +9026,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>34</v>
       </c>
@@ -8939,7 +9034,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
@@ -8947,7 +9042,7 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
@@ -8955,7 +9050,7 @@
         <v>78000</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>37</v>
       </c>
@@ -8963,7 +9058,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>38</v>
       </c>
@@ -8971,7 +9066,7 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>39</v>
       </c>
@@ -8979,43 +9074,52 @@
         <v>36000</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="4">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="4">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B29" s="4">
         <v>12.2</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>44</v>
       </c>
@@ -9023,17 +9127,20 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>77</v>
       </c>
       <c r="B33" s="4">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -9041,8 +9148,8 @@
         <v>5.41</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -9050,8 +9157,8 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -9059,94 +9166,94 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B41" s="4"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B42" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B43" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B49" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B51" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>5</v>
       </c>
@@ -9154,7 +9261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>4</v>
       </c>
@@ -9162,7 +9269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>6</v>
       </c>
@@ -9170,7 +9277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>94</v>
       </c>
@@ -9178,7 +9285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>119</v>
       </c>
@@ -9186,7 +9293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>8</v>
       </c>
@@ -9194,7 +9301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>9</v>
       </c>
@@ -9202,7 +9309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>7</v>
       </c>
@@ -9210,7 +9317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>10</v>
       </c>
@@ -9218,7 +9325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>95</v>
       </c>
@@ -9226,7 +9333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>96</v>
       </c>
@@ -9234,7 +9341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>97</v>
       </c>
@@ -9242,12 +9349,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>49</v>
       </c>
@@ -9255,8 +9362,8 @@
         <v>12.2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>50</v>
       </c>
@@ -9264,17 +9371,20 @@
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>51</v>
       </c>
       <c r="B70" s="4">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C70" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>86</v>
       </c>
@@ -9282,14 +9392,14 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>52</v>
       </c>
       <c r="B74" s="4"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>5</v>
       </c>
@@ -9297,7 +9407,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>4</v>
       </c>
@@ -9305,7 +9415,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>6</v>
       </c>
@@ -9313,7 +9423,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>8</v>
       </c>
@@ -9321,7 +9431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>9</v>
       </c>
@@ -9329,7 +9439,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>7</v>
       </c>
@@ -9337,7 +9447,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>10</v>
       </c>
@@ -9345,7 +9455,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>95</v>
       </c>
@@ -9353,7 +9463,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>96</v>
       </c>
@@ -9361,7 +9471,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>97</v>
       </c>
@@ -9369,13 +9479,13 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B86" s="4"/>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>5</v>
       </c>
@@ -9383,7 +9493,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>4</v>
       </c>
@@ -9391,7 +9501,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>6</v>
       </c>
@@ -9399,7 +9509,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>8</v>
       </c>
@@ -9407,7 +9517,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>9</v>
       </c>
@@ -9415,7 +9525,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>7</v>
       </c>
@@ -9423,7 +9533,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>10</v>
       </c>
@@ -9431,7 +9541,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>95</v>
       </c>
@@ -9439,7 +9549,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>96</v>
       </c>
@@ -9447,7 +9557,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>97</v>
       </c>
@@ -9455,30 +9565,36 @@
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B99" s="4">
         <v>25</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C99" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>56</v>
       </c>
       <c r="B101" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>57</v>
       </c>
@@ -9486,17 +9602,20 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="104" spans="1:2" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:3" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B105" s="4">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" ht="3" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C105" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>59</v>
       </c>
@@ -9504,26 +9623,29 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B110" s="4">
         <v>11.3</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C110" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B112" s="4"/>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>63</v>
       </c>
@@ -9531,13 +9653,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B114" s="4"/>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>64</v>
       </c>
@@ -9545,7 +9667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>65</v>
       </c>
@@ -9553,7 +9675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>66</v>
       </c>
@@ -9561,7 +9683,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>67</v>
       </c>
@@ -9569,7 +9691,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>68</v>
       </c>
@@ -9577,7 +9699,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>69</v>
       </c>
@@ -9585,79 +9707,94 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>70</v>
       </c>
       <c r="B123" s="4">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C123" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B125" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" ht="5.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C125" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B127" s="4">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B129" s="4">
         <v>14.3</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C129" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B132" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C132" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B134" s="4">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C134" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="8"/>
       <c r="B137" s="8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
         <v>6</v>
       </c>
@@ -9668,7 +9805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="9" t="s">
         <v>4</v>
       </c>
@@ -9679,7 +9816,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" s="9" t="s">
         <v>7</v>
       </c>
@@ -9690,7 +9827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" s="9" t="s">
         <v>5</v>
       </c>
@@ -9701,7 +9838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="9" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
output changes. update grain price for OF so late sowing gets penalty.
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\AFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A353993A-29D2-4369-A394-B723662B7121}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC3C936-502C-4A33-B6A1-C3580F39518D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -138,6 +138,14 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -146,6 +154,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Michael Young</author>
+    <author>Michael Young (21512438)</author>
   </authors>
   <commentList>
     <comment ref="A7" authorId="0" shapeId="0" xr:uid="{DF18B245-D438-41C3-B575-081F7DB8D608}">
@@ -581,6 +590,30 @@
           <t xml:space="preserve">
 %
 includes 5% stamp duty</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B56" authorId="1" shapeId="0" xr:uid="{84049E11-3C26-4C89-9C78-AB4610D5D289}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+There is a cost here so that the model doesn’t choose to sow OF late in the year so that it can get poc</t>
         </r>
       </text>
     </comment>
@@ -6472,8 +6505,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6890,11 +6923,11 @@
       </c>
       <c r="B46" s="50">
         <f>AVERAGE(B49:B60)</f>
-        <v>315</v>
+        <v>340</v>
       </c>
       <c r="C46" s="50">
         <f t="shared" ref="C46:H46" si="3">AVERAGE(C49:C60)</f>
-        <v>311.25</v>
+        <v>336.25</v>
       </c>
       <c r="D46" s="51">
         <f>AVERAGE(D49:D60)</f>
@@ -7147,10 +7180,10 @@
         <v>119</v>
       </c>
       <c r="B56" s="4">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="C56" s="4">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="D56" s="52">
         <v>1</v>
@@ -8920,7 +8953,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A2:C142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+    <sheetView topLeftCell="A111" workbookViewId="0">
       <selection activeCell="B127" sqref="B127"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
tidy up mach value and add crop monitoring. Convert labour index to L00 - L16
</commit_message>
<xml_diff>
--- a/Universal.xlsx
+++ b/Universal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\21512438\Dropbox\Michael\Work-Uni-Coding\AFO\AFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC3C936-502C-4A33-B6A1-C3580F39518D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C4363A-F537-4E12-9C39-A0FA5F6B02EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" activeTab="5" xr2:uid="{26DC18AC-FA22-4741-8965-316F71A72BB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Price" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="casual_cost">Price!$B$86</definedName>
     <definedName name="casual_super">Price!$B$88</definedName>
     <definedName name="casual_workers_comp">Price!$B$90</definedName>
-    <definedName name="clearing_value" localSheetId="5">'Mach 1'!$A$8:$B$21</definedName>
+    <definedName name="clearing_value" localSheetId="5">'Mach 1'!$A$8:$E$23</definedName>
     <definedName name="contract_bail" localSheetId="0">Price!$B$24</definedName>
     <definedName name="contract_harv_cost" localSheetId="0">Price!$A$7:$B$17</definedName>
     <definedName name="contract_harv_eff" localSheetId="4">'Mach General'!$B$21</definedName>
@@ -43,7 +43,7 @@
     <definedName name="dep_area" localSheetId="5">'Mach 1'!$B$3</definedName>
     <definedName name="diesel" localSheetId="0">Price!$B$3</definedName>
     <definedName name="diesel_rebate" localSheetId="0">Price!$B$5</definedName>
-    <definedName name="draft_seeding" localSheetId="5">'Mach 1'!$B$35</definedName>
+    <definedName name="draft_seeding" localSheetId="5">'Mach 1'!$B$37</definedName>
     <definedName name="drymatter_grazed">'[1]Crop Sim'!$S$313:$S$341</definedName>
     <definedName name="equip_insurance">Finance!$B$17</definedName>
     <definedName name="fert_cartage_cost" localSheetId="0">Price!$B$63</definedName>
@@ -51,7 +51,7 @@
     <definedName name="fixed_dep" localSheetId="1">Finance!$B$14</definedName>
     <definedName name="fixing_probability">'[1]Crop Sim'!$O$358:$P$374</definedName>
     <definedName name="flagfall" localSheetId="0">Price!$B$34</definedName>
-    <definedName name="fuel_adj_tractor" localSheetId="5">'Mach 1'!$B$37</definedName>
+    <definedName name="fuel_adj_tractor" localSheetId="5">'Mach 1'!$B$39</definedName>
     <definedName name="fungi_control_bnds">'[1]Crop Sim'!$H$150:$K$166</definedName>
     <definedName name="fungi_control_params">'[1]Crop Sim'!$H$142:$Q$145</definedName>
     <definedName name="fungi_die">'[1]Crop Sim'!$G$225:$J$230</definedName>
@@ -61,13 +61,13 @@
     <definedName name="grain_income_date" localSheetId="0">Price!$B$36</definedName>
     <definedName name="grain_income_length" localSheetId="0">Price!$B$38</definedName>
     <definedName name="grain_price" localSheetId="0">Price!$A$48:$H$60</definedName>
-    <definedName name="harv_eff" localSheetId="5">'Mach 1'!$B$72</definedName>
-    <definedName name="harv_fuel_consumption" localSheetId="5">'Mach 1'!$B$68</definedName>
+    <definedName name="harv_eff" localSheetId="5">'Mach 1'!$B$74</definedName>
+    <definedName name="harv_fuel_consumption" localSheetId="5">'Mach 1'!$B$70</definedName>
     <definedName name="harvest_index">'[1]Crop Sim'!$L$358:$M$374</definedName>
-    <definedName name="harvest_maint" localSheetId="5">'Mach 1'!$A$86:$B$96</definedName>
-    <definedName name="harvest_speed" localSheetId="5">'Mach 1'!$A$74:$B$84</definedName>
+    <definedName name="harvest_maint" localSheetId="5">'Mach 1'!$A$88:$B$98</definedName>
+    <definedName name="harvest_speed" localSheetId="5">'Mach 1'!$A$76:$B$86</definedName>
     <definedName name="harvest_yield" localSheetId="4">'Mach General'!$A$6:$B$16</definedName>
-    <definedName name="harvester_width" localSheetId="5">'Mach 1'!$B$66</definedName>
+    <definedName name="harvester_width" localSheetId="5">'Mach 1'!$B$68</definedName>
     <definedName name="initial_fungus">'[1]Crop Sim'!#REF!</definedName>
     <definedName name="initial_weed">'[1]Crop Sim'!#REF!</definedName>
     <definedName name="insurance_date">'Mach General'!$B$35</definedName>
@@ -79,8 +79,8 @@
     <definedName name="nitrogen_removed_harvest">'[1]Crop Sim'!$I$313:$I$341</definedName>
     <definedName name="nutrient_leach">'[1]Crop Sim'!$L$307</definedName>
     <definedName name="nutrient_yield_params">'[1]Crop Sim'!$H$279:$J$295</definedName>
-    <definedName name="oil_grease_factor_harv" localSheetId="5">'Mach 1'!$B$70</definedName>
-    <definedName name="oil_grease_factor_tractor" localSheetId="5">'Mach 1'!$B$24</definedName>
+    <definedName name="oil_grease_factor_harv" localSheetId="5">'Mach 1'!$B$72</definedName>
+    <definedName name="oil_grease_factor_tractor" localSheetId="5">'Mach 1'!$B$26</definedName>
     <definedName name="opportunity_cost_capital">Finance!$B$8</definedName>
     <definedName name="pasture_biomass">'[1]Crop Sim'!$H$358:$I$371</definedName>
     <definedName name="pasture_control">'[1]Crop Sim'!#REF!</definedName>
@@ -88,7 +88,7 @@
     <definedName name="permanent_ls_leave">Price!$B$84</definedName>
     <definedName name="permanent_super">Price!$B$80</definedName>
     <definedName name="permanent_workers_comp">Price!$B$82</definedName>
-    <definedName name="repair_maint_factor_tractor" localSheetId="5">'Mach 1'!$B$26</definedName>
+    <definedName name="repair_maint_factor_tractor" localSheetId="5">'Mach 1'!$B$28</definedName>
     <definedName name="ria" localSheetId="2">'Feed Budget'!$H$3</definedName>
     <definedName name="rib" localSheetId="2">'Feed Budget'!$H$5</definedName>
     <definedName name="rid" localSheetId="2">'Feed Budget'!$H$13</definedName>
@@ -98,34 +98,34 @@
     <definedName name="seed_set">'[1]Crop Sim'!$K$119:$M$121</definedName>
     <definedName name="seedbank_value">'[1]Crop Sim'!$G$119:$I$121</definedName>
     <definedName name="seeder_base_crop" localSheetId="5">'Mach 1'!#REF!</definedName>
-    <definedName name="seeder_speed_base" localSheetId="5">'Mach 1'!$B$33</definedName>
-    <definedName name="seeder_speed_crop_adj" localSheetId="5">'Mach 1'!$A$41:$B$63</definedName>
-    <definedName name="seeder_width" localSheetId="5">'Mach 1'!$B$29</definedName>
-    <definedName name="seeding_eff" localSheetId="5">'Mach 1'!$B$31</definedName>
+    <definedName name="seeder_speed_base" localSheetId="5">'Mach 1'!$B$35</definedName>
+    <definedName name="seeder_speed_crop_adj" localSheetId="5">'Mach 1'!$A$43:$B$65</definedName>
+    <definedName name="seeder_width" localSheetId="5">'Mach 1'!$B$31</definedName>
+    <definedName name="seeding_eff" localSheetId="5">'Mach 1'!$B$33</definedName>
     <definedName name="seeds_die">'[1]Crop Sim'!$W$119:$Y$121</definedName>
     <definedName name="seeds_soften">'[1]Crop Sim'!$O$119:$Q$120</definedName>
     <definedName name="seedset_min">'[1]Crop Sim'!$L$125:$M$125</definedName>
     <definedName name="seedset_slope">'[1]Crop Sim'!$L$123:$M$123</definedName>
     <definedName name="Soil_nitrate_slope">'[1]Crop Sim'!$N$389:$N$417</definedName>
-    <definedName name="sprayer_eff" localSheetId="5">'Mach 1'!$B$103</definedName>
-    <definedName name="sprayer_fuel_consumption" localSheetId="5">'Mach 1'!$B$105</definedName>
-    <definedName name="sprayer_maint" localSheetId="5">'Mach 1'!$B$107</definedName>
-    <definedName name="sprayer_speed" localSheetId="5">'Mach 1'!$B$101</definedName>
-    <definedName name="sprayer_width" localSheetId="5">'Mach 1'!$B$99</definedName>
-    <definedName name="spreader_cap" localSheetId="5">'Mach 1'!$B$121</definedName>
-    <definedName name="spreader_eff" localSheetId="5">'Mach 1'!$B$127</definedName>
-    <definedName name="spreader_fuel" localSheetId="5">'Mach 1'!$B$110</definedName>
-    <definedName name="spreader_maint" localSheetId="5">'Mach 1'!$B$129</definedName>
-    <definedName name="spreader_speed" localSheetId="5">'Mach 1'!$B$125</definedName>
-    <definedName name="spreader_width" localSheetId="5">'Mach 1'!$A$112:$B$119</definedName>
-    <definedName name="stubble_fuel_consumption" localSheetId="5">'Mach 1'!$B$132</definedName>
-    <definedName name="stubble_maint" localSheetId="5">'Mach 1'!$B$134</definedName>
+    <definedName name="sprayer_eff" localSheetId="5">'Mach 1'!$B$105</definedName>
+    <definedName name="sprayer_fuel_consumption" localSheetId="5">'Mach 1'!$B$107</definedName>
+    <definedName name="sprayer_maint" localSheetId="5">'Mach 1'!$B$109</definedName>
+    <definedName name="sprayer_speed" localSheetId="5">'Mach 1'!$B$103</definedName>
+    <definedName name="sprayer_width" localSheetId="5">'Mach 1'!$B$101</definedName>
+    <definedName name="spreader_cap" localSheetId="5">'Mach 1'!$B$123</definedName>
+    <definedName name="spreader_eff" localSheetId="5">'Mach 1'!$B$129</definedName>
+    <definedName name="spreader_fuel" localSheetId="5">'Mach 1'!$B$112</definedName>
+    <definedName name="spreader_maint" localSheetId="5">'Mach 1'!$B$131</definedName>
+    <definedName name="spreader_speed" localSheetId="5">'Mach 1'!$B$127</definedName>
+    <definedName name="spreader_width" localSheetId="5">'Mach 1'!$A$114:$B$121</definedName>
+    <definedName name="stubble_fuel_consumption" localSheetId="5">'Mach 1'!$B$134</definedName>
+    <definedName name="stubble_maint" localSheetId="5">'Mach 1'!$B$136</definedName>
     <definedName name="sup_cartage">Price!$B$29</definedName>
-    <definedName name="sup_feed">'Mach 1'!$A$137:$C$142</definedName>
+    <definedName name="sup_feed">'Mach 1'!$A$139:$C$144</definedName>
     <definedName name="sup_md_vol">'Sup Feed'!$I$10:$N$14</definedName>
     <definedName name="sup_transaction">Price!$B$31</definedName>
-    <definedName name="tillage_maint" localSheetId="5">'Mach 1'!$B$39</definedName>
-    <definedName name="time_fill_spreader" localSheetId="5">'Mach 1'!$B$123</definedName>
+    <definedName name="tillage_maint" localSheetId="5">'Mach 1'!$B$41</definedName>
+    <definedName name="time_fill_spreader" localSheetId="5">'Mach 1'!$B$125</definedName>
     <definedName name="variable_dep" localSheetId="1">Finance!#REF!</definedName>
     <definedName name="variable_dep" localSheetId="5">'Mach 1'!$B$5</definedName>
     <definedName name="weed_control_bnds">'[1]Crop Sim'!$H$54:$M$70</definedName>
@@ -1137,6 +1137,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Michael Young</author>
+    <author>Michael Young (21512438)</author>
   </authors>
   <commentList>
     <comment ref="A3" authorId="0" shapeId="0" xr:uid="{AAFD58D5-AE8A-4CCB-9657-C9B138C0F600}">
@@ -1211,6 +1212,79 @@
         </r>
       </text>
     </comment>
+    <comment ref="C8" authorId="1" shapeId="0" xr:uid="{60CA65AB-9005-43D6-981C-D34614945B09}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Percentage of the machine use due to seeding. Eg the proportion of variable dep is linked to the seeding activity.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="1" shapeId="0" xr:uid="{512FCC53-D489-4227-AFDD-2A231783071D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Proportion of machine use linked to harvest. Eg the proportion of variable dep is linked to the harvest activity.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="1" shapeId="0" xr:uid="{142C03D0-CD7D-4D43-82B5-909B38ED74DC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Percentage of the machine use for general farm activities. General farm activities don’t incur a variable level of depreciation. 
+Note machinery that doesn’t depreciate at a variable rate due to use eg silos can be given 100% allocation to this column</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="A9" authorId="0" shapeId="0" xr:uid="{B1CD0B29-B678-4B5A-AA05-C495717C8637}">
       <text>
         <r>
@@ -1231,11 +1305,83 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-main seeding tractor</t>
+big seeding tractor</t>
         </r>
       </text>
     </comment>
-    <comment ref="A18" authorId="0" shapeId="0" xr:uid="{2E8F9219-EF4F-48DB-BEAB-A7DDA35A3529}">
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{63D0F056-E26C-46D3-8557-96C8BEB1E8FD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Young:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+main tractor for spreading, spraying and chasing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C14" authorId="1" shapeId="0" xr:uid="{13AA0056-5E9D-4DD0-8975-6AAC46C7E0AD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+some used for pasture</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C15" authorId="1" shapeId="0" xr:uid="{022DE70A-A426-4215-B248-2D3B732C2C26}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Young (21512438):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+some used for pasture</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{2E8F9219-EF4F-48DB-BEAB-A7DDA35A3529}">
       <text>
         <r>
           <rPr>
@@ -1259,7 +1405,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{D1EE20E3-0899-4EB4-8B3A-EBF28636B900}">
+    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{D1EE20E3-0899-4EB4-8B3A-EBF28636B900}">
       <text>
         <r>
           <rPr>
@@ -1283,7 +1429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{B837A070-290A-48FE-A9F1-FF65B147DD8B}">
+    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{B837A070-290A-48FE-A9F1-FF65B147DD8B}">
       <text>
         <r>
           <rPr>
@@ -1307,7 +1453,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A24" authorId="0" shapeId="0" xr:uid="{88E31DB9-DA47-4E21-BBD8-CD082FA0D083}">
+    <comment ref="A26" authorId="0" shapeId="0" xr:uid="{88E31DB9-DA47-4E21-BBD8-CD082FA0D083}">
       <text>
         <r>
           <rPr>
@@ -1331,7 +1477,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A26" authorId="0" shapeId="0" xr:uid="{E2D5BC6F-CCAD-4F63-8FF3-AA1DB42A285A}">
+    <comment ref="A28" authorId="0" shapeId="0" xr:uid="{E2D5BC6F-CCAD-4F63-8FF3-AA1DB42A285A}">
       <text>
         <r>
           <rPr>
@@ -1356,7 +1502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{8508D24F-9890-44FB-AEA6-F6DFD7537CC2}">
+    <comment ref="A31" authorId="0" shapeId="0" xr:uid="{8508D24F-9890-44FB-AEA6-F6DFD7537CC2}">
       <text>
         <r>
           <rPr>
@@ -1380,7 +1526,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A31" authorId="0" shapeId="0" xr:uid="{61C90CFE-2D29-4907-B6CD-9319DAACEBD8}">
+    <comment ref="A33" authorId="0" shapeId="0" xr:uid="{61C90CFE-2D29-4907-B6CD-9319DAACEBD8}">
       <text>
         <r>
           <rPr>
@@ -1404,7 +1550,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A33" authorId="0" shapeId="0" xr:uid="{A65873CF-555B-4A86-994C-DC10556614E7}">
+    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{A65873CF-555B-4A86-994C-DC10556614E7}">
       <text>
         <r>
           <rPr>
@@ -1430,7 +1576,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A35" authorId="0" shapeId="0" xr:uid="{CF28C5E3-D67E-4632-8284-686686CDBFBF}">
+    <comment ref="A37" authorId="0" shapeId="0" xr:uid="{CF28C5E3-D67E-4632-8284-686686CDBFBF}">
       <text>
         <r>
           <rPr>
@@ -1456,7 +1602,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A37" authorId="0" shapeId="0" xr:uid="{FF459000-A9AD-4E46-98CA-516097035559}">
+    <comment ref="A39" authorId="0" shapeId="0" xr:uid="{FF459000-A9AD-4E46-98CA-516097035559}">
       <text>
         <r>
           <rPr>
@@ -1482,7 +1628,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A39" authorId="0" shapeId="0" xr:uid="{06A5A63E-B372-4BF7-8C8B-09E9186996AD}">
+    <comment ref="A41" authorId="0" shapeId="0" xr:uid="{06A5A63E-B372-4BF7-8C8B-09E9186996AD}">
       <text>
         <r>
           <rPr>
@@ -1508,7 +1654,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A41" authorId="0" shapeId="0" xr:uid="{F5C1B9DC-66F6-4DF8-8092-3844E8687AAB}">
+    <comment ref="A43" authorId="0" shapeId="0" xr:uid="{F5C1B9DC-66F6-4DF8-8092-3844E8687AAB}">
       <text>
         <r>
           <rPr>
@@ -1533,7 +1679,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{EB3EC863-815A-4F07-ADF1-BACEDBEA528E}">
+    <comment ref="A68" authorId="0" shapeId="0" xr:uid="{EB3EC863-815A-4F07-ADF1-BACEDBEA528E}">
       <text>
         <r>
           <rPr>
@@ -1557,7 +1703,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A68" authorId="0" shapeId="0" xr:uid="{3377AFBB-BAF8-4184-9D43-0D43F3CF0BCD}">
+    <comment ref="A70" authorId="0" shapeId="0" xr:uid="{3377AFBB-BAF8-4184-9D43-0D43F3CF0BCD}">
       <text>
         <r>
           <rPr>
@@ -1581,7 +1727,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B68" authorId="0" shapeId="0" xr:uid="{8F650DD9-B6D6-4B19-A197-CD333C815375}">
+    <comment ref="B70" authorId="0" shapeId="0" xr:uid="{8F650DD9-B6D6-4B19-A197-CD333C815375}">
       <text>
         <r>
           <rPr>
@@ -1606,7 +1752,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A70" authorId="0" shapeId="0" xr:uid="{1F923DBF-9E7F-4464-8708-2B0AF1340A76}">
+    <comment ref="A72" authorId="0" shapeId="0" xr:uid="{1F923DBF-9E7F-4464-8708-2B0AF1340A76}">
       <text>
         <r>
           <rPr>
@@ -1630,7 +1776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A72" authorId="0" shapeId="0" xr:uid="{925041D9-BB4A-4730-BA16-A60ED3E49090}">
+    <comment ref="A74" authorId="0" shapeId="0" xr:uid="{925041D9-BB4A-4730-BA16-A60ED3E49090}">
       <text>
         <r>
           <rPr>
@@ -1654,7 +1800,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A74" authorId="0" shapeId="0" xr:uid="{83C78BD9-1F45-41C1-83A8-FF872B400F8F}">
+    <comment ref="A76" authorId="0" shapeId="0" xr:uid="{83C78BD9-1F45-41C1-83A8-FF872B400F8F}">
       <text>
         <r>
           <rPr>
@@ -1679,7 +1825,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A86" authorId="0" shapeId="0" xr:uid="{03C07A35-AAEB-46EF-9545-55B9E522D28F}">
+    <comment ref="A88" authorId="0" shapeId="0" xr:uid="{03C07A35-AAEB-46EF-9545-55B9E522D28F}">
       <text>
         <r>
           <rPr>
@@ -1704,7 +1850,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A99" authorId="0" shapeId="0" xr:uid="{821E0CE2-6A9B-42C2-9F86-0C81A466AB82}">
+    <comment ref="A101" authorId="0" shapeId="0" xr:uid="{821E0CE2-6A9B-42C2-9F86-0C81A466AB82}">
       <text>
         <r>
           <rPr>
@@ -1728,7 +1874,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A101" authorId="0" shapeId="0" xr:uid="{D25B8429-9410-44C7-8574-A6DC0E08A456}">
+    <comment ref="A103" authorId="0" shapeId="0" xr:uid="{D25B8429-9410-44C7-8574-A6DC0E08A456}">
       <text>
         <r>
           <rPr>
@@ -1752,7 +1898,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A103" authorId="0" shapeId="0" xr:uid="{BB9ACD3C-8B60-44E6-911C-6ADC9B17BEE9}">
+    <comment ref="A105" authorId="0" shapeId="0" xr:uid="{BB9ACD3C-8B60-44E6-911C-6ADC9B17BEE9}">
       <text>
         <r>
           <rPr>
@@ -1776,7 +1922,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A105" authorId="0" shapeId="0" xr:uid="{8AE1C4AE-C9A6-42B8-87F4-4B73EC5E1B5E}">
+    <comment ref="A107" authorId="0" shapeId="0" xr:uid="{8AE1C4AE-C9A6-42B8-87F4-4B73EC5E1B5E}">
       <text>
         <r>
           <rPr>
@@ -1800,7 +1946,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A107" authorId="0" shapeId="0" xr:uid="{64BD9D49-D5FD-46A7-90EB-ABA6BC4DD5BF}">
+    <comment ref="A109" authorId="0" shapeId="0" xr:uid="{64BD9D49-D5FD-46A7-90EB-ABA6BC4DD5BF}">
       <text>
         <r>
           <rPr>
@@ -1824,7 +1970,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A110" authorId="0" shapeId="0" xr:uid="{B3CC4513-8BFF-4910-ABF7-F746405E57E7}">
+    <comment ref="A112" authorId="0" shapeId="0" xr:uid="{B3CC4513-8BFF-4910-ABF7-F746405E57E7}">
       <text>
         <r>
           <rPr>
@@ -1848,7 +1994,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A112" authorId="0" shapeId="0" xr:uid="{4922BC00-7562-4251-AF4D-B71E622B07C0}">
+    <comment ref="A114" authorId="0" shapeId="0" xr:uid="{4922BC00-7562-4251-AF4D-B71E622B07C0}">
       <text>
         <r>
           <rPr>
@@ -1873,7 +2019,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A121" authorId="0" shapeId="0" xr:uid="{22E62F09-30E0-4CD0-81DE-F02394555AD3}">
+    <comment ref="A123" authorId="0" shapeId="0" xr:uid="{22E62F09-30E0-4CD0-81DE-F02394555AD3}">
       <text>
         <r>
           <rPr>
@@ -1897,7 +2043,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A123" authorId="0" shapeId="0" xr:uid="{AF9CD173-26D1-4803-84AA-A1C88C31B999}">
+    <comment ref="A125" authorId="0" shapeId="0" xr:uid="{AF9CD173-26D1-4803-84AA-A1C88C31B999}">
       <text>
         <r>
           <rPr>
@@ -1921,7 +2067,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A125" authorId="0" shapeId="0" xr:uid="{B466F8A9-62FF-4035-B41F-6123131A64B2}">
+    <comment ref="A127" authorId="0" shapeId="0" xr:uid="{B466F8A9-62FF-4035-B41F-6123131A64B2}">
       <text>
         <r>
           <rPr>
@@ -1945,7 +2091,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A127" authorId="0" shapeId="0" xr:uid="{D36EEB6F-4421-421C-BD2B-38C8EED80323}">
+    <comment ref="A129" authorId="0" shapeId="0" xr:uid="{D36EEB6F-4421-421C-BD2B-38C8EED80323}">
       <text>
         <r>
           <rPr>
@@ -1969,7 +2115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A129" authorId="0" shapeId="0" xr:uid="{476F3EA8-18FE-4BF1-857E-DB0233D5DFAB}">
+    <comment ref="A131" authorId="0" shapeId="0" xr:uid="{476F3EA8-18FE-4BF1-857E-DB0233D5DFAB}">
       <text>
         <r>
           <rPr>
@@ -1993,7 +2139,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A132" authorId="0" shapeId="0" xr:uid="{9163A97B-97F8-4781-A636-98B9A4B8C98E}">
+    <comment ref="A134" authorId="0" shapeId="0" xr:uid="{9163A97B-97F8-4781-A636-98B9A4B8C98E}">
       <text>
         <r>
           <rPr>
@@ -2017,7 +2163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A134" authorId="0" shapeId="0" xr:uid="{30ECEA2E-A5CE-459D-8EC2-C4E59BCFCA95}">
+    <comment ref="A136" authorId="0" shapeId="0" xr:uid="{30ECEA2E-A5CE-459D-8EC2-C4E59BCFCA95}">
       <text>
         <r>
           <rPr>
@@ -2041,7 +2187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B137" authorId="0" shapeId="0" xr:uid="{115DEECC-C4B6-40BD-AC87-F415E26BB0BB}">
+    <comment ref="B139" authorId="0" shapeId="0" xr:uid="{115DEECC-C4B6-40BD-AC87-F415E26BB0BB}">
       <text>
         <r>
           <rPr>
@@ -2065,7 +2211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C137" authorId="0" shapeId="0" xr:uid="{735B890C-028D-403F-91EB-7DDBBB95923A}">
+    <comment ref="C139" authorId="0" shapeId="0" xr:uid="{735B890C-028D-403F-91EB-7DDBBB95923A}">
       <text>
         <r>
           <rPr>
@@ -2094,7 +2240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="193">
   <si>
     <t>Machinery</t>
   </si>
@@ -2177,9 +2323,6 @@
     <t>Tractor</t>
   </si>
   <si>
-    <t>tractor</t>
-  </si>
-  <si>
     <t>seeder</t>
   </si>
   <si>
@@ -2658,6 +2801,24 @@
   </si>
   <si>
     <t>$/hr</t>
+  </si>
+  <si>
+    <t>chaser bin</t>
+  </si>
+  <si>
+    <t>seeding allocation</t>
+  </si>
+  <si>
+    <t>remaining allocation</t>
+  </si>
+  <si>
+    <t>harvest allocation</t>
+  </si>
+  <si>
+    <t>tractor 1</t>
+  </si>
+  <si>
+    <t>tractor 2</t>
   </si>
 </sst>
 </file>
@@ -3167,14 +3328,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>207010</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
@@ -3191,8 +3352,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4145280" y="60960"/>
-          <a:ext cx="2613660" cy="1257300"/>
+          <a:off x="5842000" y="60960"/>
+          <a:ext cx="2639060" cy="1263650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6203,6 +6364,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6505,30 +6670,30 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -6539,8 +6704,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -6551,13 +6716,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -6568,7 +6733,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -6579,7 +6744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -6590,7 +6755,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -6601,7 +6766,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -6612,7 +6777,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -6623,7 +6788,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
@@ -6634,9 +6799,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" s="4">
         <v>300</v>
@@ -6645,9 +6810,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B16" s="4">
         <v>300</v>
@@ -6656,9 +6821,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="4">
         <v>300</v>
@@ -6667,7 +6832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>12</v>
       </c>
@@ -6678,13 +6843,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
@@ -6695,8 +6860,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
@@ -6707,8 +6872,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>16</v>
       </c>
@@ -6719,14 +6884,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B29" s="8">
         <v>15</v>
@@ -6735,12 +6900,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="6.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B31" s="8">
         <v>20</v>
@@ -6749,75 +6914,75 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B34" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B36" s="6">
         <v>43814</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B38" s="4">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B40" s="6">
         <v>43692</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="B42" s="48" t="s">
+      <c r="C42" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="48" t="s">
-        <v>93</v>
-      </c>
       <c r="D42" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="E42" s="48" t="s">
+      <c r="F42" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="F42" s="48" t="s">
+      <c r="G42" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="G42" s="48" t="s">
-        <v>101</v>
-      </c>
       <c r="H42" s="48" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B43" s="50">
         <f>AVERAGE(B49,B51,B59)</f>
@@ -6848,9 +7013,9 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="49" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B44" s="50">
         <f>AVERAGE(B57,B60)</f>
@@ -6881,9 +7046,9 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="49" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B45" s="50">
         <f>AVERAGE(B50,B52:B54,B58)</f>
@@ -6914,12 +7079,12 @@
         <v>1.0920000000000001</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B46" s="50">
         <f>AVERAGE(B49:B60)</f>
@@ -6950,36 +7115,36 @@
         <v>0.93800000000000028</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="D48" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="F48" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="G48" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="G48" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="H48" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>4</v>
       </c>
@@ -7007,7 +7172,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>10</v>
       </c>
@@ -7035,9 +7200,9 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B51" s="4">
         <v>150</v>
@@ -7063,9 +7228,9 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B52" s="4">
         <v>350</v>
@@ -7091,9 +7256,9 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B53" s="4">
         <v>350</v>
@@ -7119,7 +7284,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
@@ -7147,7 +7312,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>6</v>
       </c>
@@ -7175,9 +7340,9 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B56" s="4">
         <v>300</v>
@@ -7202,7 +7367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>9</v>
       </c>
@@ -7230,9 +7395,9 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B58" s="4">
         <v>350</v>
@@ -7258,7 +7423,7 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>5</v>
       </c>
@@ -7286,7 +7451,7 @@
         <v>0.90300000000000002</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>8</v>
       </c>
@@ -7314,150 +7479,150 @@
         <v>1.0920000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" s="5" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="B63" s="4">
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="9.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B65" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B65" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B66" s="4">
         <v>15</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67" s="4">
         <v>541</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" s="4">
         <v>339</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B69" s="4">
         <v>780</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B70" s="4">
         <v>550</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B71" s="4">
         <v>500</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B72" s="4">
         <v>520</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B76" s="4">
         <v>80000</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B78" s="4">
         <v>80000</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B80" s="52">
         <v>0.09</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B82" s="52">
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B84" s="4">
         <v>2.3E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B86" s="4">
         <v>28</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B88" s="52">
         <v>0.09</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B90" s="52">
         <v>3.5000000000000003E-2</v>
@@ -7479,18 +7644,18 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -7498,8 +7663,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -7507,38 +7672,38 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B8" s="46">
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B11" s="46">
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>23</v>
       </c>
@@ -7546,14 +7711,14 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B17" s="46">
         <v>0.02</v>
@@ -7573,77 +7738,77 @@
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="2" style="1" customWidth="1"/>
-    <col min="3" max="3" width="0.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="2.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="1.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.28515625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="0.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="1.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.26953125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="7:8" x14ac:dyDescent="0.35">
       <c r="H1" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="7:8" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G2" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G3" s="5" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="7:8" x14ac:dyDescent="0.25">
-      <c r="G3" s="5" t="s">
-        <v>111</v>
       </c>
       <c r="H3" s="4">
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="7:8" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="7:8" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G5" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H5" s="4">
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G7" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H7" s="4">
         <v>1.4</v>
       </c>
     </row>
-    <row r="8" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G9" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H9" s="4">
         <v>1.7</v>
       </c>
     </row>
-    <row r="10" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G11" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H11" s="4">
         <v>0.17</v>
       </c>
     </row>
-    <row r="12" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="7:8" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G13" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H13" s="4">
         <v>0.8</v>
@@ -7663,16 +7828,16 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" customWidth="1"/>
-    <col min="2" max="2" width="2.28515625" customWidth="1"/>
-    <col min="3" max="4" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" customWidth="1"/>
+    <col min="2" max="2" width="2.26953125" customWidth="1"/>
+    <col min="3" max="4" width="2.7265625" customWidth="1"/>
     <col min="5" max="5" width="2" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="4.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11"/>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -7700,7 +7865,7 @@
       <c r="Y1" s="12"/>
       <c r="Z1" s="12"/>
     </row>
-    <row r="2" spans="1:26" ht="5.0999999999999996" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="5.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -7728,11 +7893,11 @@
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
     </row>
-    <row r="3" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11"/>
       <c r="B3" s="12"/>
       <c r="C3" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="14"/>
@@ -7758,17 +7923,17 @@
       <c r="Y3" s="13"/>
       <c r="Z3" s="13"/>
     </row>
-    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F4" s="18"/>
       <c r="G4" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H4" s="18"/>
       <c r="I4" s="18"/>
@@ -7790,7 +7955,7 @@
       <c r="Y4" s="13"/>
       <c r="Z4" s="13"/>
     </row>
-    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="17"/>
@@ -7798,7 +7963,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H5" s="18"/>
       <c r="I5" s="18"/>
@@ -7820,7 +7985,7 @@
       <c r="Y5" s="13"/>
       <c r="Z5" s="13"/>
     </row>
-    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11"/>
       <c r="B6" s="12"/>
       <c r="C6" s="22"/>
@@ -7850,7 +8015,7 @@
       <c r="Y6" s="13"/>
       <c r="Z6" s="13"/>
     </row>
-    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="22"/>
@@ -7878,7 +8043,7 @@
       <c r="Y7" s="13"/>
       <c r="Z7" s="13"/>
     </row>
-    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="22"/>
@@ -7906,7 +8071,7 @@
       <c r="Y8" s="13"/>
       <c r="Z8" s="13"/>
     </row>
-    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="22"/>
@@ -7934,7 +8099,7 @@
       <c r="Y9" s="13"/>
       <c r="Z9" s="13"/>
     </row>
-    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="22"/>
@@ -7957,7 +8122,7 @@
         <v>5</v>
       </c>
       <c r="N10" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O10" s="27"/>
       <c r="P10" s="27"/>
@@ -7972,7 +8137,7 @@
       <c r="Y10" s="13"/>
       <c r="Z10" s="13"/>
     </row>
-    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="22"/>
@@ -7981,7 +8146,7 @@
       <c r="F11" s="28"/>
       <c r="H11" s="32"/>
       <c r="I11" s="45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J11" s="33">
         <v>11400</v>
@@ -7999,7 +8164,7 @@
         <v>7000</v>
       </c>
       <c r="O11" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P11" s="34"/>
       <c r="Q11" s="34"/>
@@ -8013,7 +8178,7 @@
       <c r="Y11" s="13"/>
       <c r="Z11" s="13"/>
     </row>
-    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="22"/>
@@ -8022,7 +8187,7 @@
       <c r="F12" s="28"/>
       <c r="H12" s="32"/>
       <c r="I12" s="45" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J12" s="33">
         <v>0.1</v>
@@ -8052,7 +8217,7 @@
       <c r="Y12" s="13"/>
       <c r="Z12" s="13"/>
     </row>
-    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="22"/>
@@ -8061,7 +8226,7 @@
       <c r="F13" s="28"/>
       <c r="H13" s="32"/>
       <c r="I13" s="45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J13" s="47">
         <v>0.9</v>
@@ -8079,7 +8244,7 @@
         <v>0.9</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P13" s="34"/>
       <c r="Q13" s="34"/>
@@ -8093,7 +8258,7 @@
       <c r="Y13" s="13"/>
       <c r="Z13" s="13"/>
     </row>
-    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="11"/>
       <c r="B14" s="12"/>
       <c r="C14" s="22"/>
@@ -8102,7 +8267,7 @@
       <c r="F14" s="28"/>
       <c r="H14" s="32"/>
       <c r="I14" s="45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J14" s="47">
         <v>0.8</v>
@@ -8120,7 +8285,7 @@
         <v>0.75</v>
       </c>
       <c r="O14" s="32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P14" s="34"/>
       <c r="Q14" s="34"/>
@@ -8134,7 +8299,7 @@
       <c r="Y14" s="13"/>
       <c r="Z14" s="13"/>
     </row>
-    <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="C15" s="22"/>
@@ -8162,7 +8327,7 @@
       <c r="Y15" s="13"/>
       <c r="Z15" s="13"/>
     </row>
-    <row r="16" spans="1:26" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="5.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11"/>
       <c r="B16" s="12"/>
       <c r="C16" s="22"/>
@@ -8190,7 +8355,7 @@
       <c r="Y16" s="13"/>
       <c r="Z16" s="13"/>
     </row>
-    <row r="17" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="C17" s="40"/>
@@ -8217,13 +8382,13 @@
       <c r="U17" s="40"/>
       <c r="V17" s="40"/>
       <c r="W17" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
       <c r="Z17" s="13"/>
     </row>
-    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -8251,7 +8416,7 @@
       <c r="Y18" s="13"/>
       <c r="Z18" s="13"/>
     </row>
-    <row r="19" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -8279,11 +8444,11 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11"/>
       <c r="B20" s="12"/>
       <c r="C20" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
@@ -8309,17 +8474,17 @@
       <c r="Y20" s="13"/>
       <c r="Z20" s="13"/>
     </row>
-    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11"/>
       <c r="B21" s="12"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H21" s="18"/>
       <c r="I21" s="18"/>
@@ -8341,7 +8506,7 @@
       <c r="Y21" s="13"/>
       <c r="Z21" s="13"/>
     </row>
-    <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="17"/>
@@ -8349,7 +8514,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="18"/>
       <c r="G22" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H22" s="18"/>
       <c r="I22" s="18"/>
@@ -8371,7 +8536,7 @@
       <c r="Y22" s="13"/>
       <c r="Z22" s="13"/>
     </row>
-    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="11"/>
       <c r="B23" s="12"/>
       <c r="C23" s="22"/>
@@ -8401,7 +8566,7 @@
       <c r="Y23" s="13"/>
       <c r="Z23" s="13"/>
     </row>
-    <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
       <c r="B24" s="12"/>
       <c r="C24" s="22"/>
@@ -8429,7 +8594,7 @@
       <c r="Y24" s="13"/>
       <c r="Z24" s="13"/>
     </row>
-    <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11"/>
       <c r="B25" s="12"/>
       <c r="C25" s="22"/>
@@ -8457,7 +8622,7 @@
       <c r="Y25" s="13"/>
       <c r="Z25" s="13"/>
     </row>
-    <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="12"/>
       <c r="C26" s="22"/>
@@ -8467,7 +8632,7 @@
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J26" s="26" t="s">
         <v>6</v>
@@ -8482,7 +8647,7 @@
         <v>5</v>
       </c>
       <c r="N26" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O26" s="27"/>
       <c r="P26" s="27"/>
@@ -8497,7 +8662,7 @@
       <c r="Y26" s="13"/>
       <c r="Z26" s="13"/>
     </row>
-    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="12"/>
       <c r="C27" s="22"/>
@@ -8507,22 +8672,22 @@
       <c r="G27" s="29"/>
       <c r="H27" s="29"/>
       <c r="I27" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J27" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K27" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L27" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M27" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N27" s="30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O27" s="30"/>
       <c r="P27" s="30"/>
@@ -8537,7 +8702,7 @@
       <c r="Y27" s="13"/>
       <c r="Z27" s="13"/>
     </row>
-    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="22"/>
@@ -8546,7 +8711,7 @@
       <c r="F28" s="28"/>
       <c r="H28" s="32"/>
       <c r="I28" s="45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="J28" s="44">
         <v>0.45</v>
@@ -8564,7 +8729,7 @@
         <v>1</v>
       </c>
       <c r="O28" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P28" s="34"/>
       <c r="Q28" s="34"/>
@@ -8578,7 +8743,7 @@
       <c r="Y28" s="13"/>
       <c r="Z28" s="13"/>
     </row>
-    <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11"/>
       <c r="B29" s="12"/>
       <c r="C29" s="22"/>
@@ -8606,7 +8771,7 @@
       <c r="Y29" s="13"/>
       <c r="Z29" s="13"/>
     </row>
-    <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11"/>
       <c r="B30" s="12"/>
       <c r="C30" s="22"/>
@@ -8634,7 +8799,7 @@
       <c r="Y30" s="13"/>
       <c r="Z30" s="13"/>
     </row>
-    <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11"/>
       <c r="B31" s="12"/>
       <c r="C31" s="40"/>
@@ -8661,13 +8826,13 @@
       <c r="U31" s="40"/>
       <c r="V31" s="40"/>
       <c r="W31" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="X31" s="13"/>
       <c r="Y31" s="13"/>
       <c r="Z31" s="13"/>
     </row>
-    <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -8710,41 +8875,41 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="24.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="B3" s="4">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="9.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="9.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -8752,7 +8917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -8760,7 +8925,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -8768,7 +8933,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -8776,7 +8941,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -8784,7 +8949,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
@@ -8792,7 +8957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -8800,60 +8965,60 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B15" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="B19" s="4">
         <v>12.2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="4"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>5</v>
       </c>
@@ -8861,7 +9026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>4</v>
       </c>
@@ -8869,7 +9034,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>6</v>
       </c>
@@ -8877,7 +9042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>8</v>
       </c>
@@ -8885,7 +9050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>9</v>
       </c>
@@ -8893,7 +9058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
@@ -8901,7 +9066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>10</v>
       </c>
@@ -8909,33 +9074,33 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B31" s="4">
         <v>4.5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B32" s="4">
         <v>4.5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B33" s="4">
         <v>4.5</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B35" s="6">
         <v>43554</v>
@@ -8951,25 +9116,28 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A689975D-2450-4766-909D-59787FB65B03}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A2:C142"/>
+  <dimension ref="A2:E144"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="B127" sqref="B127"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="26" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="13.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.36328125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -8980,878 +9148,1030 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="6.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="6.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="52">
         <v>0.08</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>191</v>
       </c>
       <c r="B9" s="4">
         <v>188000</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="52">
+        <v>1</v>
+      </c>
+      <c r="D9" s="52">
+        <v>0</v>
+      </c>
+      <c r="E9" s="52">
+        <f>1-C9-D9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4">
         <v>87000</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="52">
+        <v>1</v>
+      </c>
+      <c r="D10" s="52">
+        <v>0</v>
+      </c>
+      <c r="E10" s="52">
+        <f t="shared" ref="E10:E23" si="0">1-C10-D10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="4">
         <v>297000</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="52">
+        <v>0</v>
+      </c>
+      <c r="D11" s="52">
+        <v>1</v>
+      </c>
+      <c r="E11" s="52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="4">
+        <v>30000</v>
+      </c>
+      <c r="C12" s="52">
+        <v>0</v>
+      </c>
+      <c r="D12" s="52">
+        <v>1</v>
+      </c>
+      <c r="E12" s="52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B13" s="4">
+        <v>188000</v>
+      </c>
+      <c r="C13" s="52">
+        <v>0.3</v>
+      </c>
+      <c r="D13" s="52">
+        <v>0.3</v>
+      </c>
+      <c r="E13" s="52">
+        <f t="shared" si="0"/>
+        <v>0.39999999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="4">
+        <v>90000</v>
+      </c>
+      <c r="C14" s="52">
+        <v>0.85</v>
+      </c>
+      <c r="D14" s="52">
+        <v>0</v>
+      </c>
+      <c r="E14" s="52">
+        <f t="shared" si="0"/>
+        <v>0.15000000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="4">
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="B15" s="4">
+        <v>35000</v>
+      </c>
+      <c r="C15" s="52">
+        <v>0.85</v>
+      </c>
+      <c r="D15" s="52">
+        <v>0</v>
+      </c>
+      <c r="E15" s="52">
+        <f t="shared" si="0"/>
+        <v>0.15000000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="4">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="B16" s="4">
+        <v>15000</v>
+      </c>
+      <c r="C16" s="52">
+        <v>0</v>
+      </c>
+      <c r="D16" s="52">
+        <v>0</v>
+      </c>
+      <c r="E16" s="52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="4">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="B17" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C17" s="52">
+        <v>0</v>
+      </c>
+      <c r="D17" s="52">
+        <v>0</v>
+      </c>
+      <c r="E17" s="52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="4">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="B18" s="4">
+        <v>75000</v>
+      </c>
+      <c r="C18" s="52">
+        <v>0</v>
+      </c>
+      <c r="D18" s="52">
+        <v>0</v>
+      </c>
+      <c r="E18" s="52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="4">
-        <v>75000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="B19" s="4">
+        <v>36000</v>
+      </c>
+      <c r="C19" s="52">
+        <v>0.3</v>
+      </c>
+      <c r="D19" s="52">
+        <v>0.3</v>
+      </c>
+      <c r="E19" s="52">
+        <f t="shared" si="0"/>
+        <v>0.39999999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B20" s="4">
+        <v>78000</v>
+      </c>
+      <c r="C20" s="52">
+        <v>0</v>
+      </c>
+      <c r="D20" s="52">
+        <v>0</v>
+      </c>
+      <c r="E20" s="52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="4">
+        <v>22000</v>
+      </c>
+      <c r="C21" s="52">
+        <v>0</v>
+      </c>
+      <c r="D21" s="52">
+        <v>0</v>
+      </c>
+      <c r="E21" s="52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="4">
+        <v>50000</v>
+      </c>
+      <c r="C22" s="52">
+        <v>0</v>
+      </c>
+      <c r="D22" s="52">
+        <v>0</v>
+      </c>
+      <c r="E22" s="52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="4">
         <v>36000</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="4">
-        <v>78000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="4">
-        <v>22000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="4">
-        <v>110000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="C23" s="52">
+        <v>0</v>
+      </c>
+      <c r="D23" s="52">
+        <v>0</v>
+      </c>
+      <c r="E23" s="52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="4">
-        <v>36000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="B26" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B28" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="4">
+        <v>12.2</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="4">
-        <v>1.25</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+    <row r="32" spans="1:5" ht="9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="4">
-        <v>12.2</v>
-      </c>
-      <c r="C29" s="1" t="s">
+      <c r="B33" s="4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="4">
+        <v>12</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B33" s="4">
-        <v>12</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>81</v>
-      </c>
-      <c r="B35">
-        <v>5.41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>80</v>
       </c>
       <c r="B37">
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5.41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>79</v>
       </c>
       <c r="B39">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41">
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B41" s="4"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="B42" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B43" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="B43" s="4"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B44" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B45" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B46" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B48" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B49" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B50" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B51" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>5</v>
+        <v>173</v>
       </c>
       <c r="B52" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
-        <v>4</v>
+        <v>174</v>
       </c>
       <c r="B53" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B54" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
       <c r="B55" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
-        <v>119</v>
+        <v>6</v>
       </c>
       <c r="B56" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="B57" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
       <c r="B58" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B59" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B60" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="B61" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="B62" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B63" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="3" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B64" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+      <c r="B68" s="4">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B66" s="4">
-        <v>12.2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+      <c r="B70" s="4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B68" s="4">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+      <c r="B72" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B70" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B72" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B74" s="4"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+      <c r="B76" s="4"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="B75" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B76" s="4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="B77" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78" s="4">
         <v>8</v>
       </c>
-      <c r="B78" s="4">
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="B79" s="4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B80" s="4">
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B81" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B82" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B81" s="4">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B82" s="4">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="B83" s="4">
         <v>5.5</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B84" s="4">
         <v>5.5</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B85" s="4">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B86" s="4"/>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B86" s="4">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B88" s="4"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="B87" s="4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B88" s="4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="4" t="s">
-        <v>6</v>
       </c>
       <c r="B89" s="4">
         <v>33</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B90" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B90" s="4">
+      <c r="B92" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="4" t="s">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B91" s="4">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B92" s="4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
-        <v>10</v>
       </c>
       <c r="B93" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="B94" s="4">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="B95" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B96" s="4">
         <v>38</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B97" s="4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B98" s="4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
+      <c r="B101" s="4">
+        <v>25</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B99" s="4">
-        <v>25</v>
-      </c>
-      <c r="C99" s="1" t="s">
+      <c r="B103" s="4">
+        <v>20</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
+    <row r="104" spans="1:3" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="B101" s="4">
-        <v>20</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B103" s="4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="4" t="s">
-        <v>58</v>
       </c>
       <c r="B105" s="4">
         <v>0.6</v>
       </c>
-      <c r="C105" s="1" t="s">
+    </row>
+    <row r="106" spans="1:3" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B107" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="3" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B109" s="4">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B112" s="4">
+        <v>11.3</v>
+      </c>
+      <c r="C112" s="1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B107" s="4">
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="4" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B110" s="4">
-        <v>11.3</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
+      <c r="B114" s="4"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="B112" s="4"/>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B113" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B114" s="4"/>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="4" t="s">
-        <v>64</v>
       </c>
       <c r="B115" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B116" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="B116" s="4"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B117" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B118" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B119" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B120" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B121" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B123" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B121" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="7.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="4" t="s">
+      <c r="B125" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="7.9" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B123" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="C123" s="1" t="s">
+      <c r="B127" s="4">
+        <v>20</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="5.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B129" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B131" s="4">
+        <v>14.3</v>
+      </c>
+      <c r="C131" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="7.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B125" s="4">
-        <v>20</v>
-      </c>
-      <c r="C125" s="1" t="s">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B134" s="4">
+        <v>2</v>
+      </c>
+      <c r="C134" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="5.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B127" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B129" s="4">
-        <v>14.3</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="4" t="s">
+    <row r="135" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B132" s="4">
-        <v>2</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A134" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B134" s="4">
+      <c r="B136" s="4">
         <v>1.3</v>
       </c>
-      <c r="C134" s="1" t="s">
+      <c r="C136" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A137" s="8"/>
-      <c r="B137" s="8" t="s">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" s="8"/>
+      <c r="B139" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C139" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C137" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="9" t="s">
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" s="9" t="s">
         <v>6</v>
-      </c>
-      <c r="B138" s="8">
-        <v>1</v>
-      </c>
-      <c r="C138" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A139" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B139" s="8">
-        <v>1</v>
-      </c>
-      <c r="C139" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A140" s="9" t="s">
-        <v>7</v>
       </c>
       <c r="B140" s="8">
         <v>1</v>
@@ -9860,9 +10180,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B141" s="8">
         <v>1</v>
@@ -9871,14 +10191,36 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142" s="9" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="B142" s="8">
         <v>1</v>
       </c>
       <c r="C142" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B143" s="8">
+        <v>1</v>
+      </c>
+      <c r="C143" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B144" s="8">
+        <v>1</v>
+      </c>
+      <c r="C144" s="8">
         <v>3</v>
       </c>
     </row>

</xml_diff>